<commit_message>
quiz db populate from excel
</commit_message>
<xml_diff>
--- a/data/quiz-data.xlsx
+++ b/data/quiz-data.xlsx
@@ -5,19 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ninju\Internship\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VIT\Placement\Internship\SFS intern\Project-Backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE27BDB3-1F47-4520-811E-B9D92E5CD1A2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F549E466-061C-41C8-AB89-2F178B2FAE06}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Training" sheetId="3" r:id="rId1"/>
-    <sheet name="quiz" sheetId="2" r:id="rId2"/>
+    <sheet name="Quiz" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="137">
   <si>
     <t>Constipation</t>
   </si>
@@ -376,22 +376,77 @@
   </si>
   <si>
     <t>I am fine</t>
+  </si>
+  <si>
+    <t>Section number</t>
+  </si>
+  <si>
+    <t>Section name</t>
+  </si>
+  <si>
+    <t>About Your Gut</t>
+  </si>
+  <si>
+    <t>About Your Lifestyle</t>
+  </si>
+  <si>
+    <t>One Last Thing</t>
+  </si>
+  <si>
+    <t>About You</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Others</t>
+  </si>
+  <si>
+    <t>Daily Activity Level</t>
+  </si>
+  <si>
+    <t>Sedentary/Couch Potato</t>
+  </si>
+  <si>
+    <t>Light Exercise/Somewhat Active</t>
+  </si>
+  <si>
+    <t>Moderate Exercise/Average Activity</t>
+  </si>
+  <si>
+    <t>Active Individuals/Very Active</t>
+  </si>
+  <si>
+    <t>Extremely Active Individuals/Extremely Active</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Dersired weight</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -407,6 +462,19 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -450,7 +518,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -458,16 +526,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -754,23 +824,23 @@
       <selection activeCell="C2" sqref="C2:C78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.26953125" customWidth="1"/>
-    <col min="2" max="2" width="35.36328125" customWidth="1"/>
-    <col min="3" max="3" width="15.7265625" customWidth="1"/>
-    <col min="4" max="4" width="16.1796875" customWidth="1"/>
-    <col min="5" max="5" width="16.81640625" customWidth="1"/>
-    <col min="6" max="6" width="15.81640625" customWidth="1"/>
+    <col min="1" max="1" width="20.21875" customWidth="1"/>
+    <col min="2" max="2" width="35.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.77734375" customWidth="1"/>
+    <col min="4" max="4" width="16.21875" customWidth="1"/>
+    <col min="5" max="5" width="16.77734375" customWidth="1"/>
+    <col min="6" max="6" width="15.77734375" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="13.7265625" customWidth="1"/>
-    <col min="9" max="9" width="18.81640625" customWidth="1"/>
+    <col min="8" max="8" width="13.77734375" customWidth="1"/>
+    <col min="9" max="9" width="18.77734375" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
-    <col min="11" max="11" width="13.453125" customWidth="1"/>
-    <col min="12" max="12" width="12.6328125" customWidth="1"/>
+    <col min="11" max="11" width="13.44140625" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="54" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="50.4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>95</v>
       </c>
@@ -808,7 +878,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -846,7 +916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -884,7 +954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -922,7 +992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -960,7 +1030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -998,7 +1068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1036,7 +1106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1074,7 +1144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1112,7 +1182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1150,7 +1220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1188,7 +1258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1226,7 +1296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1264,7 +1334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1302,7 +1372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1340,7 +1410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2</v>
       </c>
@@ -1378,7 +1448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1416,7 +1486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2</v>
       </c>
@@ -1454,7 +1524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1492,7 +1562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2</v>
       </c>
@@ -1530,7 +1600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2</v>
       </c>
@@ -1568,7 +1638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2</v>
       </c>
@@ -1606,7 +1676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2</v>
       </c>
@@ -1644,7 +1714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2</v>
       </c>
@@ -1682,7 +1752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1720,7 +1790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2</v>
       </c>
@@ -1758,7 +1828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2</v>
       </c>
@@ -1796,7 +1866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2</v>
       </c>
@@ -1834,7 +1904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>2</v>
       </c>
@@ -1872,7 +1942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2</v>
       </c>
@@ -1910,7 +1980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>3</v>
       </c>
@@ -1948,7 +2018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>3</v>
       </c>
@@ -1986,7 +2056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>3</v>
       </c>
@@ -2024,7 +2094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>4</v>
       </c>
@@ -2062,7 +2132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>4</v>
       </c>
@@ -2100,7 +2170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>4</v>
       </c>
@@ -2138,7 +2208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>4</v>
       </c>
@@ -2176,7 +2246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>5</v>
       </c>
@@ -2214,7 +2284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>5</v>
       </c>
@@ -2252,7 +2322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>5</v>
       </c>
@@ -2290,7 +2360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>5</v>
       </c>
@@ -2328,7 +2398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>6</v>
       </c>
@@ -2366,7 +2436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>6</v>
       </c>
@@ -2404,7 +2474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>6</v>
       </c>
@@ -2442,7 +2512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>6</v>
       </c>
@@ -2480,7 +2550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>6</v>
       </c>
@@ -2518,7 +2588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>6</v>
       </c>
@@ -2556,7 +2626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>6</v>
       </c>
@@ -2594,7 +2664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>6</v>
       </c>
@@ -2632,7 +2702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>6</v>
       </c>
@@ -2670,7 +2740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>6</v>
       </c>
@@ -2708,7 +2778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>6</v>
       </c>
@@ -2746,7 +2816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>6</v>
       </c>
@@ -2784,7 +2854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>6</v>
       </c>
@@ -2822,7 +2892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>6</v>
       </c>
@@ -2860,7 +2930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>7</v>
       </c>
@@ -2898,7 +2968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>7</v>
       </c>
@@ -2936,7 +3006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>7</v>
       </c>
@@ -2974,7 +3044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>7</v>
       </c>
@@ -3012,7 +3082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>7</v>
       </c>
@@ -3050,7 +3120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>7</v>
       </c>
@@ -3088,7 +3158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>8</v>
       </c>
@@ -3126,7 +3196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>8</v>
       </c>
@@ -3164,7 +3234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>8</v>
       </c>
@@ -3202,7 +3272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>8</v>
       </c>
@@ -3240,7 +3310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>8</v>
       </c>
@@ -3278,7 +3348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>9</v>
       </c>
@@ -3316,7 +3386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>9</v>
       </c>
@@ -3354,7 +3424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>10</v>
       </c>
@@ -3392,7 +3462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>10</v>
       </c>
@@ -3430,7 +3500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>10</v>
       </c>
@@ -3468,7 +3538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>10</v>
       </c>
@@ -3506,7 +3576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>10</v>
       </c>
@@ -3544,7 +3614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>10</v>
       </c>
@@ -3582,7 +3652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>10</v>
       </c>
@@ -3620,7 +3690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>10</v>
       </c>
@@ -3658,7 +3728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>10</v>
       </c>
@@ -3696,7 +3766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>10</v>
       </c>
@@ -3741,750 +3811,1454 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{209B6C40-D49A-460E-9F0A-D52ECA57AEC1}">
-  <dimension ref="A1:D82"/>
+  <dimension ref="A1:F94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.7265625" customWidth="1"/>
-    <col min="2" max="2" width="73.81640625" customWidth="1"/>
-    <col min="3" max="3" width="26.7265625" customWidth="1"/>
-    <col min="4" max="4" width="37.26953125" customWidth="1"/>
-    <col min="5" max="5" width="23.90625" customWidth="1"/>
-    <col min="6" max="6" width="21.54296875" customWidth="1"/>
-    <col min="7" max="7" width="22.36328125" customWidth="1"/>
-    <col min="8" max="8" width="25.81640625" customWidth="1"/>
-    <col min="9" max="9" width="22.54296875" customWidth="1"/>
-    <col min="10" max="10" width="19.90625" customWidth="1"/>
-    <col min="11" max="11" width="20" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="24.77734375" customWidth="1"/>
+    <col min="4" max="4" width="73.77734375" customWidth="1"/>
+    <col min="5" max="5" width="26.77734375" customWidth="1"/>
+    <col min="6" max="6" width="41.5546875" customWidth="1"/>
+    <col min="7" max="7" width="23.88671875" customWidth="1"/>
+    <col min="8" max="8" width="21.5546875" customWidth="1"/>
+    <col min="9" max="9" width="22.33203125" customWidth="1"/>
+    <col min="10" max="10" width="25.77734375" customWidth="1"/>
+    <col min="11" max="11" width="22.5546875" customWidth="1"/>
+    <col min="12" max="12" width="19.88671875" customWidth="1"/>
+    <col min="13" max="13" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" s="6">
+        <v>1</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="6">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" s="6">
+        <v>1</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C4" s="6">
+        <v>1</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
+        <v>1</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C5" s="6">
+        <v>2</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="6">
+        <v>1</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C6" s="6">
+        <v>2</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="6">
+        <v>1</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C7" s="6">
+        <v>2</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="6">
+        <v>1</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C8" s="6">
+        <v>2</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="6">
+        <v>1</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C9" s="6">
+        <v>2</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="6">
+        <v>1</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C10" s="6">
+        <v>3</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="6">
+        <v>1</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C11" s="6">
+        <v>4</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="6">
+        <v>1</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C12" s="6">
+        <v>5</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="6">
+        <v>1</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C13" s="6">
+        <v>6</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>118</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
         <v>97</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E14" t="s">
         <v>110</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>118</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>118</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="38.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1" t="s">
+    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>118</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>118</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>118</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>118</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>118</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22" t="s">
+        <v>118</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="F22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>118</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="F23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="B24" t="s">
+        <v>118</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="F24" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14">
-        <v>1</v>
-      </c>
-      <c r="D14" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="B25" t="s">
+        <v>118</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="F25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>2</v>
+      </c>
+      <c r="B26" t="s">
+        <v>118</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="F26" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15">
-        <v>1</v>
-      </c>
-      <c r="D15" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>2</v>
+      </c>
+      <c r="B27" t="s">
+        <v>118</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="F27" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16">
-        <v>2</v>
-      </c>
-      <c r="B16" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>2</v>
+      </c>
+      <c r="B28" t="s">
+        <v>118</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28" t="s">
         <v>98</v>
       </c>
-      <c r="C16" t="s">
+      <c r="E28" t="s">
         <v>110</v>
       </c>
-      <c r="D16" t="s">
+      <c r="F28" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17">
-        <v>2</v>
-      </c>
-      <c r="D17" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>2</v>
+      </c>
+      <c r="B29" t="s">
+        <v>118</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="F29" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18">
-        <v>2</v>
-      </c>
-      <c r="D18" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>2</v>
+      </c>
+      <c r="B30" t="s">
+        <v>118</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="F30" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19">
-        <v>2</v>
-      </c>
-      <c r="D19" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>2</v>
+      </c>
+      <c r="B31" t="s">
+        <v>118</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="F31" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20">
-        <v>2</v>
-      </c>
-      <c r="D20" t="s">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>2</v>
+      </c>
+      <c r="B32" t="s">
+        <v>118</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="F32" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21">
-        <v>2</v>
-      </c>
-      <c r="D21" t="s">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>2</v>
+      </c>
+      <c r="B33" t="s">
+        <v>118</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="F33" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22">
-        <v>2</v>
-      </c>
-      <c r="D22" t="s">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>2</v>
+      </c>
+      <c r="B34" t="s">
+        <v>118</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="F34" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23">
-        <v>2</v>
-      </c>
-      <c r="D23" t="s">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>2</v>
+      </c>
+      <c r="B35" t="s">
+        <v>118</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+      <c r="F35" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24">
-        <v>2</v>
-      </c>
-      <c r="D24" t="s">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>2</v>
+      </c>
+      <c r="B36" t="s">
+        <v>118</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+      <c r="F36" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25">
-        <v>2</v>
-      </c>
-      <c r="D25" t="s">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>2</v>
+      </c>
+      <c r="B37" t="s">
+        <v>118</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+      <c r="F37" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26">
-        <v>2</v>
-      </c>
-      <c r="D26" t="s">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>2</v>
+      </c>
+      <c r="B38" t="s">
+        <v>118</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
+      </c>
+      <c r="F38" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27">
-        <v>2</v>
-      </c>
-      <c r="D27" t="s">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>2</v>
+      </c>
+      <c r="B39" t="s">
+        <v>118</v>
+      </c>
+      <c r="C39">
+        <v>2</v>
+      </c>
+      <c r="F39" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28">
-        <v>2</v>
-      </c>
-      <c r="D28" t="s">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>2</v>
+      </c>
+      <c r="B40" t="s">
+        <v>118</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
+      </c>
+      <c r="F40" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29">
-        <v>2</v>
-      </c>
-      <c r="D29" t="s">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>2</v>
+      </c>
+      <c r="B41" t="s">
+        <v>118</v>
+      </c>
+      <c r="C41">
+        <v>2</v>
+      </c>
+      <c r="F41" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30">
-        <v>2</v>
-      </c>
-      <c r="D30" t="s">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>2</v>
+      </c>
+      <c r="B42" t="s">
+        <v>118</v>
+      </c>
+      <c r="C42">
+        <v>2</v>
+      </c>
+      <c r="F42" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>2</v>
+      </c>
+      <c r="B43" t="s">
+        <v>118</v>
+      </c>
+      <c r="C43">
         <v>3</v>
       </c>
-      <c r="B31" t="s">
+      <c r="D43" t="s">
         <v>99</v>
       </c>
-      <c r="C31" t="s">
+      <c r="E43" t="s">
         <v>110</v>
       </c>
-      <c r="D31" t="s">
+      <c r="F43" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>2</v>
+      </c>
+      <c r="B44" t="s">
+        <v>118</v>
+      </c>
+      <c r="C44">
         <v>3</v>
       </c>
-      <c r="D32" t="s">
+      <c r="F44" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>2</v>
+      </c>
+      <c r="B45" t="s">
+        <v>118</v>
+      </c>
+      <c r="C45">
         <v>3</v>
       </c>
-      <c r="D33" t="s">
+      <c r="F45" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>2</v>
+      </c>
+      <c r="B46" t="s">
+        <v>118</v>
+      </c>
+      <c r="C46">
         <v>4</v>
       </c>
-      <c r="B34" t="s">
+      <c r="D46" t="s">
         <v>100</v>
       </c>
-      <c r="C34" t="s">
+      <c r="E46" t="s">
         <v>110</v>
       </c>
-      <c r="D34" t="s">
+      <c r="F46" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>2</v>
+      </c>
+      <c r="B47" t="s">
+        <v>118</v>
+      </c>
+      <c r="C47">
         <v>4</v>
       </c>
-      <c r="D35" t="s">
+      <c r="F47" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>2</v>
+      </c>
+      <c r="B48" t="s">
+        <v>118</v>
+      </c>
+      <c r="C48">
         <v>4</v>
       </c>
-      <c r="D36" t="s">
+      <c r="F48" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>2</v>
+      </c>
+      <c r="B49" t="s">
+        <v>118</v>
+      </c>
+      <c r="C49">
         <v>4</v>
       </c>
-      <c r="D37" t="s">
+      <c r="F49" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>2</v>
+      </c>
+      <c r="B50" t="s">
+        <v>118</v>
+      </c>
+      <c r="C50">
         <v>5</v>
       </c>
-      <c r="B38" t="s">
+      <c r="D50" t="s">
         <v>101</v>
       </c>
-      <c r="C38" t="s">
+      <c r="E50" t="s">
         <v>110</v>
       </c>
-      <c r="D38" t="s">
+      <c r="F50" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>2</v>
+      </c>
+      <c r="B51" t="s">
+        <v>118</v>
+      </c>
+      <c r="C51">
         <v>5</v>
       </c>
-      <c r="D39" t="s">
+      <c r="F51" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>2</v>
+      </c>
+      <c r="B52" t="s">
+        <v>118</v>
+      </c>
+      <c r="C52">
         <v>5</v>
       </c>
-      <c r="D40" t="s">
+      <c r="F52" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>2</v>
+      </c>
+      <c r="B53" t="s">
+        <v>118</v>
+      </c>
+      <c r="C53">
         <v>5</v>
       </c>
-      <c r="D41" t="s">
+      <c r="F53" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A42">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>2</v>
+      </c>
+      <c r="B54" t="s">
+        <v>118</v>
+      </c>
+      <c r="C54">
         <v>6</v>
       </c>
-      <c r="B42" t="s">
+      <c r="D54" t="s">
         <v>102</v>
       </c>
-      <c r="C42" t="s">
+      <c r="E54" t="s">
         <v>110</v>
       </c>
-      <c r="D42" t="s">
+      <c r="F54" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A43">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>2</v>
+      </c>
+      <c r="B55" t="s">
+        <v>118</v>
+      </c>
+      <c r="C55">
         <v>6</v>
       </c>
-      <c r="D43" t="s">
+      <c r="F55" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A44">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>2</v>
+      </c>
+      <c r="B56" t="s">
+        <v>118</v>
+      </c>
+      <c r="C56">
         <v>6</v>
       </c>
-      <c r="D44" t="s">
+      <c r="F56" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A45">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>2</v>
+      </c>
+      <c r="B57" t="s">
+        <v>118</v>
+      </c>
+      <c r="C57">
         <v>6</v>
       </c>
-      <c r="D45" t="s">
+      <c r="F57" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A46">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>2</v>
+      </c>
+      <c r="B58" t="s">
+        <v>118</v>
+      </c>
+      <c r="C58">
         <v>6</v>
       </c>
-      <c r="D46" t="s">
+      <c r="F58" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A47">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>2</v>
+      </c>
+      <c r="B59" t="s">
+        <v>118</v>
+      </c>
+      <c r="C59">
         <v>6</v>
       </c>
-      <c r="D47" t="s">
+      <c r="F59" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A48">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>2</v>
+      </c>
+      <c r="B60" t="s">
+        <v>118</v>
+      </c>
+      <c r="C60">
         <v>6</v>
       </c>
-      <c r="D48" t="s">
+      <c r="F60" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A49">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>2</v>
+      </c>
+      <c r="B61" t="s">
+        <v>118</v>
+      </c>
+      <c r="C61">
         <v>6</v>
       </c>
-      <c r="D49" t="s">
+      <c r="F61" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A50">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>2</v>
+      </c>
+      <c r="B62" t="s">
+        <v>118</v>
+      </c>
+      <c r="C62">
         <v>6</v>
       </c>
-      <c r="D50" t="s">
+      <c r="F62" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A51">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>2</v>
+      </c>
+      <c r="B63" t="s">
+        <v>118</v>
+      </c>
+      <c r="C63">
         <v>6</v>
       </c>
-      <c r="D51" t="s">
+      <c r="F63" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A52">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>2</v>
+      </c>
+      <c r="B64" t="s">
+        <v>118</v>
+      </c>
+      <c r="C64">
         <v>6</v>
       </c>
-      <c r="D52" t="s">
+      <c r="F64" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A53">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>2</v>
+      </c>
+      <c r="B65" t="s">
+        <v>118</v>
+      </c>
+      <c r="C65">
         <v>6</v>
       </c>
-      <c r="D53" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A54">
+      <c r="F65" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>2</v>
+      </c>
+      <c r="B66" t="s">
+        <v>118</v>
+      </c>
+      <c r="C66">
         <v>6</v>
       </c>
-      <c r="D54" t="s">
+      <c r="F66" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A55">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>2</v>
+      </c>
+      <c r="B67" t="s">
+        <v>118</v>
+      </c>
+      <c r="C67">
         <v>6</v>
       </c>
-      <c r="D55" t="s">
+      <c r="F67" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A56">
-        <v>7</v>
-      </c>
-      <c r="B56" t="s">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>3</v>
+      </c>
+      <c r="B68" t="s">
+        <v>119</v>
+      </c>
+      <c r="C68">
+        <v>1</v>
+      </c>
+      <c r="D68" t="s">
         <v>103</v>
       </c>
-      <c r="C56" t="s">
+      <c r="E68" t="s">
         <v>110</v>
       </c>
-      <c r="D56" t="s">
+      <c r="F68" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A57">
-        <v>7</v>
-      </c>
-      <c r="D57" t="s">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>3</v>
+      </c>
+      <c r="B69" t="s">
+        <v>119</v>
+      </c>
+      <c r="C69">
+        <v>1</v>
+      </c>
+      <c r="F69" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A58">
-        <v>7</v>
-      </c>
-      <c r="D58" t="s">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>3</v>
+      </c>
+      <c r="B70" t="s">
+        <v>119</v>
+      </c>
+      <c r="C70">
+        <v>1</v>
+      </c>
+      <c r="F70" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A59">
-        <v>7</v>
-      </c>
-      <c r="D59" t="s">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>3</v>
+      </c>
+      <c r="B71" t="s">
+        <v>119</v>
+      </c>
+      <c r="C71">
+        <v>1</v>
+      </c>
+      <c r="F71" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A60">
-        <v>7</v>
-      </c>
-      <c r="D60" t="s">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>3</v>
+      </c>
+      <c r="B72" t="s">
+        <v>119</v>
+      </c>
+      <c r="C72">
+        <v>1</v>
+      </c>
+      <c r="F72" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A61">
-        <v>7</v>
-      </c>
-      <c r="D61" t="s">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>3</v>
+      </c>
+      <c r="B73" t="s">
+        <v>119</v>
+      </c>
+      <c r="C73">
+        <v>1</v>
+      </c>
+      <c r="F73" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A62">
-        <v>8</v>
-      </c>
-      <c r="B62" t="s">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>3</v>
+      </c>
+      <c r="B74" t="s">
+        <v>119</v>
+      </c>
+      <c r="C74">
+        <v>2</v>
+      </c>
+      <c r="D74" t="s">
         <v>104</v>
       </c>
-      <c r="C62" t="s">
+      <c r="E74" t="s">
         <v>111</v>
       </c>
-      <c r="D62" t="s">
+      <c r="F74" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A63">
-        <v>8</v>
-      </c>
-      <c r="D63" t="s">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>3</v>
+      </c>
+      <c r="B75" t="s">
+        <v>119</v>
+      </c>
+      <c r="C75">
+        <v>2</v>
+      </c>
+      <c r="F75" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A64">
-        <v>8</v>
-      </c>
-      <c r="D64" t="s">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>3</v>
+      </c>
+      <c r="B76" t="s">
+        <v>119</v>
+      </c>
+      <c r="C76">
+        <v>2</v>
+      </c>
+      <c r="F76" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A65">
-        <v>8</v>
-      </c>
-      <c r="D65" t="s">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>3</v>
+      </c>
+      <c r="B77" t="s">
+        <v>119</v>
+      </c>
+      <c r="C77">
+        <v>2</v>
+      </c>
+      <c r="F77" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A66">
-        <v>8</v>
-      </c>
-      <c r="D66" t="s">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>3</v>
+      </c>
+      <c r="B78" t="s">
+        <v>119</v>
+      </c>
+      <c r="C78">
+        <v>2</v>
+      </c>
+      <c r="F78" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A67">
-        <v>9</v>
-      </c>
-      <c r="B67" t="s">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>3</v>
+      </c>
+      <c r="B79" t="s">
+        <v>119</v>
+      </c>
+      <c r="C79">
+        <v>3</v>
+      </c>
+      <c r="D79" t="s">
         <v>105</v>
       </c>
-      <c r="C67" t="s">
+      <c r="E79" t="s">
         <v>111</v>
       </c>
-      <c r="D67" t="s">
+      <c r="F79" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A68">
-        <v>9</v>
-      </c>
-      <c r="D68" t="s">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>3</v>
+      </c>
+      <c r="B80" t="s">
+        <v>119</v>
+      </c>
+      <c r="C80">
+        <v>3</v>
+      </c>
+      <c r="F80" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A69">
-        <v>10</v>
-      </c>
-      <c r="B69" t="s">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>3</v>
+      </c>
+      <c r="B81" t="s">
+        <v>119</v>
+      </c>
+      <c r="C81">
+        <v>4</v>
+      </c>
+      <c r="D81" t="s">
         <v>106</v>
       </c>
-      <c r="C69" t="s">
+      <c r="E81" t="s">
         <v>110</v>
       </c>
-      <c r="D69" t="s">
+      <c r="F81" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A70">
-        <v>10</v>
-      </c>
-      <c r="D70" t="s">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>3</v>
+      </c>
+      <c r="B82" t="s">
+        <v>119</v>
+      </c>
+      <c r="C82">
+        <v>4</v>
+      </c>
+      <c r="F82" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A71">
-        <v>10</v>
-      </c>
-      <c r="D71" t="s">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>3</v>
+      </c>
+      <c r="B83" t="s">
+        <v>119</v>
+      </c>
+      <c r="C83">
+        <v>4</v>
+      </c>
+      <c r="F83" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A72">
-        <v>10</v>
-      </c>
-      <c r="D72" t="s">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>3</v>
+      </c>
+      <c r="B84" t="s">
+        <v>119</v>
+      </c>
+      <c r="C84">
+        <v>4</v>
+      </c>
+      <c r="F84" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A73">
-        <v>10</v>
-      </c>
-      <c r="D73" t="s">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>3</v>
+      </c>
+      <c r="B85" t="s">
+        <v>119</v>
+      </c>
+      <c r="C85">
+        <v>4</v>
+      </c>
+      <c r="F85" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A74">
-        <v>10</v>
-      </c>
-      <c r="D74" t="s">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>3</v>
+      </c>
+      <c r="B86" t="s">
+        <v>119</v>
+      </c>
+      <c r="C86">
+        <v>4</v>
+      </c>
+      <c r="F86" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A75">
-        <v>10</v>
-      </c>
-      <c r="D75" t="s">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>3</v>
+      </c>
+      <c r="B87" t="s">
+        <v>119</v>
+      </c>
+      <c r="C87">
+        <v>4</v>
+      </c>
+      <c r="F87" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A76">
-        <v>10</v>
-      </c>
-      <c r="D76" t="s">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>3</v>
+      </c>
+      <c r="B88" t="s">
+        <v>119</v>
+      </c>
+      <c r="C88">
+        <v>4</v>
+      </c>
+      <c r="F88" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A77">
-        <v>10</v>
-      </c>
-      <c r="D77" t="s">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>3</v>
+      </c>
+      <c r="B89" t="s">
+        <v>119</v>
+      </c>
+      <c r="C89">
+        <v>4</v>
+      </c>
+      <c r="F89" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A78">
-        <v>10</v>
-      </c>
-      <c r="D78" t="s">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>3</v>
+      </c>
+      <c r="B90" t="s">
+        <v>119</v>
+      </c>
+      <c r="C90">
+        <v>4</v>
+      </c>
+      <c r="F90" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A79">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>4</v>
+      </c>
+      <c r="B91" t="s">
+        <v>120</v>
+      </c>
+      <c r="C91">
         <v>11</v>
       </c>
-      <c r="B79" t="s">
+      <c r="D91" t="s">
         <v>107</v>
       </c>
-      <c r="C79" t="s">
+      <c r="E91" t="s">
         <v>110</v>
       </c>
-      <c r="D79" t="s">
+      <c r="F91" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A80">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>4</v>
+      </c>
+      <c r="B92" t="s">
+        <v>120</v>
+      </c>
+      <c r="C92">
         <v>11</v>
       </c>
-      <c r="D80" t="s">
+      <c r="F92" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A81">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>4</v>
+      </c>
+      <c r="B93" t="s">
+        <v>120</v>
+      </c>
+      <c r="C93">
         <v>11</v>
       </c>
-      <c r="D81" t="s">
+      <c r="F93" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A82">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>4</v>
+      </c>
+      <c r="B94" t="s">
+        <v>120</v>
+      </c>
+      <c r="C94">
         <v>11</v>
       </c>
-      <c r="D82" t="s">
+      <c r="F94" t="s">
         <v>115</v>
       </c>
     </row>
@@ -4502,80 +5276,80 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.54296875" customWidth="1"/>
-    <col min="2" max="2" width="28.7265625" customWidth="1"/>
-    <col min="3" max="3" width="18.453125" customWidth="1"/>
-    <col min="4" max="4" width="18.90625" customWidth="1"/>
-    <col min="5" max="5" width="18.26953125" customWidth="1"/>
+    <col min="1" max="1" width="21.5546875" customWidth="1"/>
+    <col min="2" max="2" width="28.77734375" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" customWidth="1"/>
+    <col min="5" max="5" width="18.21875" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="29.1796875" customWidth="1"/>
-    <col min="8" max="8" width="15.08984375" customWidth="1"/>
-    <col min="9" max="9" width="13.26953125" customWidth="1"/>
-    <col min="10" max="10" width="29.1796875" customWidth="1"/>
-    <col min="11" max="11" width="21.7265625" customWidth="1"/>
-    <col min="12" max="12" width="18.54296875" customWidth="1"/>
-    <col min="13" max="13" width="15.7265625" customWidth="1"/>
-    <col min="16" max="16" width="11.1796875" customWidth="1"/>
-    <col min="17" max="17" width="18.26953125" customWidth="1"/>
+    <col min="7" max="7" width="29.21875" customWidth="1"/>
+    <col min="8" max="8" width="15.109375" customWidth="1"/>
+    <col min="9" max="9" width="13.21875" customWidth="1"/>
+    <col min="10" max="10" width="29.21875" customWidth="1"/>
+    <col min="11" max="11" width="21.77734375" customWidth="1"/>
+    <col min="12" max="12" width="18.5546875" customWidth="1"/>
+    <col min="13" max="13" width="15.77734375" customWidth="1"/>
+    <col min="16" max="16" width="11.21875" customWidth="1"/>
+    <col min="17" max="17" width="18.21875" customWidth="1"/>
     <col min="18" max="18" width="36" customWidth="1"/>
-    <col min="19" max="19" width="8.90625" customWidth="1"/>
+    <col min="19" max="19" width="8.88671875" customWidth="1"/>
     <col min="20" max="20" width="30" customWidth="1"/>
-    <col min="21" max="21" width="12.81640625" customWidth="1"/>
-    <col min="22" max="22" width="11.6328125" customWidth="1"/>
-    <col min="23" max="23" width="11.36328125" customWidth="1"/>
-    <col min="24" max="24" width="15.453125" customWidth="1"/>
-    <col min="25" max="25" width="31.54296875" customWidth="1"/>
-    <col min="26" max="26" width="20.36328125" customWidth="1"/>
-    <col min="27" max="27" width="10.7265625" customWidth="1"/>
-    <col min="28" max="28" width="18.90625" customWidth="1"/>
-    <col min="29" max="29" width="25.26953125" customWidth="1"/>
-    <col min="30" max="30" width="23.90625" customWidth="1"/>
-    <col min="31" max="31" width="18.81640625" customWidth="1"/>
-    <col min="32" max="32" width="11.54296875" customWidth="1"/>
-    <col min="33" max="33" width="17.6328125" customWidth="1"/>
-    <col min="34" max="34" width="26.453125" customWidth="1"/>
-    <col min="35" max="35" width="15.90625" customWidth="1"/>
-    <col min="36" max="36" width="33.1796875" customWidth="1"/>
-    <col min="37" max="37" width="34.7265625" customWidth="1"/>
-    <col min="38" max="38" width="15.1796875" customWidth="1"/>
+    <col min="21" max="21" width="12.77734375" customWidth="1"/>
+    <col min="22" max="22" width="11.6640625" customWidth="1"/>
+    <col min="23" max="23" width="11.33203125" customWidth="1"/>
+    <col min="24" max="24" width="15.44140625" customWidth="1"/>
+    <col min="25" max="25" width="31.5546875" customWidth="1"/>
+    <col min="26" max="26" width="20.33203125" customWidth="1"/>
+    <col min="27" max="27" width="10.77734375" customWidth="1"/>
+    <col min="28" max="28" width="18.88671875" customWidth="1"/>
+    <col min="29" max="29" width="25.21875" customWidth="1"/>
+    <col min="30" max="30" width="23.88671875" customWidth="1"/>
+    <col min="31" max="31" width="18.77734375" customWidth="1"/>
+    <col min="32" max="32" width="11.5546875" customWidth="1"/>
+    <col min="33" max="33" width="17.6640625" customWidth="1"/>
+    <col min="34" max="34" width="26.44140625" customWidth="1"/>
+    <col min="35" max="35" width="15.88671875" customWidth="1"/>
+    <col min="36" max="36" width="33.21875" customWidth="1"/>
+    <col min="37" max="37" width="34.77734375" customWidth="1"/>
+    <col min="38" max="38" width="15.21875" customWidth="1"/>
     <col min="39" max="39" width="33" customWidth="1"/>
     <col min="40" max="40" width="32" customWidth="1"/>
-    <col min="41" max="41" width="25.54296875" customWidth="1"/>
-    <col min="42" max="42" width="11.26953125" customWidth="1"/>
-    <col min="43" max="43" width="14.453125" customWidth="1"/>
-    <col min="44" max="44" width="31.36328125" customWidth="1"/>
-    <col min="45" max="45" width="23.1796875" customWidth="1"/>
-    <col min="46" max="46" width="34.453125" customWidth="1"/>
-    <col min="47" max="47" width="12.453125" customWidth="1"/>
-    <col min="48" max="48" width="10.7265625" customWidth="1"/>
-    <col min="49" max="49" width="17.6328125" customWidth="1"/>
-    <col min="52" max="52" width="13.08984375" customWidth="1"/>
-    <col min="53" max="53" width="14.26953125" customWidth="1"/>
-    <col min="54" max="54" width="17.81640625" customWidth="1"/>
-    <col min="55" max="55" width="10.54296875" customWidth="1"/>
-    <col min="56" max="56" width="18.1796875" customWidth="1"/>
-    <col min="57" max="57" width="10.90625" customWidth="1"/>
-    <col min="58" max="58" width="14.1796875" customWidth="1"/>
-    <col min="59" max="59" width="9.08984375" customWidth="1"/>
-    <col min="61" max="61" width="11.1796875" customWidth="1"/>
-    <col min="63" max="63" width="16.453125" customWidth="1"/>
-    <col min="64" max="64" width="17.7265625" customWidth="1"/>
-    <col min="65" max="65" width="18.36328125" customWidth="1"/>
-    <col min="66" max="66" width="22.26953125" customWidth="1"/>
-    <col min="67" max="67" width="13.54296875" customWidth="1"/>
-    <col min="69" max="69" width="13.453125" customWidth="1"/>
-    <col min="70" max="70" width="24.26953125" customWidth="1"/>
-    <col min="72" max="72" width="14.26953125" customWidth="1"/>
-    <col min="74" max="74" width="12.81640625" customWidth="1"/>
-    <col min="75" max="75" width="22.36328125" customWidth="1"/>
-    <col min="77" max="77" width="27.26953125" customWidth="1"/>
-    <col min="78" max="78" width="26.54296875" customWidth="1"/>
-    <col min="80" max="80" width="11.90625" customWidth="1"/>
+    <col min="41" max="41" width="25.5546875" customWidth="1"/>
+    <col min="42" max="42" width="11.21875" customWidth="1"/>
+    <col min="43" max="43" width="14.44140625" customWidth="1"/>
+    <col min="44" max="44" width="31.33203125" customWidth="1"/>
+    <col min="45" max="45" width="23.21875" customWidth="1"/>
+    <col min="46" max="46" width="34.44140625" customWidth="1"/>
+    <col min="47" max="47" width="12.44140625" customWidth="1"/>
+    <col min="48" max="48" width="10.77734375" customWidth="1"/>
+    <col min="49" max="49" width="17.6640625" customWidth="1"/>
+    <col min="52" max="52" width="13.109375" customWidth="1"/>
+    <col min="53" max="53" width="14.21875" customWidth="1"/>
+    <col min="54" max="54" width="17.77734375" customWidth="1"/>
+    <col min="55" max="55" width="10.5546875" customWidth="1"/>
+    <col min="56" max="56" width="18.21875" customWidth="1"/>
+    <col min="57" max="57" width="10.88671875" customWidth="1"/>
+    <col min="58" max="58" width="14.21875" customWidth="1"/>
+    <col min="59" max="59" width="9.109375" customWidth="1"/>
+    <col min="61" max="61" width="11.21875" customWidth="1"/>
+    <col min="63" max="63" width="16.44140625" customWidth="1"/>
+    <col min="64" max="64" width="17.77734375" customWidth="1"/>
+    <col min="65" max="65" width="18.33203125" customWidth="1"/>
+    <col min="66" max="66" width="22.21875" customWidth="1"/>
+    <col min="67" max="67" width="13.5546875" customWidth="1"/>
+    <col min="69" max="69" width="13.44140625" customWidth="1"/>
+    <col min="70" max="70" width="24.21875" customWidth="1"/>
+    <col min="72" max="72" width="14.21875" customWidth="1"/>
+    <col min="74" max="74" width="12.77734375" customWidth="1"/>
+    <col min="75" max="75" width="22.33203125" customWidth="1"/>
+    <col min="77" max="77" width="27.21875" customWidth="1"/>
+    <col min="78" max="78" width="26.5546875" customWidth="1"/>
+    <col min="80" max="80" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:78" ht="59" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:78" ht="58.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>73</v>
       </c>
@@ -4811,7 +5585,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>79</v>
       </c>
@@ -5047,7 +5821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>78</v>
       </c>
@@ -5283,7 +6057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>77</v>
       </c>
@@ -5519,7 +6293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>82</v>
       </c>
@@ -5755,7 +6529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>76</v>
       </c>
@@ -5991,7 +6765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>75</v>
       </c>
@@ -6227,7 +7001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>74</v>
       </c>
@@ -6463,7 +7237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>80</v>
       </c>
@@ -6699,7 +7473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>81</v>
       </c>
@@ -6935,7 +7709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>83</v>
       </c>

</xml_diff>

<commit_message>
training ml model with excel initial commit
</commit_message>
<xml_diff>
--- a/data/quiz-data.xlsx
+++ b/data/quiz-data.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ninju\Internship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE27BDB3-1F47-4520-811E-B9D92E5CD1A2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7174DA6C-5DD8-48BC-9DCE-CDF2E223549C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Training" sheetId="3" r:id="rId1"/>
-    <sheet name="quiz" sheetId="2" r:id="rId2"/>
+    <sheet name="Quiz" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="116">
   <si>
     <t>Constipation</t>
   </si>
@@ -282,6 +282,9 @@
     <t>NoP</t>
   </si>
   <si>
+    <t>Symptoms</t>
+  </si>
+  <si>
     <t>Poor dietary choices</t>
   </si>
   <si>
@@ -307,9 +310,6 @@
   </si>
   <si>
     <t>Mal-absorption</t>
-  </si>
-  <si>
-    <t>No problem</t>
   </si>
   <si>
     <t>Question</t>
@@ -750,8 +750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B5FB84D-C3CE-41F8-8DF2-CD77A0B9A49A}">
   <dimension ref="A1:L78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C78"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -775,38 +775,36 @@
         <v>95</v>
       </c>
       <c r="B1" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="L1" s="5" t="s">
         <v>93</v>
       </c>
+      <c r="L1" s="5"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2">
@@ -842,9 +840,6 @@
       <c r="K2">
         <v>1</v>
       </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3">
@@ -880,9 +875,6 @@
       <c r="K3">
         <v>1</v>
       </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4">
@@ -918,9 +910,6 @@
       <c r="K4">
         <v>0</v>
       </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
     </row>
     <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5">
@@ -956,9 +945,6 @@
       <c r="K5">
         <v>0</v>
       </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6">
@@ -994,9 +980,6 @@
       <c r="K6">
         <v>0</v>
       </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7">
@@ -1032,9 +1015,6 @@
       <c r="K7">
         <v>0</v>
       </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8">
@@ -1070,9 +1050,6 @@
       <c r="K8">
         <v>0</v>
       </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9">
@@ -1108,9 +1085,6 @@
       <c r="K9">
         <v>0</v>
       </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10">
@@ -1146,9 +1120,6 @@
       <c r="K10">
         <v>0</v>
       </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11">
@@ -1184,9 +1155,6 @@
       <c r="K11">
         <v>0</v>
       </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12">
@@ -1222,9 +1190,6 @@
       <c r="K12">
         <v>1</v>
       </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13">
@@ -1260,9 +1225,6 @@
       <c r="K13">
         <v>1</v>
       </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14">
@@ -1298,9 +1260,6 @@
       <c r="K14">
         <v>1</v>
       </c>
-      <c r="L14">
-        <v>0</v>
-      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15">
@@ -1334,9 +1293,6 @@
         <v>0</v>
       </c>
       <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="L15">
         <v>0</v>
       </c>
     </row>
@@ -1374,11 +1330,8 @@
       <c r="K16">
         <v>0</v>
       </c>
-      <c r="L16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1412,11 +1365,8 @@
       <c r="K17">
         <v>0</v>
       </c>
-      <c r="L17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2</v>
       </c>
@@ -1450,11 +1400,8 @@
       <c r="K18">
         <v>0</v>
       </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1488,11 +1435,8 @@
       <c r="K19">
         <v>0</v>
       </c>
-      <c r="L19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>2</v>
       </c>
@@ -1526,11 +1470,8 @@
       <c r="K20">
         <v>0</v>
       </c>
-      <c r="L20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>2</v>
       </c>
@@ -1564,11 +1505,8 @@
       <c r="K21">
         <v>0</v>
       </c>
-      <c r="L21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>2</v>
       </c>
@@ -1602,11 +1540,8 @@
       <c r="K22">
         <v>0</v>
       </c>
-      <c r="L22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>2</v>
       </c>
@@ -1640,11 +1575,8 @@
       <c r="K23">
         <v>0</v>
       </c>
-      <c r="L23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>2</v>
       </c>
@@ -1678,11 +1610,8 @@
       <c r="K24">
         <v>1</v>
       </c>
-      <c r="L24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1716,11 +1645,8 @@
       <c r="K25">
         <v>1</v>
       </c>
-      <c r="L25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>2</v>
       </c>
@@ -1754,11 +1680,8 @@
       <c r="K26">
         <v>1</v>
       </c>
-      <c r="L26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>2</v>
       </c>
@@ -1792,11 +1715,8 @@
       <c r="K27">
         <v>1</v>
       </c>
-      <c r="L27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>2</v>
       </c>
@@ -1830,11 +1750,8 @@
       <c r="K28">
         <v>0</v>
       </c>
-      <c r="L28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>2</v>
       </c>
@@ -1868,11 +1785,8 @@
       <c r="K29">
         <v>0</v>
       </c>
-      <c r="L29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>2</v>
       </c>
@@ -1906,11 +1820,8 @@
       <c r="K30">
         <v>0</v>
       </c>
-      <c r="L30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>3</v>
       </c>
@@ -1944,11 +1855,8 @@
       <c r="K31">
         <v>0</v>
       </c>
-      <c r="L31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>3</v>
       </c>
@@ -1982,11 +1890,8 @@
       <c r="K32">
         <v>0</v>
       </c>
-      <c r="L32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>3</v>
       </c>
@@ -2020,11 +1925,8 @@
       <c r="K33">
         <v>0</v>
       </c>
-      <c r="L33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>4</v>
       </c>
@@ -2058,11 +1960,8 @@
       <c r="K34">
         <v>0</v>
       </c>
-      <c r="L34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>4</v>
       </c>
@@ -2096,11 +1995,8 @@
       <c r="K35">
         <v>0</v>
       </c>
-      <c r="L35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>4</v>
       </c>
@@ -2134,11 +2030,8 @@
       <c r="K36">
         <v>0</v>
       </c>
-      <c r="L36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>4</v>
       </c>
@@ -2172,11 +2065,8 @@
       <c r="K37">
         <v>0</v>
       </c>
-      <c r="L37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>5</v>
       </c>
@@ -2210,11 +2100,8 @@
       <c r="K38">
         <v>0</v>
       </c>
-      <c r="L38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>5</v>
       </c>
@@ -2248,11 +2135,8 @@
       <c r="K39">
         <v>0</v>
       </c>
-      <c r="L39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>5</v>
       </c>
@@ -2286,11 +2170,8 @@
       <c r="K40">
         <v>0</v>
       </c>
-      <c r="L40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>5</v>
       </c>
@@ -2324,11 +2205,8 @@
       <c r="K41">
         <v>0</v>
       </c>
-      <c r="L41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>6</v>
       </c>
@@ -2362,11 +2240,8 @@
       <c r="K42">
         <v>0</v>
       </c>
-      <c r="L42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>6</v>
       </c>
@@ -2400,11 +2275,8 @@
       <c r="K43">
         <v>0</v>
       </c>
-      <c r="L43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>6</v>
       </c>
@@ -2438,11 +2310,8 @@
       <c r="K44">
         <v>1</v>
       </c>
-      <c r="L44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>6</v>
       </c>
@@ -2476,11 +2345,8 @@
       <c r="K45">
         <v>1</v>
       </c>
-      <c r="L45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>6</v>
       </c>
@@ -2514,11 +2380,8 @@
       <c r="K46">
         <v>1</v>
       </c>
-      <c r="L46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>6</v>
       </c>
@@ -2552,11 +2415,8 @@
       <c r="K47">
         <v>1</v>
       </c>
-      <c r="L47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>6</v>
       </c>
@@ -2590,11 +2450,8 @@
       <c r="K48">
         <v>1</v>
       </c>
-      <c r="L48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>6</v>
       </c>
@@ -2628,11 +2485,8 @@
       <c r="K49">
         <v>1</v>
       </c>
-      <c r="L49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>6</v>
       </c>
@@ -2666,11 +2520,8 @@
       <c r="K50">
         <v>1</v>
       </c>
-      <c r="L50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>6</v>
       </c>
@@ -2704,11 +2555,8 @@
       <c r="K51">
         <v>1</v>
       </c>
-      <c r="L51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>6</v>
       </c>
@@ -2742,11 +2590,8 @@
       <c r="K52">
         <v>1</v>
       </c>
-      <c r="L52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>6</v>
       </c>
@@ -2780,11 +2625,8 @@
       <c r="K53">
         <v>1</v>
       </c>
-      <c r="L53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>6</v>
       </c>
@@ -2818,11 +2660,8 @@
       <c r="K54">
         <v>0</v>
       </c>
-      <c r="L54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>6</v>
       </c>
@@ -2856,11 +2695,8 @@
       <c r="K55">
         <v>0</v>
       </c>
-      <c r="L55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>7</v>
       </c>
@@ -2894,11 +2730,8 @@
       <c r="K56">
         <v>0</v>
       </c>
-      <c r="L56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>7</v>
       </c>
@@ -2932,11 +2765,8 @@
       <c r="K57">
         <v>0</v>
       </c>
-      <c r="L57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>7</v>
       </c>
@@ -2970,11 +2800,8 @@
       <c r="K58">
         <v>0</v>
       </c>
-      <c r="L58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>7</v>
       </c>
@@ -3008,11 +2835,8 @@
       <c r="K59">
         <v>0</v>
       </c>
-      <c r="L59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>7</v>
       </c>
@@ -3046,11 +2870,8 @@
       <c r="K60">
         <v>0</v>
       </c>
-      <c r="L60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>7</v>
       </c>
@@ -3084,11 +2905,8 @@
       <c r="K61">
         <v>0</v>
       </c>
-      <c r="L61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>8</v>
       </c>
@@ -3122,11 +2940,8 @@
       <c r="K62">
         <v>0</v>
       </c>
-      <c r="L62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>8</v>
       </c>
@@ -3160,11 +2975,8 @@
       <c r="K63">
         <v>0</v>
       </c>
-      <c r="L63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>8</v>
       </c>
@@ -3198,11 +3010,8 @@
       <c r="K64">
         <v>0</v>
       </c>
-      <c r="L64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>8</v>
       </c>
@@ -3236,11 +3045,8 @@
       <c r="K65">
         <v>0</v>
       </c>
-      <c r="L65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>8</v>
       </c>
@@ -3274,11 +3080,8 @@
       <c r="K66">
         <v>0</v>
       </c>
-      <c r="L66">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>9</v>
       </c>
@@ -3312,11 +3115,8 @@
       <c r="K67">
         <v>0</v>
       </c>
-      <c r="L67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>9</v>
       </c>
@@ -3350,11 +3150,8 @@
       <c r="K68">
         <v>0</v>
       </c>
-      <c r="L68">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>10</v>
       </c>
@@ -3388,11 +3185,8 @@
       <c r="K69">
         <v>0</v>
       </c>
-      <c r="L69">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>10</v>
       </c>
@@ -3426,11 +3220,8 @@
       <c r="K70">
         <v>0</v>
       </c>
-      <c r="L70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>10</v>
       </c>
@@ -3464,11 +3255,8 @@
       <c r="K71">
         <v>0</v>
       </c>
-      <c r="L71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>10</v>
       </c>
@@ -3502,11 +3290,8 @@
       <c r="K72">
         <v>0</v>
       </c>
-      <c r="L72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>10</v>
       </c>
@@ -3540,11 +3325,8 @@
       <c r="K73">
         <v>0</v>
       </c>
-      <c r="L73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>10</v>
       </c>
@@ -3578,11 +3360,8 @@
       <c r="K74">
         <v>1</v>
       </c>
-      <c r="L74">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>10</v>
       </c>
@@ -3616,11 +3395,8 @@
       <c r="K75">
         <v>0</v>
       </c>
-      <c r="L75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>10</v>
       </c>
@@ -3654,11 +3430,8 @@
       <c r="K76">
         <v>0</v>
       </c>
-      <c r="L76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>10</v>
       </c>
@@ -3692,11 +3465,8 @@
       <c r="K77">
         <v>0</v>
       </c>
-      <c r="L77">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>10</v>
       </c>
@@ -3728,9 +3498,6 @@
         <v>0</v>
       </c>
       <c r="K78">
-        <v>0</v>
-      </c>
-      <c r="L78">
         <v>0</v>
       </c>
     </row>
@@ -3743,7 +3510,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{209B6C40-D49A-460E-9F0A-D52ECA57AEC1}">
   <dimension ref="A1:D82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>

<commit_message>
quiz data population and conclusions
</commit_message>
<xml_diff>
--- a/data/quiz-data.xlsx
+++ b/data/quiz-data.xlsx
@@ -5,19 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ninju\Internship\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VIT\Placement\Internship\SFS intern\Project-Backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7174DA6C-5DD8-48BC-9DCE-CDF2E223549C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F549E466-061C-41C8-AB89-2F178B2FAE06}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Training" sheetId="3" r:id="rId1"/>
     <sheet name="Quiz" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="137">
   <si>
     <t>Constipation</t>
   </si>
@@ -282,9 +282,6 @@
     <t>NoP</t>
   </si>
   <si>
-    <t>Symptoms</t>
-  </si>
-  <si>
     <t>Poor dietary choices</t>
   </si>
   <si>
@@ -312,6 +309,9 @@
     <t>Mal-absorption</t>
   </si>
   <si>
+    <t>No problem</t>
+  </si>
+  <si>
     <t>Question</t>
   </si>
   <si>
@@ -376,22 +376,77 @@
   </si>
   <si>
     <t>I am fine</t>
+  </si>
+  <si>
+    <t>Section number</t>
+  </si>
+  <si>
+    <t>Section name</t>
+  </si>
+  <si>
+    <t>About Your Gut</t>
+  </si>
+  <si>
+    <t>About Your Lifestyle</t>
+  </si>
+  <si>
+    <t>One Last Thing</t>
+  </si>
+  <si>
+    <t>About You</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Others</t>
+  </si>
+  <si>
+    <t>Daily Activity Level</t>
+  </si>
+  <si>
+    <t>Sedentary/Couch Potato</t>
+  </si>
+  <si>
+    <t>Light Exercise/Somewhat Active</t>
+  </si>
+  <si>
+    <t>Moderate Exercise/Average Activity</t>
+  </si>
+  <si>
+    <t>Active Individuals/Very Active</t>
+  </si>
+  <si>
+    <t>Extremely Active Individuals/Extremely Active</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Dersired weight</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -407,6 +462,19 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -450,7 +518,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -458,16 +526,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -750,63 +820,65 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B5FB84D-C3CE-41F8-8DF2-CD77A0B9A49A}">
   <dimension ref="A1:L78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.26953125" customWidth="1"/>
-    <col min="2" max="2" width="35.36328125" customWidth="1"/>
-    <col min="3" max="3" width="15.7265625" customWidth="1"/>
-    <col min="4" max="4" width="16.1796875" customWidth="1"/>
-    <col min="5" max="5" width="16.81640625" customWidth="1"/>
-    <col min="6" max="6" width="15.81640625" customWidth="1"/>
+    <col min="1" max="1" width="20.21875" customWidth="1"/>
+    <col min="2" max="2" width="35.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.77734375" customWidth="1"/>
+    <col min="4" max="4" width="16.21875" customWidth="1"/>
+    <col min="5" max="5" width="16.77734375" customWidth="1"/>
+    <col min="6" max="6" width="15.77734375" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="13.7265625" customWidth="1"/>
-    <col min="9" max="9" width="18.81640625" customWidth="1"/>
+    <col min="8" max="8" width="13.77734375" customWidth="1"/>
+    <col min="9" max="9" width="18.77734375" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
-    <col min="11" max="11" width="13.453125" customWidth="1"/>
-    <col min="12" max="12" width="12.6328125" customWidth="1"/>
+    <col min="11" max="11" width="13.44140625" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="54" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="50.4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>95</v>
       </c>
       <c r="B1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="L1" s="5"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -840,8 +912,11 @@
       <c r="K2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -875,8 +950,11 @@
       <c r="K3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -910,8 +988,11 @@
       <c r="K4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -945,8 +1026,11 @@
       <c r="K5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -980,8 +1064,11 @@
       <c r="K6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1015,8 +1102,11 @@
       <c r="K7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1050,8 +1140,11 @@
       <c r="K8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1085,8 +1178,11 @@
       <c r="K9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1120,8 +1216,11 @@
       <c r="K10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1155,8 +1254,11 @@
       <c r="K11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1190,8 +1292,11 @@
       <c r="K12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1225,8 +1330,11 @@
       <c r="K13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1260,8 +1368,11 @@
       <c r="K14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1295,8 +1406,11 @@
       <c r="K15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2</v>
       </c>
@@ -1330,8 +1444,11 @@
       <c r="K16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1365,8 +1482,11 @@
       <c r="K17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2</v>
       </c>
@@ -1400,8 +1520,11 @@
       <c r="K18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1435,8 +1558,11 @@
       <c r="K19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2</v>
       </c>
@@ -1470,8 +1596,11 @@
       <c r="K20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2</v>
       </c>
@@ -1505,8 +1634,11 @@
       <c r="K21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2</v>
       </c>
@@ -1540,8 +1672,11 @@
       <c r="K22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2</v>
       </c>
@@ -1575,8 +1710,11 @@
       <c r="K23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2</v>
       </c>
@@ -1610,8 +1748,11 @@
       <c r="K24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1645,8 +1786,11 @@
       <c r="K25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2</v>
       </c>
@@ -1680,8 +1824,11 @@
       <c r="K26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2</v>
       </c>
@@ -1715,8 +1862,11 @@
       <c r="K27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2</v>
       </c>
@@ -1750,8 +1900,11 @@
       <c r="K28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>2</v>
       </c>
@@ -1785,8 +1938,11 @@
       <c r="K29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2</v>
       </c>
@@ -1820,8 +1976,11 @@
       <c r="K30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>3</v>
       </c>
@@ -1855,8 +2014,11 @@
       <c r="K31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>3</v>
       </c>
@@ -1890,8 +2052,11 @@
       <c r="K32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>3</v>
       </c>
@@ -1925,8 +2090,11 @@
       <c r="K33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>4</v>
       </c>
@@ -1960,8 +2128,11 @@
       <c r="K34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>4</v>
       </c>
@@ -1995,8 +2166,11 @@
       <c r="K35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>4</v>
       </c>
@@ -2030,8 +2204,11 @@
       <c r="K36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>4</v>
       </c>
@@ -2065,8 +2242,11 @@
       <c r="K37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>5</v>
       </c>
@@ -2100,8 +2280,11 @@
       <c r="K38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>5</v>
       </c>
@@ -2135,8 +2318,11 @@
       <c r="K39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>5</v>
       </c>
@@ -2170,8 +2356,11 @@
       <c r="K40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>5</v>
       </c>
@@ -2205,8 +2394,11 @@
       <c r="K41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>6</v>
       </c>
@@ -2240,8 +2432,11 @@
       <c r="K42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>6</v>
       </c>
@@ -2275,8 +2470,11 @@
       <c r="K43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>6</v>
       </c>
@@ -2310,8 +2508,11 @@
       <c r="K44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>6</v>
       </c>
@@ -2345,8 +2546,11 @@
       <c r="K45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>6</v>
       </c>
@@ -2380,8 +2584,11 @@
       <c r="K46">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>6</v>
       </c>
@@ -2415,8 +2622,11 @@
       <c r="K47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>6</v>
       </c>
@@ -2450,8 +2660,11 @@
       <c r="K48">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>6</v>
       </c>
@@ -2485,8 +2698,11 @@
       <c r="K49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>6</v>
       </c>
@@ -2520,8 +2736,11 @@
       <c r="K50">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>6</v>
       </c>
@@ -2555,8 +2774,11 @@
       <c r="K51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>6</v>
       </c>
@@ -2590,8 +2812,11 @@
       <c r="K52">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>6</v>
       </c>
@@ -2625,8 +2850,11 @@
       <c r="K53">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>6</v>
       </c>
@@ -2660,8 +2888,11 @@
       <c r="K54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>6</v>
       </c>
@@ -2695,8 +2926,11 @@
       <c r="K55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>7</v>
       </c>
@@ -2730,8 +2964,11 @@
       <c r="K56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>7</v>
       </c>
@@ -2765,8 +3002,11 @@
       <c r="K57">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>7</v>
       </c>
@@ -2800,8 +3040,11 @@
       <c r="K58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>7</v>
       </c>
@@ -2835,8 +3078,11 @@
       <c r="K59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>7</v>
       </c>
@@ -2870,8 +3116,11 @@
       <c r="K60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>7</v>
       </c>
@@ -2905,8 +3154,11 @@
       <c r="K61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>8</v>
       </c>
@@ -2940,8 +3192,11 @@
       <c r="K62">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>8</v>
       </c>
@@ -2975,8 +3230,11 @@
       <c r="K63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>8</v>
       </c>
@@ -3010,8 +3268,11 @@
       <c r="K64">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>8</v>
       </c>
@@ -3045,8 +3306,11 @@
       <c r="K65">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>8</v>
       </c>
@@ -3080,8 +3344,11 @@
       <c r="K66">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>9</v>
       </c>
@@ -3115,8 +3382,11 @@
       <c r="K67">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>9</v>
       </c>
@@ -3150,8 +3420,11 @@
       <c r="K68">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>10</v>
       </c>
@@ -3185,8 +3458,11 @@
       <c r="K69">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>10</v>
       </c>
@@ -3220,8 +3496,11 @@
       <c r="K70">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>10</v>
       </c>
@@ -3255,8 +3534,11 @@
       <c r="K71">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>10</v>
       </c>
@@ -3290,8 +3572,11 @@
       <c r="K72">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>10</v>
       </c>
@@ -3325,8 +3610,11 @@
       <c r="K73">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>10</v>
       </c>
@@ -3360,8 +3648,11 @@
       <c r="K74">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>10</v>
       </c>
@@ -3395,8 +3686,11 @@
       <c r="K75">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>10</v>
       </c>
@@ -3430,8 +3724,11 @@
       <c r="K76">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>10</v>
       </c>
@@ -3465,8 +3762,11 @@
       <c r="K77">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>10</v>
       </c>
@@ -3498,6 +3798,9 @@
         <v>0</v>
       </c>
       <c r="K78">
+        <v>0</v>
+      </c>
+      <c r="L78">
         <v>0</v>
       </c>
     </row>
@@ -3508,750 +3811,1454 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{209B6C40-D49A-460E-9F0A-D52ECA57AEC1}">
-  <dimension ref="A1:D82"/>
+  <dimension ref="A1:F94"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.7265625" customWidth="1"/>
-    <col min="2" max="2" width="73.81640625" customWidth="1"/>
-    <col min="3" max="3" width="26.7265625" customWidth="1"/>
-    <col min="4" max="4" width="37.26953125" customWidth="1"/>
-    <col min="5" max="5" width="23.90625" customWidth="1"/>
-    <col min="6" max="6" width="21.54296875" customWidth="1"/>
-    <col min="7" max="7" width="22.36328125" customWidth="1"/>
-    <col min="8" max="8" width="25.81640625" customWidth="1"/>
-    <col min="9" max="9" width="22.54296875" customWidth="1"/>
-    <col min="10" max="10" width="19.90625" customWidth="1"/>
-    <col min="11" max="11" width="20" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="24.77734375" customWidth="1"/>
+    <col min="4" max="4" width="73.77734375" customWidth="1"/>
+    <col min="5" max="5" width="26.77734375" customWidth="1"/>
+    <col min="6" max="6" width="41.5546875" customWidth="1"/>
+    <col min="7" max="7" width="23.88671875" customWidth="1"/>
+    <col min="8" max="8" width="21.5546875" customWidth="1"/>
+    <col min="9" max="9" width="22.33203125" customWidth="1"/>
+    <col min="10" max="10" width="25.77734375" customWidth="1"/>
+    <col min="11" max="11" width="22.5546875" customWidth="1"/>
+    <col min="12" max="12" width="19.88671875" customWidth="1"/>
+    <col min="13" max="13" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" s="6">
+        <v>1</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="6">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" s="6">
+        <v>1</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C4" s="6">
+        <v>1</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
+        <v>1</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C5" s="6">
+        <v>2</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="6">
+        <v>1</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C6" s="6">
+        <v>2</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="6">
+        <v>1</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C7" s="6">
+        <v>2</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="6">
+        <v>1</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C8" s="6">
+        <v>2</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="6">
+        <v>1</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C9" s="6">
+        <v>2</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="6">
+        <v>1</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C10" s="6">
+        <v>3</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="6">
+        <v>1</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C11" s="6">
+        <v>4</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="6">
+        <v>1</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C12" s="6">
+        <v>5</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="6">
+        <v>1</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C13" s="6">
+        <v>6</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>118</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
         <v>97</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E14" t="s">
         <v>110</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>118</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>118</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="38.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1" t="s">
+    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>118</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>118</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>118</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>118</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>118</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22" t="s">
+        <v>118</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="F22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>118</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="F23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="B24" t="s">
+        <v>118</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="F24" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14">
-        <v>1</v>
-      </c>
-      <c r="D14" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="B25" t="s">
+        <v>118</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="F25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>2</v>
+      </c>
+      <c r="B26" t="s">
+        <v>118</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="F26" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15">
-        <v>1</v>
-      </c>
-      <c r="D15" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>2</v>
+      </c>
+      <c r="B27" t="s">
+        <v>118</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="F27" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16">
-        <v>2</v>
-      </c>
-      <c r="B16" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>2</v>
+      </c>
+      <c r="B28" t="s">
+        <v>118</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28" t="s">
         <v>98</v>
       </c>
-      <c r="C16" t="s">
+      <c r="E28" t="s">
         <v>110</v>
       </c>
-      <c r="D16" t="s">
+      <c r="F28" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17">
-        <v>2</v>
-      </c>
-      <c r="D17" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>2</v>
+      </c>
+      <c r="B29" t="s">
+        <v>118</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="F29" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18">
-        <v>2</v>
-      </c>
-      <c r="D18" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>2</v>
+      </c>
+      <c r="B30" t="s">
+        <v>118</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="F30" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19">
-        <v>2</v>
-      </c>
-      <c r="D19" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>2</v>
+      </c>
+      <c r="B31" t="s">
+        <v>118</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="F31" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20">
-        <v>2</v>
-      </c>
-      <c r="D20" t="s">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>2</v>
+      </c>
+      <c r="B32" t="s">
+        <v>118</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="F32" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21">
-        <v>2</v>
-      </c>
-      <c r="D21" t="s">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>2</v>
+      </c>
+      <c r="B33" t="s">
+        <v>118</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="F33" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22">
-        <v>2</v>
-      </c>
-      <c r="D22" t="s">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>2</v>
+      </c>
+      <c r="B34" t="s">
+        <v>118</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="F34" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23">
-        <v>2</v>
-      </c>
-      <c r="D23" t="s">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>2</v>
+      </c>
+      <c r="B35" t="s">
+        <v>118</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+      <c r="F35" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24">
-        <v>2</v>
-      </c>
-      <c r="D24" t="s">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>2</v>
+      </c>
+      <c r="B36" t="s">
+        <v>118</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+      <c r="F36" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25">
-        <v>2</v>
-      </c>
-      <c r="D25" t="s">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>2</v>
+      </c>
+      <c r="B37" t="s">
+        <v>118</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+      <c r="F37" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26">
-        <v>2</v>
-      </c>
-      <c r="D26" t="s">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>2</v>
+      </c>
+      <c r="B38" t="s">
+        <v>118</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
+      </c>
+      <c r="F38" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27">
-        <v>2</v>
-      </c>
-      <c r="D27" t="s">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>2</v>
+      </c>
+      <c r="B39" t="s">
+        <v>118</v>
+      </c>
+      <c r="C39">
+        <v>2</v>
+      </c>
+      <c r="F39" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28">
-        <v>2</v>
-      </c>
-      <c r="D28" t="s">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>2</v>
+      </c>
+      <c r="B40" t="s">
+        <v>118</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
+      </c>
+      <c r="F40" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29">
-        <v>2</v>
-      </c>
-      <c r="D29" t="s">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>2</v>
+      </c>
+      <c r="B41" t="s">
+        <v>118</v>
+      </c>
+      <c r="C41">
+        <v>2</v>
+      </c>
+      <c r="F41" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30">
-        <v>2</v>
-      </c>
-      <c r="D30" t="s">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>2</v>
+      </c>
+      <c r="B42" t="s">
+        <v>118</v>
+      </c>
+      <c r="C42">
+        <v>2</v>
+      </c>
+      <c r="F42" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>2</v>
+      </c>
+      <c r="B43" t="s">
+        <v>118</v>
+      </c>
+      <c r="C43">
         <v>3</v>
       </c>
-      <c r="B31" t="s">
+      <c r="D43" t="s">
         <v>99</v>
       </c>
-      <c r="C31" t="s">
+      <c r="E43" t="s">
         <v>110</v>
       </c>
-      <c r="D31" t="s">
+      <c r="F43" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>2</v>
+      </c>
+      <c r="B44" t="s">
+        <v>118</v>
+      </c>
+      <c r="C44">
         <v>3</v>
       </c>
-      <c r="D32" t="s">
+      <c r="F44" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>2</v>
+      </c>
+      <c r="B45" t="s">
+        <v>118</v>
+      </c>
+      <c r="C45">
         <v>3</v>
       </c>
-      <c r="D33" t="s">
+      <c r="F45" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>2</v>
+      </c>
+      <c r="B46" t="s">
+        <v>118</v>
+      </c>
+      <c r="C46">
         <v>4</v>
       </c>
-      <c r="B34" t="s">
+      <c r="D46" t="s">
         <v>100</v>
       </c>
-      <c r="C34" t="s">
+      <c r="E46" t="s">
         <v>110</v>
       </c>
-      <c r="D34" t="s">
+      <c r="F46" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>2</v>
+      </c>
+      <c r="B47" t="s">
+        <v>118</v>
+      </c>
+      <c r="C47">
         <v>4</v>
       </c>
-      <c r="D35" t="s">
+      <c r="F47" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>2</v>
+      </c>
+      <c r="B48" t="s">
+        <v>118</v>
+      </c>
+      <c r="C48">
         <v>4</v>
       </c>
-      <c r="D36" t="s">
+      <c r="F48" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>2</v>
+      </c>
+      <c r="B49" t="s">
+        <v>118</v>
+      </c>
+      <c r="C49">
         <v>4</v>
       </c>
-      <c r="D37" t="s">
+      <c r="F49" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>2</v>
+      </c>
+      <c r="B50" t="s">
+        <v>118</v>
+      </c>
+      <c r="C50">
         <v>5</v>
       </c>
-      <c r="B38" t="s">
+      <c r="D50" t="s">
         <v>101</v>
       </c>
-      <c r="C38" t="s">
+      <c r="E50" t="s">
         <v>110</v>
       </c>
-      <c r="D38" t="s">
+      <c r="F50" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>2</v>
+      </c>
+      <c r="B51" t="s">
+        <v>118</v>
+      </c>
+      <c r="C51">
         <v>5</v>
       </c>
-      <c r="D39" t="s">
+      <c r="F51" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>2</v>
+      </c>
+      <c r="B52" t="s">
+        <v>118</v>
+      </c>
+      <c r="C52">
         <v>5</v>
       </c>
-      <c r="D40" t="s">
+      <c r="F52" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>2</v>
+      </c>
+      <c r="B53" t="s">
+        <v>118</v>
+      </c>
+      <c r="C53">
         <v>5</v>
       </c>
-      <c r="D41" t="s">
+      <c r="F53" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A42">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>2</v>
+      </c>
+      <c r="B54" t="s">
+        <v>118</v>
+      </c>
+      <c r="C54">
         <v>6</v>
       </c>
-      <c r="B42" t="s">
+      <c r="D54" t="s">
         <v>102</v>
       </c>
-      <c r="C42" t="s">
+      <c r="E54" t="s">
         <v>110</v>
       </c>
-      <c r="D42" t="s">
+      <c r="F54" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A43">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>2</v>
+      </c>
+      <c r="B55" t="s">
+        <v>118</v>
+      </c>
+      <c r="C55">
         <v>6</v>
       </c>
-      <c r="D43" t="s">
+      <c r="F55" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A44">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>2</v>
+      </c>
+      <c r="B56" t="s">
+        <v>118</v>
+      </c>
+      <c r="C56">
         <v>6</v>
       </c>
-      <c r="D44" t="s">
+      <c r="F56" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A45">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>2</v>
+      </c>
+      <c r="B57" t="s">
+        <v>118</v>
+      </c>
+      <c r="C57">
         <v>6</v>
       </c>
-      <c r="D45" t="s">
+      <c r="F57" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A46">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>2</v>
+      </c>
+      <c r="B58" t="s">
+        <v>118</v>
+      </c>
+      <c r="C58">
         <v>6</v>
       </c>
-      <c r="D46" t="s">
+      <c r="F58" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A47">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>2</v>
+      </c>
+      <c r="B59" t="s">
+        <v>118</v>
+      </c>
+      <c r="C59">
         <v>6</v>
       </c>
-      <c r="D47" t="s">
+      <c r="F59" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A48">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>2</v>
+      </c>
+      <c r="B60" t="s">
+        <v>118</v>
+      </c>
+      <c r="C60">
         <v>6</v>
       </c>
-      <c r="D48" t="s">
+      <c r="F60" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A49">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>2</v>
+      </c>
+      <c r="B61" t="s">
+        <v>118</v>
+      </c>
+      <c r="C61">
         <v>6</v>
       </c>
-      <c r="D49" t="s">
+      <c r="F61" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A50">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>2</v>
+      </c>
+      <c r="B62" t="s">
+        <v>118</v>
+      </c>
+      <c r="C62">
         <v>6</v>
       </c>
-      <c r="D50" t="s">
+      <c r="F62" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A51">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>2</v>
+      </c>
+      <c r="B63" t="s">
+        <v>118</v>
+      </c>
+      <c r="C63">
         <v>6</v>
       </c>
-      <c r="D51" t="s">
+      <c r="F63" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A52">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>2</v>
+      </c>
+      <c r="B64" t="s">
+        <v>118</v>
+      </c>
+      <c r="C64">
         <v>6</v>
       </c>
-      <c r="D52" t="s">
+      <c r="F64" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A53">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>2</v>
+      </c>
+      <c r="B65" t="s">
+        <v>118</v>
+      </c>
+      <c r="C65">
         <v>6</v>
       </c>
-      <c r="D53" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A54">
+      <c r="F65" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>2</v>
+      </c>
+      <c r="B66" t="s">
+        <v>118</v>
+      </c>
+      <c r="C66">
         <v>6</v>
       </c>
-      <c r="D54" t="s">
+      <c r="F66" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A55">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>2</v>
+      </c>
+      <c r="B67" t="s">
+        <v>118</v>
+      </c>
+      <c r="C67">
         <v>6</v>
       </c>
-      <c r="D55" t="s">
+      <c r="F67" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A56">
-        <v>7</v>
-      </c>
-      <c r="B56" t="s">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>3</v>
+      </c>
+      <c r="B68" t="s">
+        <v>119</v>
+      </c>
+      <c r="C68">
+        <v>1</v>
+      </c>
+      <c r="D68" t="s">
         <v>103</v>
       </c>
-      <c r="C56" t="s">
+      <c r="E68" t="s">
         <v>110</v>
       </c>
-      <c r="D56" t="s">
+      <c r="F68" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A57">
-        <v>7</v>
-      </c>
-      <c r="D57" t="s">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>3</v>
+      </c>
+      <c r="B69" t="s">
+        <v>119</v>
+      </c>
+      <c r="C69">
+        <v>1</v>
+      </c>
+      <c r="F69" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A58">
-        <v>7</v>
-      </c>
-      <c r="D58" t="s">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>3</v>
+      </c>
+      <c r="B70" t="s">
+        <v>119</v>
+      </c>
+      <c r="C70">
+        <v>1</v>
+      </c>
+      <c r="F70" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A59">
-        <v>7</v>
-      </c>
-      <c r="D59" t="s">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>3</v>
+      </c>
+      <c r="B71" t="s">
+        <v>119</v>
+      </c>
+      <c r="C71">
+        <v>1</v>
+      </c>
+      <c r="F71" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A60">
-        <v>7</v>
-      </c>
-      <c r="D60" t="s">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>3</v>
+      </c>
+      <c r="B72" t="s">
+        <v>119</v>
+      </c>
+      <c r="C72">
+        <v>1</v>
+      </c>
+      <c r="F72" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A61">
-        <v>7</v>
-      </c>
-      <c r="D61" t="s">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>3</v>
+      </c>
+      <c r="B73" t="s">
+        <v>119</v>
+      </c>
+      <c r="C73">
+        <v>1</v>
+      </c>
+      <c r="F73" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A62">
-        <v>8</v>
-      </c>
-      <c r="B62" t="s">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>3</v>
+      </c>
+      <c r="B74" t="s">
+        <v>119</v>
+      </c>
+      <c r="C74">
+        <v>2</v>
+      </c>
+      <c r="D74" t="s">
         <v>104</v>
       </c>
-      <c r="C62" t="s">
+      <c r="E74" t="s">
         <v>111</v>
       </c>
-      <c r="D62" t="s">
+      <c r="F74" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A63">
-        <v>8</v>
-      </c>
-      <c r="D63" t="s">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>3</v>
+      </c>
+      <c r="B75" t="s">
+        <v>119</v>
+      </c>
+      <c r="C75">
+        <v>2</v>
+      </c>
+      <c r="F75" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A64">
-        <v>8</v>
-      </c>
-      <c r="D64" t="s">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>3</v>
+      </c>
+      <c r="B76" t="s">
+        <v>119</v>
+      </c>
+      <c r="C76">
+        <v>2</v>
+      </c>
+      <c r="F76" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A65">
-        <v>8</v>
-      </c>
-      <c r="D65" t="s">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>3</v>
+      </c>
+      <c r="B77" t="s">
+        <v>119</v>
+      </c>
+      <c r="C77">
+        <v>2</v>
+      </c>
+      <c r="F77" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A66">
-        <v>8</v>
-      </c>
-      <c r="D66" t="s">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>3</v>
+      </c>
+      <c r="B78" t="s">
+        <v>119</v>
+      </c>
+      <c r="C78">
+        <v>2</v>
+      </c>
+      <c r="F78" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A67">
-        <v>9</v>
-      </c>
-      <c r="B67" t="s">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>3</v>
+      </c>
+      <c r="B79" t="s">
+        <v>119</v>
+      </c>
+      <c r="C79">
+        <v>3</v>
+      </c>
+      <c r="D79" t="s">
         <v>105</v>
       </c>
-      <c r="C67" t="s">
+      <c r="E79" t="s">
         <v>111</v>
       </c>
-      <c r="D67" t="s">
+      <c r="F79" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A68">
-        <v>9</v>
-      </c>
-      <c r="D68" t="s">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>3</v>
+      </c>
+      <c r="B80" t="s">
+        <v>119</v>
+      </c>
+      <c r="C80">
+        <v>3</v>
+      </c>
+      <c r="F80" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A69">
-        <v>10</v>
-      </c>
-      <c r="B69" t="s">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>3</v>
+      </c>
+      <c r="B81" t="s">
+        <v>119</v>
+      </c>
+      <c r="C81">
+        <v>4</v>
+      </c>
+      <c r="D81" t="s">
         <v>106</v>
       </c>
-      <c r="C69" t="s">
+      <c r="E81" t="s">
         <v>110</v>
       </c>
-      <c r="D69" t="s">
+      <c r="F81" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A70">
-        <v>10</v>
-      </c>
-      <c r="D70" t="s">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>3</v>
+      </c>
+      <c r="B82" t="s">
+        <v>119</v>
+      </c>
+      <c r="C82">
+        <v>4</v>
+      </c>
+      <c r="F82" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A71">
-        <v>10</v>
-      </c>
-      <c r="D71" t="s">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>3</v>
+      </c>
+      <c r="B83" t="s">
+        <v>119</v>
+      </c>
+      <c r="C83">
+        <v>4</v>
+      </c>
+      <c r="F83" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A72">
-        <v>10</v>
-      </c>
-      <c r="D72" t="s">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>3</v>
+      </c>
+      <c r="B84" t="s">
+        <v>119</v>
+      </c>
+      <c r="C84">
+        <v>4</v>
+      </c>
+      <c r="F84" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A73">
-        <v>10</v>
-      </c>
-      <c r="D73" t="s">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>3</v>
+      </c>
+      <c r="B85" t="s">
+        <v>119</v>
+      </c>
+      <c r="C85">
+        <v>4</v>
+      </c>
+      <c r="F85" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A74">
-        <v>10</v>
-      </c>
-      <c r="D74" t="s">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>3</v>
+      </c>
+      <c r="B86" t="s">
+        <v>119</v>
+      </c>
+      <c r="C86">
+        <v>4</v>
+      </c>
+      <c r="F86" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A75">
-        <v>10</v>
-      </c>
-      <c r="D75" t="s">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>3</v>
+      </c>
+      <c r="B87" t="s">
+        <v>119</v>
+      </c>
+      <c r="C87">
+        <v>4</v>
+      </c>
+      <c r="F87" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A76">
-        <v>10</v>
-      </c>
-      <c r="D76" t="s">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>3</v>
+      </c>
+      <c r="B88" t="s">
+        <v>119</v>
+      </c>
+      <c r="C88">
+        <v>4</v>
+      </c>
+      <c r="F88" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A77">
-        <v>10</v>
-      </c>
-      <c r="D77" t="s">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>3</v>
+      </c>
+      <c r="B89" t="s">
+        <v>119</v>
+      </c>
+      <c r="C89">
+        <v>4</v>
+      </c>
+      <c r="F89" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A78">
-        <v>10</v>
-      </c>
-      <c r="D78" t="s">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>3</v>
+      </c>
+      <c r="B90" t="s">
+        <v>119</v>
+      </c>
+      <c r="C90">
+        <v>4</v>
+      </c>
+      <c r="F90" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A79">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>4</v>
+      </c>
+      <c r="B91" t="s">
+        <v>120</v>
+      </c>
+      <c r="C91">
         <v>11</v>
       </c>
-      <c r="B79" t="s">
+      <c r="D91" t="s">
         <v>107</v>
       </c>
-      <c r="C79" t="s">
+      <c r="E91" t="s">
         <v>110</v>
       </c>
-      <c r="D79" t="s">
+      <c r="F91" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A80">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>4</v>
+      </c>
+      <c r="B92" t="s">
+        <v>120</v>
+      </c>
+      <c r="C92">
         <v>11</v>
       </c>
-      <c r="D80" t="s">
+      <c r="F92" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A81">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>4</v>
+      </c>
+      <c r="B93" t="s">
+        <v>120</v>
+      </c>
+      <c r="C93">
         <v>11</v>
       </c>
-      <c r="D81" t="s">
+      <c r="F93" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A82">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>4</v>
+      </c>
+      <c r="B94" t="s">
+        <v>120</v>
+      </c>
+      <c r="C94">
         <v>11</v>
       </c>
-      <c r="D82" t="s">
+      <c r="F94" t="s">
         <v>115</v>
       </c>
     </row>
@@ -4269,80 +5276,80 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.54296875" customWidth="1"/>
-    <col min="2" max="2" width="28.7265625" customWidth="1"/>
-    <col min="3" max="3" width="18.453125" customWidth="1"/>
-    <col min="4" max="4" width="18.90625" customWidth="1"/>
-    <col min="5" max="5" width="18.26953125" customWidth="1"/>
+    <col min="1" max="1" width="21.5546875" customWidth="1"/>
+    <col min="2" max="2" width="28.77734375" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" customWidth="1"/>
+    <col min="5" max="5" width="18.21875" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="29.1796875" customWidth="1"/>
-    <col min="8" max="8" width="15.08984375" customWidth="1"/>
-    <col min="9" max="9" width="13.26953125" customWidth="1"/>
-    <col min="10" max="10" width="29.1796875" customWidth="1"/>
-    <col min="11" max="11" width="21.7265625" customWidth="1"/>
-    <col min="12" max="12" width="18.54296875" customWidth="1"/>
-    <col min="13" max="13" width="15.7265625" customWidth="1"/>
-    <col min="16" max="16" width="11.1796875" customWidth="1"/>
-    <col min="17" max="17" width="18.26953125" customWidth="1"/>
+    <col min="7" max="7" width="29.21875" customWidth="1"/>
+    <col min="8" max="8" width="15.109375" customWidth="1"/>
+    <col min="9" max="9" width="13.21875" customWidth="1"/>
+    <col min="10" max="10" width="29.21875" customWidth="1"/>
+    <col min="11" max="11" width="21.77734375" customWidth="1"/>
+    <col min="12" max="12" width="18.5546875" customWidth="1"/>
+    <col min="13" max="13" width="15.77734375" customWidth="1"/>
+    <col min="16" max="16" width="11.21875" customWidth="1"/>
+    <col min="17" max="17" width="18.21875" customWidth="1"/>
     <col min="18" max="18" width="36" customWidth="1"/>
-    <col min="19" max="19" width="8.90625" customWidth="1"/>
+    <col min="19" max="19" width="8.88671875" customWidth="1"/>
     <col min="20" max="20" width="30" customWidth="1"/>
-    <col min="21" max="21" width="12.81640625" customWidth="1"/>
-    <col min="22" max="22" width="11.6328125" customWidth="1"/>
-    <col min="23" max="23" width="11.36328125" customWidth="1"/>
-    <col min="24" max="24" width="15.453125" customWidth="1"/>
-    <col min="25" max="25" width="31.54296875" customWidth="1"/>
-    <col min="26" max="26" width="20.36328125" customWidth="1"/>
-    <col min="27" max="27" width="10.7265625" customWidth="1"/>
-    <col min="28" max="28" width="18.90625" customWidth="1"/>
-    <col min="29" max="29" width="25.26953125" customWidth="1"/>
-    <col min="30" max="30" width="23.90625" customWidth="1"/>
-    <col min="31" max="31" width="18.81640625" customWidth="1"/>
-    <col min="32" max="32" width="11.54296875" customWidth="1"/>
-    <col min="33" max="33" width="17.6328125" customWidth="1"/>
-    <col min="34" max="34" width="26.453125" customWidth="1"/>
-    <col min="35" max="35" width="15.90625" customWidth="1"/>
-    <col min="36" max="36" width="33.1796875" customWidth="1"/>
-    <col min="37" max="37" width="34.7265625" customWidth="1"/>
-    <col min="38" max="38" width="15.1796875" customWidth="1"/>
+    <col min="21" max="21" width="12.77734375" customWidth="1"/>
+    <col min="22" max="22" width="11.6640625" customWidth="1"/>
+    <col min="23" max="23" width="11.33203125" customWidth="1"/>
+    <col min="24" max="24" width="15.44140625" customWidth="1"/>
+    <col min="25" max="25" width="31.5546875" customWidth="1"/>
+    <col min="26" max="26" width="20.33203125" customWidth="1"/>
+    <col min="27" max="27" width="10.77734375" customWidth="1"/>
+    <col min="28" max="28" width="18.88671875" customWidth="1"/>
+    <col min="29" max="29" width="25.21875" customWidth="1"/>
+    <col min="30" max="30" width="23.88671875" customWidth="1"/>
+    <col min="31" max="31" width="18.77734375" customWidth="1"/>
+    <col min="32" max="32" width="11.5546875" customWidth="1"/>
+    <col min="33" max="33" width="17.6640625" customWidth="1"/>
+    <col min="34" max="34" width="26.44140625" customWidth="1"/>
+    <col min="35" max="35" width="15.88671875" customWidth="1"/>
+    <col min="36" max="36" width="33.21875" customWidth="1"/>
+    <col min="37" max="37" width="34.77734375" customWidth="1"/>
+    <col min="38" max="38" width="15.21875" customWidth="1"/>
     <col min="39" max="39" width="33" customWidth="1"/>
     <col min="40" max="40" width="32" customWidth="1"/>
-    <col min="41" max="41" width="25.54296875" customWidth="1"/>
-    <col min="42" max="42" width="11.26953125" customWidth="1"/>
-    <col min="43" max="43" width="14.453125" customWidth="1"/>
-    <col min="44" max="44" width="31.36328125" customWidth="1"/>
-    <col min="45" max="45" width="23.1796875" customWidth="1"/>
-    <col min="46" max="46" width="34.453125" customWidth="1"/>
-    <col min="47" max="47" width="12.453125" customWidth="1"/>
-    <col min="48" max="48" width="10.7265625" customWidth="1"/>
-    <col min="49" max="49" width="17.6328125" customWidth="1"/>
-    <col min="52" max="52" width="13.08984375" customWidth="1"/>
-    <col min="53" max="53" width="14.26953125" customWidth="1"/>
-    <col min="54" max="54" width="17.81640625" customWidth="1"/>
-    <col min="55" max="55" width="10.54296875" customWidth="1"/>
-    <col min="56" max="56" width="18.1796875" customWidth="1"/>
-    <col min="57" max="57" width="10.90625" customWidth="1"/>
-    <col min="58" max="58" width="14.1796875" customWidth="1"/>
-    <col min="59" max="59" width="9.08984375" customWidth="1"/>
-    <col min="61" max="61" width="11.1796875" customWidth="1"/>
-    <col min="63" max="63" width="16.453125" customWidth="1"/>
-    <col min="64" max="64" width="17.7265625" customWidth="1"/>
-    <col min="65" max="65" width="18.36328125" customWidth="1"/>
-    <col min="66" max="66" width="22.26953125" customWidth="1"/>
-    <col min="67" max="67" width="13.54296875" customWidth="1"/>
-    <col min="69" max="69" width="13.453125" customWidth="1"/>
-    <col min="70" max="70" width="24.26953125" customWidth="1"/>
-    <col min="72" max="72" width="14.26953125" customWidth="1"/>
-    <col min="74" max="74" width="12.81640625" customWidth="1"/>
-    <col min="75" max="75" width="22.36328125" customWidth="1"/>
-    <col min="77" max="77" width="27.26953125" customWidth="1"/>
-    <col min="78" max="78" width="26.54296875" customWidth="1"/>
-    <col min="80" max="80" width="11.90625" customWidth="1"/>
+    <col min="41" max="41" width="25.5546875" customWidth="1"/>
+    <col min="42" max="42" width="11.21875" customWidth="1"/>
+    <col min="43" max="43" width="14.44140625" customWidth="1"/>
+    <col min="44" max="44" width="31.33203125" customWidth="1"/>
+    <col min="45" max="45" width="23.21875" customWidth="1"/>
+    <col min="46" max="46" width="34.44140625" customWidth="1"/>
+    <col min="47" max="47" width="12.44140625" customWidth="1"/>
+    <col min="48" max="48" width="10.77734375" customWidth="1"/>
+    <col min="49" max="49" width="17.6640625" customWidth="1"/>
+    <col min="52" max="52" width="13.109375" customWidth="1"/>
+    <col min="53" max="53" width="14.21875" customWidth="1"/>
+    <col min="54" max="54" width="17.77734375" customWidth="1"/>
+    <col min="55" max="55" width="10.5546875" customWidth="1"/>
+    <col min="56" max="56" width="18.21875" customWidth="1"/>
+    <col min="57" max="57" width="10.88671875" customWidth="1"/>
+    <col min="58" max="58" width="14.21875" customWidth="1"/>
+    <col min="59" max="59" width="9.109375" customWidth="1"/>
+    <col min="61" max="61" width="11.21875" customWidth="1"/>
+    <col min="63" max="63" width="16.44140625" customWidth="1"/>
+    <col min="64" max="64" width="17.77734375" customWidth="1"/>
+    <col min="65" max="65" width="18.33203125" customWidth="1"/>
+    <col min="66" max="66" width="22.21875" customWidth="1"/>
+    <col min="67" max="67" width="13.5546875" customWidth="1"/>
+    <col min="69" max="69" width="13.44140625" customWidth="1"/>
+    <col min="70" max="70" width="24.21875" customWidth="1"/>
+    <col min="72" max="72" width="14.21875" customWidth="1"/>
+    <col min="74" max="74" width="12.77734375" customWidth="1"/>
+    <col min="75" max="75" width="22.33203125" customWidth="1"/>
+    <col min="77" max="77" width="27.21875" customWidth="1"/>
+    <col min="78" max="78" width="26.5546875" customWidth="1"/>
+    <col min="80" max="80" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:78" ht="59" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:78" ht="58.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>73</v>
       </c>
@@ -4578,7 +5585,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>79</v>
       </c>
@@ -4814,7 +5821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>78</v>
       </c>
@@ -5050,7 +6057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>77</v>
       </c>
@@ -5286,7 +6293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>82</v>
       </c>
@@ -5522,7 +6529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>76</v>
       </c>
@@ -5758,7 +6765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>75</v>
       </c>
@@ -5994,7 +7001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>74</v>
       </c>
@@ -6230,7 +7237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>80</v>
       </c>
@@ -6466,7 +7473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>81</v>
       </c>
@@ -6702,7 +7709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>83</v>
       </c>

</xml_diff>

<commit_message>
database upload and model training using excel.
</commit_message>
<xml_diff>
--- a/data/quiz-data.xlsx
+++ b/data/quiz-data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VIT\Placement\Internship\SFS intern\Project-Backend\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aditya\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F549E466-061C-41C8-AB89-2F178B2FAE06}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4AA851C-F8CB-49D5-B156-A4F50A24326A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Training" sheetId="3" r:id="rId1"/>
@@ -396,9 +396,6 @@
     <t>About You</t>
   </si>
   <si>
-    <t>Gender</t>
-  </si>
-  <si>
     <t>Male</t>
   </si>
   <si>
@@ -439,6 +436,9 @@
   </si>
   <si>
     <t>Dersired weight</t>
+  </si>
+  <si>
+    <t>Gender 1234</t>
   </si>
 </sst>
 </file>
@@ -824,23 +824,23 @@
       <selection activeCell="C2" sqref="C2:C78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.21875" customWidth="1"/>
-    <col min="2" max="2" width="35.33203125" customWidth="1"/>
-    <col min="3" max="3" width="15.77734375" customWidth="1"/>
-    <col min="4" max="4" width="16.21875" customWidth="1"/>
-    <col min="5" max="5" width="16.77734375" customWidth="1"/>
-    <col min="6" max="6" width="15.77734375" customWidth="1"/>
+    <col min="1" max="1" width="20.1796875" customWidth="1"/>
+    <col min="2" max="2" width="35.36328125" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" customWidth="1"/>
+    <col min="4" max="4" width="16.1796875" customWidth="1"/>
+    <col min="5" max="5" width="16.81640625" customWidth="1"/>
+    <col min="6" max="6" width="15.81640625" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="13.77734375" customWidth="1"/>
-    <col min="9" max="9" width="18.77734375" customWidth="1"/>
+    <col min="8" max="8" width="13.81640625" customWidth="1"/>
+    <col min="9" max="9" width="18.81640625" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
-    <col min="11" max="11" width="13.44140625" customWidth="1"/>
-    <col min="12" max="12" width="12.6640625" customWidth="1"/>
+    <col min="11" max="11" width="13.453125" customWidth="1"/>
+    <col min="12" max="12" width="12.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="50.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="54" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>95</v>
       </c>
@@ -878,7 +878,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -916,7 +916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -954,7 +954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1</v>
       </c>
@@ -992,7 +992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1030,7 +1030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1068,7 +1068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1106,7 +1106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1182,7 +1182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1220,7 +1220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1258,7 +1258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1296,7 +1296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1334,7 +1334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1372,7 +1372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1410,7 +1410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2</v>
       </c>
@@ -1448,7 +1448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1486,7 +1486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2</v>
       </c>
@@ -1524,7 +1524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1562,7 +1562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>2</v>
       </c>
@@ -1600,7 +1600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>2</v>
       </c>
@@ -1638,7 +1638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>2</v>
       </c>
@@ -1676,7 +1676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>2</v>
       </c>
@@ -1714,7 +1714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>2</v>
       </c>
@@ -1752,7 +1752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1790,7 +1790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>2</v>
       </c>
@@ -1828,7 +1828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>2</v>
       </c>
@@ -1866,7 +1866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>2</v>
       </c>
@@ -1904,7 +1904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>2</v>
       </c>
@@ -1942,7 +1942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>2</v>
       </c>
@@ -1980,7 +1980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>3</v>
       </c>
@@ -2018,7 +2018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>3</v>
       </c>
@@ -2056,7 +2056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>3</v>
       </c>
@@ -2094,7 +2094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>4</v>
       </c>
@@ -2132,7 +2132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>4</v>
       </c>
@@ -2170,7 +2170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>4</v>
       </c>
@@ -2208,7 +2208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>4</v>
       </c>
@@ -2246,7 +2246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>5</v>
       </c>
@@ -2284,7 +2284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>5</v>
       </c>
@@ -2322,7 +2322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>5</v>
       </c>
@@ -2360,7 +2360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>5</v>
       </c>
@@ -2398,7 +2398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>6</v>
       </c>
@@ -2436,7 +2436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>6</v>
       </c>
@@ -2474,7 +2474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>6</v>
       </c>
@@ -2512,7 +2512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>6</v>
       </c>
@@ -2550,7 +2550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>6</v>
       </c>
@@ -2588,7 +2588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>6</v>
       </c>
@@ -2626,7 +2626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>6</v>
       </c>
@@ -2664,7 +2664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>6</v>
       </c>
@@ -2702,7 +2702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>6</v>
       </c>
@@ -2740,7 +2740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>6</v>
       </c>
@@ -2778,7 +2778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>6</v>
       </c>
@@ -2816,7 +2816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>6</v>
       </c>
@@ -2854,7 +2854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>6</v>
       </c>
@@ -2892,7 +2892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>6</v>
       </c>
@@ -2930,7 +2930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>7</v>
       </c>
@@ -2968,7 +2968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>7</v>
       </c>
@@ -3006,7 +3006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>7</v>
       </c>
@@ -3044,7 +3044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>7</v>
       </c>
@@ -3082,7 +3082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>7</v>
       </c>
@@ -3120,7 +3120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>7</v>
       </c>
@@ -3158,7 +3158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>8</v>
       </c>
@@ -3196,7 +3196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>8</v>
       </c>
@@ -3234,7 +3234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>8</v>
       </c>
@@ -3272,7 +3272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>8</v>
       </c>
@@ -3310,7 +3310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>8</v>
       </c>
@@ -3348,7 +3348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>9</v>
       </c>
@@ -3386,7 +3386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>9</v>
       </c>
@@ -3424,7 +3424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>10</v>
       </c>
@@ -3462,7 +3462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>10</v>
       </c>
@@ -3500,7 +3500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>10</v>
       </c>
@@ -3538,7 +3538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>10</v>
       </c>
@@ -3576,7 +3576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>10</v>
       </c>
@@ -3614,7 +3614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>10</v>
       </c>
@@ -3652,7 +3652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>10</v>
       </c>
@@ -3690,7 +3690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>10</v>
       </c>
@@ -3728,7 +3728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>10</v>
       </c>
@@ -3766,7 +3766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>10</v>
       </c>
@@ -3814,27 +3814,27 @@
   <dimension ref="A1:F94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" customWidth="1"/>
+    <col min="1" max="1" width="17.90625" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="24.77734375" customWidth="1"/>
-    <col min="4" max="4" width="73.77734375" customWidth="1"/>
-    <col min="5" max="5" width="26.77734375" customWidth="1"/>
-    <col min="6" max="6" width="41.5546875" customWidth="1"/>
-    <col min="7" max="7" width="23.88671875" customWidth="1"/>
-    <col min="8" max="8" width="21.5546875" customWidth="1"/>
-    <col min="9" max="9" width="22.33203125" customWidth="1"/>
-    <col min="10" max="10" width="25.77734375" customWidth="1"/>
-    <col min="11" max="11" width="22.5546875" customWidth="1"/>
-    <col min="12" max="12" width="19.88671875" customWidth="1"/>
+    <col min="3" max="3" width="24.81640625" customWidth="1"/>
+    <col min="4" max="4" width="73.81640625" customWidth="1"/>
+    <col min="5" max="5" width="26.81640625" customWidth="1"/>
+    <col min="6" max="6" width="41.54296875" customWidth="1"/>
+    <col min="7" max="7" width="23.90625" customWidth="1"/>
+    <col min="8" max="8" width="21.54296875" customWidth="1"/>
+    <col min="9" max="9" width="22.36328125" customWidth="1"/>
+    <col min="10" max="10" width="25.81640625" customWidth="1"/>
+    <col min="11" max="11" width="22.54296875" customWidth="1"/>
+    <col min="12" max="12" width="19.90625" customWidth="1"/>
     <col min="13" max="13" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>116</v>
       </c>
@@ -3854,7 +3854,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -3865,16 +3865,16 @@
         <v>1</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>111</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -3887,10 +3887,10 @@
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
         <v>1</v>
       </c>
@@ -3903,10 +3903,10 @@
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
         <v>1</v>
       </c>
@@ -3917,16 +3917,16 @@
         <v>2</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>111</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>1</v>
       </c>
@@ -3939,10 +3939,10 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>1</v>
       </c>
@@ -3955,10 +3955,10 @@
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="8" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
         <v>1</v>
       </c>
@@ -3971,10 +3971,10 @@
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="8" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6">
         <v>1</v>
       </c>
@@ -3987,10 +3987,10 @@
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="8" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="6">
         <v>1</v>
       </c>
@@ -4001,14 +4001,14 @@
         <v>3</v>
       </c>
       <c r="D10" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="E10" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="E10" s="6" t="s">
-        <v>133</v>
-      </c>
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <v>1</v>
       </c>
@@ -4019,14 +4019,14 @@
         <v>4</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="6">
         <v>1</v>
       </c>
@@ -4037,14 +4037,14 @@
         <v>5</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="6">
         <v>1</v>
       </c>
@@ -4055,14 +4055,14 @@
         <v>6</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F13" s="7"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2</v>
       </c>
@@ -4082,7 +4082,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2</v>
       </c>
@@ -4096,7 +4096,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2</v>
       </c>
@@ -4110,7 +4110,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2</v>
       </c>
@@ -4124,7 +4124,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2</v>
       </c>
@@ -4138,7 +4138,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>2</v>
       </c>
@@ -4152,7 +4152,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>2</v>
       </c>
@@ -4166,7 +4166,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>2</v>
       </c>
@@ -4180,7 +4180,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>2</v>
       </c>
@@ -4194,7 +4194,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>2</v>
       </c>
@@ -4208,7 +4208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>2</v>
       </c>
@@ -4222,7 +4222,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>2</v>
       </c>
@@ -4236,7 +4236,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>2</v>
       </c>
@@ -4250,7 +4250,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>2</v>
       </c>
@@ -4264,7 +4264,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>2</v>
       </c>
@@ -4284,7 +4284,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>2</v>
       </c>
@@ -4298,7 +4298,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>2</v>
       </c>
@@ -4312,7 +4312,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>2</v>
       </c>
@@ -4326,7 +4326,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>2</v>
       </c>
@@ -4340,7 +4340,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>2</v>
       </c>
@@ -4354,7 +4354,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>2</v>
       </c>
@@ -4368,7 +4368,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>2</v>
       </c>
@@ -4382,7 +4382,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>2</v>
       </c>
@@ -4396,7 +4396,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>2</v>
       </c>
@@ -4410,7 +4410,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>2</v>
       </c>
@@ -4424,7 +4424,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>2</v>
       </c>
@@ -4438,7 +4438,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>2</v>
       </c>
@@ -4452,7 +4452,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>2</v>
       </c>
@@ -4466,7 +4466,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>2</v>
       </c>
@@ -4480,7 +4480,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>2</v>
       </c>
@@ -4500,7 +4500,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>2</v>
       </c>
@@ -4514,7 +4514,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>2</v>
       </c>
@@ -4528,7 +4528,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>2</v>
       </c>
@@ -4548,7 +4548,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>2</v>
       </c>
@@ -4562,7 +4562,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>2</v>
       </c>
@@ -4576,7 +4576,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>2</v>
       </c>
@@ -4590,7 +4590,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>2</v>
       </c>
@@ -4610,7 +4610,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>2</v>
       </c>
@@ -4624,7 +4624,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>2</v>
       </c>
@@ -4638,7 +4638,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>2</v>
       </c>
@@ -4652,7 +4652,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>2</v>
       </c>
@@ -4672,7 +4672,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>2</v>
       </c>
@@ -4686,7 +4686,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>2</v>
       </c>
@@ -4700,7 +4700,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>2</v>
       </c>
@@ -4714,7 +4714,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>2</v>
       </c>
@@ -4728,7 +4728,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>2</v>
       </c>
@@ -4742,7 +4742,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>2</v>
       </c>
@@ -4756,7 +4756,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>2</v>
       </c>
@@ -4770,7 +4770,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>2</v>
       </c>
@@ -4784,7 +4784,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>2</v>
       </c>
@@ -4798,7 +4798,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>2</v>
       </c>
@@ -4812,7 +4812,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>2</v>
       </c>
@@ -4826,7 +4826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>2</v>
       </c>
@@ -4840,7 +4840,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>2</v>
       </c>
@@ -4854,7 +4854,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>3</v>
       </c>
@@ -4874,7 +4874,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>3</v>
       </c>
@@ -4888,7 +4888,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>3</v>
       </c>
@@ -4902,7 +4902,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>3</v>
       </c>
@@ -4916,7 +4916,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>3</v>
       </c>
@@ -4930,7 +4930,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>3</v>
       </c>
@@ -4944,7 +4944,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>3</v>
       </c>
@@ -4964,7 +4964,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>3</v>
       </c>
@@ -4978,7 +4978,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>3</v>
       </c>
@@ -4992,7 +4992,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>3</v>
       </c>
@@ -5006,7 +5006,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>3</v>
       </c>
@@ -5020,7 +5020,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>3</v>
       </c>
@@ -5040,7 +5040,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>3</v>
       </c>
@@ -5054,7 +5054,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>3</v>
       </c>
@@ -5074,7 +5074,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>3</v>
       </c>
@@ -5088,7 +5088,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>3</v>
       </c>
@@ -5102,7 +5102,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>3</v>
       </c>
@@ -5116,7 +5116,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>3</v>
       </c>
@@ -5130,7 +5130,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>3</v>
       </c>
@@ -5144,7 +5144,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>3</v>
       </c>
@@ -5158,7 +5158,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>3</v>
       </c>
@@ -5172,7 +5172,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>3</v>
       </c>
@@ -5186,7 +5186,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>3</v>
       </c>
@@ -5200,7 +5200,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>4</v>
       </c>
@@ -5220,7 +5220,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>4</v>
       </c>
@@ -5234,7 +5234,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>4</v>
       </c>
@@ -5248,7 +5248,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>4</v>
       </c>
@@ -5276,80 +5276,80 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.5546875" customWidth="1"/>
-    <col min="2" max="2" width="28.77734375" customWidth="1"/>
-    <col min="3" max="3" width="18.44140625" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" customWidth="1"/>
-    <col min="5" max="5" width="18.21875" customWidth="1"/>
+    <col min="1" max="1" width="21.54296875" customWidth="1"/>
+    <col min="2" max="2" width="28.81640625" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" customWidth="1"/>
+    <col min="4" max="4" width="18.90625" customWidth="1"/>
+    <col min="5" max="5" width="18.1796875" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="29.21875" customWidth="1"/>
-    <col min="8" max="8" width="15.109375" customWidth="1"/>
-    <col min="9" max="9" width="13.21875" customWidth="1"/>
-    <col min="10" max="10" width="29.21875" customWidth="1"/>
-    <col min="11" max="11" width="21.77734375" customWidth="1"/>
-    <col min="12" max="12" width="18.5546875" customWidth="1"/>
-    <col min="13" max="13" width="15.77734375" customWidth="1"/>
-    <col min="16" max="16" width="11.21875" customWidth="1"/>
-    <col min="17" max="17" width="18.21875" customWidth="1"/>
+    <col min="7" max="7" width="29.1796875" customWidth="1"/>
+    <col min="8" max="8" width="15.08984375" customWidth="1"/>
+    <col min="9" max="9" width="13.1796875" customWidth="1"/>
+    <col min="10" max="10" width="29.1796875" customWidth="1"/>
+    <col min="11" max="11" width="21.81640625" customWidth="1"/>
+    <col min="12" max="12" width="18.54296875" customWidth="1"/>
+    <col min="13" max="13" width="15.81640625" customWidth="1"/>
+    <col min="16" max="16" width="11.1796875" customWidth="1"/>
+    <col min="17" max="17" width="18.1796875" customWidth="1"/>
     <col min="18" max="18" width="36" customWidth="1"/>
-    <col min="19" max="19" width="8.88671875" customWidth="1"/>
+    <col min="19" max="19" width="8.90625" customWidth="1"/>
     <col min="20" max="20" width="30" customWidth="1"/>
-    <col min="21" max="21" width="12.77734375" customWidth="1"/>
-    <col min="22" max="22" width="11.6640625" customWidth="1"/>
-    <col min="23" max="23" width="11.33203125" customWidth="1"/>
-    <col min="24" max="24" width="15.44140625" customWidth="1"/>
-    <col min="25" max="25" width="31.5546875" customWidth="1"/>
-    <col min="26" max="26" width="20.33203125" customWidth="1"/>
-    <col min="27" max="27" width="10.77734375" customWidth="1"/>
-    <col min="28" max="28" width="18.88671875" customWidth="1"/>
-    <col min="29" max="29" width="25.21875" customWidth="1"/>
-    <col min="30" max="30" width="23.88671875" customWidth="1"/>
-    <col min="31" max="31" width="18.77734375" customWidth="1"/>
-    <col min="32" max="32" width="11.5546875" customWidth="1"/>
-    <col min="33" max="33" width="17.6640625" customWidth="1"/>
-    <col min="34" max="34" width="26.44140625" customWidth="1"/>
-    <col min="35" max="35" width="15.88671875" customWidth="1"/>
-    <col min="36" max="36" width="33.21875" customWidth="1"/>
-    <col min="37" max="37" width="34.77734375" customWidth="1"/>
-    <col min="38" max="38" width="15.21875" customWidth="1"/>
+    <col min="21" max="21" width="12.81640625" customWidth="1"/>
+    <col min="22" max="22" width="11.6328125" customWidth="1"/>
+    <col min="23" max="23" width="11.36328125" customWidth="1"/>
+    <col min="24" max="24" width="15.453125" customWidth="1"/>
+    <col min="25" max="25" width="31.54296875" customWidth="1"/>
+    <col min="26" max="26" width="20.36328125" customWidth="1"/>
+    <col min="27" max="27" width="10.81640625" customWidth="1"/>
+    <col min="28" max="28" width="18.90625" customWidth="1"/>
+    <col min="29" max="29" width="25.1796875" customWidth="1"/>
+    <col min="30" max="30" width="23.90625" customWidth="1"/>
+    <col min="31" max="31" width="18.81640625" customWidth="1"/>
+    <col min="32" max="32" width="11.54296875" customWidth="1"/>
+    <col min="33" max="33" width="17.6328125" customWidth="1"/>
+    <col min="34" max="34" width="26.453125" customWidth="1"/>
+    <col min="35" max="35" width="15.90625" customWidth="1"/>
+    <col min="36" max="36" width="33.1796875" customWidth="1"/>
+    <col min="37" max="37" width="34.81640625" customWidth="1"/>
+    <col min="38" max="38" width="15.1796875" customWidth="1"/>
     <col min="39" max="39" width="33" customWidth="1"/>
     <col min="40" max="40" width="32" customWidth="1"/>
-    <col min="41" max="41" width="25.5546875" customWidth="1"/>
-    <col min="42" max="42" width="11.21875" customWidth="1"/>
-    <col min="43" max="43" width="14.44140625" customWidth="1"/>
-    <col min="44" max="44" width="31.33203125" customWidth="1"/>
-    <col min="45" max="45" width="23.21875" customWidth="1"/>
-    <col min="46" max="46" width="34.44140625" customWidth="1"/>
-    <col min="47" max="47" width="12.44140625" customWidth="1"/>
-    <col min="48" max="48" width="10.77734375" customWidth="1"/>
-    <col min="49" max="49" width="17.6640625" customWidth="1"/>
-    <col min="52" max="52" width="13.109375" customWidth="1"/>
-    <col min="53" max="53" width="14.21875" customWidth="1"/>
-    <col min="54" max="54" width="17.77734375" customWidth="1"/>
-    <col min="55" max="55" width="10.5546875" customWidth="1"/>
-    <col min="56" max="56" width="18.21875" customWidth="1"/>
-    <col min="57" max="57" width="10.88671875" customWidth="1"/>
-    <col min="58" max="58" width="14.21875" customWidth="1"/>
-    <col min="59" max="59" width="9.109375" customWidth="1"/>
-    <col min="61" max="61" width="11.21875" customWidth="1"/>
-    <col min="63" max="63" width="16.44140625" customWidth="1"/>
-    <col min="64" max="64" width="17.77734375" customWidth="1"/>
-    <col min="65" max="65" width="18.33203125" customWidth="1"/>
-    <col min="66" max="66" width="22.21875" customWidth="1"/>
-    <col min="67" max="67" width="13.5546875" customWidth="1"/>
-    <col min="69" max="69" width="13.44140625" customWidth="1"/>
-    <col min="70" max="70" width="24.21875" customWidth="1"/>
-    <col min="72" max="72" width="14.21875" customWidth="1"/>
-    <col min="74" max="74" width="12.77734375" customWidth="1"/>
-    <col min="75" max="75" width="22.33203125" customWidth="1"/>
-    <col min="77" max="77" width="27.21875" customWidth="1"/>
-    <col min="78" max="78" width="26.5546875" customWidth="1"/>
-    <col min="80" max="80" width="11.88671875" customWidth="1"/>
+    <col min="41" max="41" width="25.54296875" customWidth="1"/>
+    <col min="42" max="42" width="11.1796875" customWidth="1"/>
+    <col min="43" max="43" width="14.453125" customWidth="1"/>
+    <col min="44" max="44" width="31.36328125" customWidth="1"/>
+    <col min="45" max="45" width="23.1796875" customWidth="1"/>
+    <col min="46" max="46" width="34.453125" customWidth="1"/>
+    <col min="47" max="47" width="12.453125" customWidth="1"/>
+    <col min="48" max="48" width="10.81640625" customWidth="1"/>
+    <col min="49" max="49" width="17.6328125" customWidth="1"/>
+    <col min="52" max="52" width="13.08984375" customWidth="1"/>
+    <col min="53" max="53" width="14.1796875" customWidth="1"/>
+    <col min="54" max="54" width="17.81640625" customWidth="1"/>
+    <col min="55" max="55" width="10.54296875" customWidth="1"/>
+    <col min="56" max="56" width="18.1796875" customWidth="1"/>
+    <col min="57" max="57" width="10.90625" customWidth="1"/>
+    <col min="58" max="58" width="14.1796875" customWidth="1"/>
+    <col min="59" max="59" width="9.08984375" customWidth="1"/>
+    <col min="61" max="61" width="11.1796875" customWidth="1"/>
+    <col min="63" max="63" width="16.453125" customWidth="1"/>
+    <col min="64" max="64" width="17.81640625" customWidth="1"/>
+    <col min="65" max="65" width="18.36328125" customWidth="1"/>
+    <col min="66" max="66" width="22.1796875" customWidth="1"/>
+    <col min="67" max="67" width="13.54296875" customWidth="1"/>
+    <col min="69" max="69" width="13.453125" customWidth="1"/>
+    <col min="70" max="70" width="24.1796875" customWidth="1"/>
+    <col min="72" max="72" width="14.1796875" customWidth="1"/>
+    <col min="74" max="74" width="12.81640625" customWidth="1"/>
+    <col min="75" max="75" width="22.36328125" customWidth="1"/>
+    <col min="77" max="77" width="27.1796875" customWidth="1"/>
+    <col min="78" max="78" width="26.54296875" customWidth="1"/>
+    <col min="80" max="80" width="11.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:78" ht="58.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:78" ht="59" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>73</v>
       </c>
@@ -5585,7 +5585,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>79</v>
       </c>
@@ -5821,7 +5821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>78</v>
       </c>
@@ -6057,7 +6057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>77</v>
       </c>
@@ -6293,7 +6293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>82</v>
       </c>
@@ -6529,7 +6529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>76</v>
       </c>
@@ -6765,7 +6765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>75</v>
       </c>
@@ -7001,7 +7001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>74</v>
       </c>
@@ -7237,7 +7237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>80</v>
       </c>
@@ -7473,7 +7473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>81</v>
       </c>
@@ -7709,7 +7709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>83</v>
       </c>

</xml_diff>

<commit_message>
Database update, swagger doc update
</commit_message>
<xml_diff>
--- a/data/quiz-data.xlsx
+++ b/data/quiz-data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aditya\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VIT\Placement\Internship\SFS intern\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4AA851C-F8CB-49D5-B156-A4F50A24326A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CCF839E-3819-4841-A665-5B121A1B1702}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Training" sheetId="3" r:id="rId1"/>
@@ -438,7 +438,7 @@
     <t>Dersired weight</t>
   </si>
   <si>
-    <t>Gender 1234</t>
+    <t>Gender 456123</t>
   </si>
 </sst>
 </file>
@@ -824,23 +824,23 @@
       <selection activeCell="C2" sqref="C2:C78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.1796875" customWidth="1"/>
-    <col min="2" max="2" width="35.36328125" customWidth="1"/>
-    <col min="3" max="3" width="15.81640625" customWidth="1"/>
-    <col min="4" max="4" width="16.1796875" customWidth="1"/>
-    <col min="5" max="5" width="16.81640625" customWidth="1"/>
-    <col min="6" max="6" width="15.81640625" customWidth="1"/>
+    <col min="1" max="1" width="20.21875" customWidth="1"/>
+    <col min="2" max="2" width="35.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.77734375" customWidth="1"/>
+    <col min="4" max="4" width="16.21875" customWidth="1"/>
+    <col min="5" max="5" width="16.77734375" customWidth="1"/>
+    <col min="6" max="6" width="15.77734375" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="13.81640625" customWidth="1"/>
-    <col min="9" max="9" width="18.81640625" customWidth="1"/>
+    <col min="8" max="8" width="13.77734375" customWidth="1"/>
+    <col min="9" max="9" width="18.77734375" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
-    <col min="11" max="11" width="13.453125" customWidth="1"/>
-    <col min="12" max="12" width="12.6328125" customWidth="1"/>
+    <col min="11" max="11" width="13.44140625" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="54" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="50.4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>95</v>
       </c>
@@ -878,7 +878,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -916,7 +916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -954,7 +954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -992,7 +992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1030,7 +1030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1068,7 +1068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1106,7 +1106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1182,7 +1182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1220,7 +1220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1258,7 +1258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1296,7 +1296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1334,7 +1334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1372,7 +1372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1410,7 +1410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2</v>
       </c>
@@ -1448,7 +1448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1486,7 +1486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2</v>
       </c>
@@ -1524,7 +1524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1562,7 +1562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2</v>
       </c>
@@ -1600,7 +1600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2</v>
       </c>
@@ -1638,7 +1638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2</v>
       </c>
@@ -1676,7 +1676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2</v>
       </c>
@@ -1714,7 +1714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2</v>
       </c>
@@ -1752,7 +1752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1790,7 +1790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2</v>
       </c>
@@ -1828,7 +1828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2</v>
       </c>
@@ -1866,7 +1866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2</v>
       </c>
@@ -1904,7 +1904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>2</v>
       </c>
@@ -1942,7 +1942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2</v>
       </c>
@@ -1980,7 +1980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>3</v>
       </c>
@@ -2018,7 +2018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>3</v>
       </c>
@@ -2056,7 +2056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>3</v>
       </c>
@@ -2094,7 +2094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>4</v>
       </c>
@@ -2132,7 +2132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>4</v>
       </c>
@@ -2170,7 +2170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>4</v>
       </c>
@@ -2208,7 +2208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>4</v>
       </c>
@@ -2246,7 +2246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>5</v>
       </c>
@@ -2284,7 +2284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>5</v>
       </c>
@@ -2322,7 +2322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>5</v>
       </c>
@@ -2360,7 +2360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>5</v>
       </c>
@@ -2398,7 +2398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>6</v>
       </c>
@@ -2436,7 +2436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>6</v>
       </c>
@@ -2474,7 +2474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>6</v>
       </c>
@@ -2512,7 +2512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>6</v>
       </c>
@@ -2550,7 +2550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>6</v>
       </c>
@@ -2588,7 +2588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>6</v>
       </c>
@@ -2626,7 +2626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>6</v>
       </c>
@@ -2664,7 +2664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>6</v>
       </c>
@@ -2702,7 +2702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>6</v>
       </c>
@@ -2740,7 +2740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>6</v>
       </c>
@@ -2778,7 +2778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>6</v>
       </c>
@@ -2816,7 +2816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>6</v>
       </c>
@@ -2854,7 +2854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>6</v>
       </c>
@@ -2892,7 +2892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>6</v>
       </c>
@@ -2930,7 +2930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>7</v>
       </c>
@@ -2968,7 +2968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>7</v>
       </c>
@@ -3006,7 +3006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>7</v>
       </c>
@@ -3044,7 +3044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>7</v>
       </c>
@@ -3082,7 +3082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>7</v>
       </c>
@@ -3120,7 +3120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>7</v>
       </c>
@@ -3158,7 +3158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>8</v>
       </c>
@@ -3196,7 +3196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>8</v>
       </c>
@@ -3234,7 +3234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>8</v>
       </c>
@@ -3272,7 +3272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>8</v>
       </c>
@@ -3310,7 +3310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>8</v>
       </c>
@@ -3348,7 +3348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>9</v>
       </c>
@@ -3386,7 +3386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>9</v>
       </c>
@@ -3424,7 +3424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>10</v>
       </c>
@@ -3462,7 +3462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>10</v>
       </c>
@@ -3500,7 +3500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>10</v>
       </c>
@@ -3538,7 +3538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>10</v>
       </c>
@@ -3576,7 +3576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>10</v>
       </c>
@@ -3614,7 +3614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>10</v>
       </c>
@@ -3652,7 +3652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>10</v>
       </c>
@@ -3690,7 +3690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>10</v>
       </c>
@@ -3728,7 +3728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>10</v>
       </c>
@@ -3766,7 +3766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>10</v>
       </c>
@@ -3814,27 +3814,27 @@
   <dimension ref="A1:F94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C94" sqref="C94"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.90625" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="24.81640625" customWidth="1"/>
-    <col min="4" max="4" width="73.81640625" customWidth="1"/>
-    <col min="5" max="5" width="26.81640625" customWidth="1"/>
-    <col min="6" max="6" width="41.54296875" customWidth="1"/>
-    <col min="7" max="7" width="23.90625" customWidth="1"/>
-    <col min="8" max="8" width="21.54296875" customWidth="1"/>
-    <col min="9" max="9" width="22.36328125" customWidth="1"/>
-    <col min="10" max="10" width="25.81640625" customWidth="1"/>
-    <col min="11" max="11" width="22.54296875" customWidth="1"/>
-    <col min="12" max="12" width="19.90625" customWidth="1"/>
+    <col min="3" max="3" width="24.77734375" customWidth="1"/>
+    <col min="4" max="4" width="73.77734375" customWidth="1"/>
+    <col min="5" max="5" width="26.77734375" customWidth="1"/>
+    <col min="6" max="6" width="41.5546875" customWidth="1"/>
+    <col min="7" max="7" width="23.88671875" customWidth="1"/>
+    <col min="8" max="8" width="21.5546875" customWidth="1"/>
+    <col min="9" max="9" width="22.33203125" customWidth="1"/>
+    <col min="10" max="10" width="25.77734375" customWidth="1"/>
+    <col min="11" max="11" width="22.5546875" customWidth="1"/>
+    <col min="12" max="12" width="19.88671875" customWidth="1"/>
     <col min="13" max="13" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>116</v>
       </c>
@@ -3854,7 +3854,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -3874,7 +3874,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -3890,7 +3890,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>1</v>
       </c>
@@ -3906,7 +3906,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>1</v>
       </c>
@@ -3926,7 +3926,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>1</v>
       </c>
@@ -3942,7 +3942,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>1</v>
       </c>
@@ -3958,7 +3958,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>1</v>
       </c>
@@ -3974,7 +3974,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>1</v>
       </c>
@@ -3990,7 +3990,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>1</v>
       </c>
@@ -4008,7 +4008,7 @@
       </c>
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>1</v>
       </c>
@@ -4026,7 +4026,7 @@
       </c>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>1</v>
       </c>
@@ -4044,7 +4044,7 @@
       </c>
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>1</v>
       </c>
@@ -4062,7 +4062,7 @@
       </c>
       <c r="F13" s="7"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2</v>
       </c>
@@ -4082,7 +4082,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2</v>
       </c>
@@ -4096,7 +4096,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2</v>
       </c>
@@ -4110,7 +4110,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2</v>
       </c>
@@ -4124,7 +4124,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2</v>
       </c>
@@ -4138,7 +4138,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2</v>
       </c>
@@ -4152,7 +4152,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2</v>
       </c>
@@ -4166,7 +4166,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2</v>
       </c>
@@ -4180,7 +4180,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2</v>
       </c>
@@ -4194,7 +4194,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2</v>
       </c>
@@ -4208,7 +4208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2</v>
       </c>
@@ -4222,7 +4222,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2</v>
       </c>
@@ -4236,7 +4236,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2</v>
       </c>
@@ -4250,7 +4250,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2</v>
       </c>
@@ -4264,7 +4264,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2</v>
       </c>
@@ -4284,7 +4284,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>2</v>
       </c>
@@ -4298,7 +4298,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2</v>
       </c>
@@ -4312,7 +4312,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>2</v>
       </c>
@@ -4326,7 +4326,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>2</v>
       </c>
@@ -4340,7 +4340,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>2</v>
       </c>
@@ -4354,7 +4354,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>2</v>
       </c>
@@ -4368,7 +4368,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>2</v>
       </c>
@@ -4382,7 +4382,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>2</v>
       </c>
@@ -4396,7 +4396,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>2</v>
       </c>
@@ -4410,7 +4410,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>2</v>
       </c>
@@ -4424,7 +4424,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>2</v>
       </c>
@@ -4438,7 +4438,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>2</v>
       </c>
@@ -4452,7 +4452,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>2</v>
       </c>
@@ -4466,7 +4466,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>2</v>
       </c>
@@ -4480,7 +4480,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>2</v>
       </c>
@@ -4500,7 +4500,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>2</v>
       </c>
@@ -4514,7 +4514,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>2</v>
       </c>
@@ -4528,7 +4528,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>2</v>
       </c>
@@ -4548,7 +4548,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>2</v>
       </c>
@@ -4562,7 +4562,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>2</v>
       </c>
@@ -4576,7 +4576,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>2</v>
       </c>
@@ -4590,7 +4590,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>2</v>
       </c>
@@ -4610,7 +4610,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>2</v>
       </c>
@@ -4624,7 +4624,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>2</v>
       </c>
@@ -4638,7 +4638,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>2</v>
       </c>
@@ -4652,7 +4652,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>2</v>
       </c>
@@ -4672,7 +4672,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>2</v>
       </c>
@@ -4686,7 +4686,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>2</v>
       </c>
@@ -4700,7 +4700,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>2</v>
       </c>
@@ -4714,7 +4714,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>2</v>
       </c>
@@ -4728,7 +4728,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>2</v>
       </c>
@@ -4742,7 +4742,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>2</v>
       </c>
@@ -4756,7 +4756,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>2</v>
       </c>
@@ -4770,7 +4770,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>2</v>
       </c>
@@ -4784,7 +4784,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>2</v>
       </c>
@@ -4798,7 +4798,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>2</v>
       </c>
@@ -4812,7 +4812,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>2</v>
       </c>
@@ -4826,7 +4826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>2</v>
       </c>
@@ -4840,7 +4840,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>2</v>
       </c>
@@ -4854,7 +4854,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>3</v>
       </c>
@@ -4874,7 +4874,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>3</v>
       </c>
@@ -4888,7 +4888,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>3</v>
       </c>
@@ -4902,7 +4902,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>3</v>
       </c>
@@ -4916,7 +4916,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>3</v>
       </c>
@@ -4930,7 +4930,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>3</v>
       </c>
@@ -4944,7 +4944,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>3</v>
       </c>
@@ -4964,7 +4964,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>3</v>
       </c>
@@ -4978,7 +4978,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>3</v>
       </c>
@@ -4992,7 +4992,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>3</v>
       </c>
@@ -5006,7 +5006,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>3</v>
       </c>
@@ -5020,7 +5020,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>3</v>
       </c>
@@ -5040,7 +5040,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>3</v>
       </c>
@@ -5054,7 +5054,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>3</v>
       </c>
@@ -5074,7 +5074,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>3</v>
       </c>
@@ -5088,7 +5088,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>3</v>
       </c>
@@ -5102,7 +5102,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>3</v>
       </c>
@@ -5116,7 +5116,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>3</v>
       </c>
@@ -5130,7 +5130,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>3</v>
       </c>
@@ -5144,7 +5144,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>3</v>
       </c>
@@ -5158,7 +5158,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>3</v>
       </c>
@@ -5172,7 +5172,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>3</v>
       </c>
@@ -5186,7 +5186,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>3</v>
       </c>
@@ -5200,7 +5200,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>4</v>
       </c>
@@ -5208,7 +5208,7 @@
         <v>120</v>
       </c>
       <c r="C91">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D91" t="s">
         <v>107</v>
@@ -5220,7 +5220,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>4</v>
       </c>
@@ -5228,13 +5228,13 @@
         <v>120</v>
       </c>
       <c r="C92">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F92" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>4</v>
       </c>
@@ -5242,13 +5242,13 @@
         <v>120</v>
       </c>
       <c r="C93">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F93" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>4</v>
       </c>
@@ -5256,7 +5256,7 @@
         <v>120</v>
       </c>
       <c r="C94">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F94" t="s">
         <v>115</v>
@@ -5276,80 +5276,80 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.54296875" customWidth="1"/>
-    <col min="2" max="2" width="28.81640625" customWidth="1"/>
-    <col min="3" max="3" width="18.453125" customWidth="1"/>
-    <col min="4" max="4" width="18.90625" customWidth="1"/>
-    <col min="5" max="5" width="18.1796875" customWidth="1"/>
+    <col min="1" max="1" width="21.5546875" customWidth="1"/>
+    <col min="2" max="2" width="28.77734375" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" customWidth="1"/>
+    <col min="5" max="5" width="18.21875" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="29.1796875" customWidth="1"/>
-    <col min="8" max="8" width="15.08984375" customWidth="1"/>
-    <col min="9" max="9" width="13.1796875" customWidth="1"/>
-    <col min="10" max="10" width="29.1796875" customWidth="1"/>
-    <col min="11" max="11" width="21.81640625" customWidth="1"/>
-    <col min="12" max="12" width="18.54296875" customWidth="1"/>
-    <col min="13" max="13" width="15.81640625" customWidth="1"/>
-    <col min="16" max="16" width="11.1796875" customWidth="1"/>
-    <col min="17" max="17" width="18.1796875" customWidth="1"/>
+    <col min="7" max="7" width="29.21875" customWidth="1"/>
+    <col min="8" max="8" width="15.109375" customWidth="1"/>
+    <col min="9" max="9" width="13.21875" customWidth="1"/>
+    <col min="10" max="10" width="29.21875" customWidth="1"/>
+    <col min="11" max="11" width="21.77734375" customWidth="1"/>
+    <col min="12" max="12" width="18.5546875" customWidth="1"/>
+    <col min="13" max="13" width="15.77734375" customWidth="1"/>
+    <col min="16" max="16" width="11.21875" customWidth="1"/>
+    <col min="17" max="17" width="18.21875" customWidth="1"/>
     <col min="18" max="18" width="36" customWidth="1"/>
-    <col min="19" max="19" width="8.90625" customWidth="1"/>
+    <col min="19" max="19" width="8.88671875" customWidth="1"/>
     <col min="20" max="20" width="30" customWidth="1"/>
-    <col min="21" max="21" width="12.81640625" customWidth="1"/>
-    <col min="22" max="22" width="11.6328125" customWidth="1"/>
-    <col min="23" max="23" width="11.36328125" customWidth="1"/>
-    <col min="24" max="24" width="15.453125" customWidth="1"/>
-    <col min="25" max="25" width="31.54296875" customWidth="1"/>
-    <col min="26" max="26" width="20.36328125" customWidth="1"/>
-    <col min="27" max="27" width="10.81640625" customWidth="1"/>
-    <col min="28" max="28" width="18.90625" customWidth="1"/>
-    <col min="29" max="29" width="25.1796875" customWidth="1"/>
-    <col min="30" max="30" width="23.90625" customWidth="1"/>
-    <col min="31" max="31" width="18.81640625" customWidth="1"/>
-    <col min="32" max="32" width="11.54296875" customWidth="1"/>
-    <col min="33" max="33" width="17.6328125" customWidth="1"/>
-    <col min="34" max="34" width="26.453125" customWidth="1"/>
-    <col min="35" max="35" width="15.90625" customWidth="1"/>
-    <col min="36" max="36" width="33.1796875" customWidth="1"/>
-    <col min="37" max="37" width="34.81640625" customWidth="1"/>
-    <col min="38" max="38" width="15.1796875" customWidth="1"/>
+    <col min="21" max="21" width="12.77734375" customWidth="1"/>
+    <col min="22" max="22" width="11.6640625" customWidth="1"/>
+    <col min="23" max="23" width="11.33203125" customWidth="1"/>
+    <col min="24" max="24" width="15.44140625" customWidth="1"/>
+    <col min="25" max="25" width="31.5546875" customWidth="1"/>
+    <col min="26" max="26" width="20.33203125" customWidth="1"/>
+    <col min="27" max="27" width="10.77734375" customWidth="1"/>
+    <col min="28" max="28" width="18.88671875" customWidth="1"/>
+    <col min="29" max="29" width="25.21875" customWidth="1"/>
+    <col min="30" max="30" width="23.88671875" customWidth="1"/>
+    <col min="31" max="31" width="18.77734375" customWidth="1"/>
+    <col min="32" max="32" width="11.5546875" customWidth="1"/>
+    <col min="33" max="33" width="17.6640625" customWidth="1"/>
+    <col min="34" max="34" width="26.44140625" customWidth="1"/>
+    <col min="35" max="35" width="15.88671875" customWidth="1"/>
+    <col min="36" max="36" width="33.21875" customWidth="1"/>
+    <col min="37" max="37" width="34.77734375" customWidth="1"/>
+    <col min="38" max="38" width="15.21875" customWidth="1"/>
     <col min="39" max="39" width="33" customWidth="1"/>
     <col min="40" max="40" width="32" customWidth="1"/>
-    <col min="41" max="41" width="25.54296875" customWidth="1"/>
-    <col min="42" max="42" width="11.1796875" customWidth="1"/>
-    <col min="43" max="43" width="14.453125" customWidth="1"/>
-    <col min="44" max="44" width="31.36328125" customWidth="1"/>
-    <col min="45" max="45" width="23.1796875" customWidth="1"/>
-    <col min="46" max="46" width="34.453125" customWidth="1"/>
-    <col min="47" max="47" width="12.453125" customWidth="1"/>
-    <col min="48" max="48" width="10.81640625" customWidth="1"/>
-    <col min="49" max="49" width="17.6328125" customWidth="1"/>
-    <col min="52" max="52" width="13.08984375" customWidth="1"/>
-    <col min="53" max="53" width="14.1796875" customWidth="1"/>
-    <col min="54" max="54" width="17.81640625" customWidth="1"/>
-    <col min="55" max="55" width="10.54296875" customWidth="1"/>
-    <col min="56" max="56" width="18.1796875" customWidth="1"/>
-    <col min="57" max="57" width="10.90625" customWidth="1"/>
-    <col min="58" max="58" width="14.1796875" customWidth="1"/>
-    <col min="59" max="59" width="9.08984375" customWidth="1"/>
-    <col min="61" max="61" width="11.1796875" customWidth="1"/>
-    <col min="63" max="63" width="16.453125" customWidth="1"/>
-    <col min="64" max="64" width="17.81640625" customWidth="1"/>
-    <col min="65" max="65" width="18.36328125" customWidth="1"/>
-    <col min="66" max="66" width="22.1796875" customWidth="1"/>
-    <col min="67" max="67" width="13.54296875" customWidth="1"/>
-    <col min="69" max="69" width="13.453125" customWidth="1"/>
-    <col min="70" max="70" width="24.1796875" customWidth="1"/>
-    <col min="72" max="72" width="14.1796875" customWidth="1"/>
-    <col min="74" max="74" width="12.81640625" customWidth="1"/>
-    <col min="75" max="75" width="22.36328125" customWidth="1"/>
-    <col min="77" max="77" width="27.1796875" customWidth="1"/>
-    <col min="78" max="78" width="26.54296875" customWidth="1"/>
-    <col min="80" max="80" width="11.90625" customWidth="1"/>
+    <col min="41" max="41" width="25.5546875" customWidth="1"/>
+    <col min="42" max="42" width="11.21875" customWidth="1"/>
+    <col min="43" max="43" width="14.44140625" customWidth="1"/>
+    <col min="44" max="44" width="31.33203125" customWidth="1"/>
+    <col min="45" max="45" width="23.21875" customWidth="1"/>
+    <col min="46" max="46" width="34.44140625" customWidth="1"/>
+    <col min="47" max="47" width="12.44140625" customWidth="1"/>
+    <col min="48" max="48" width="10.77734375" customWidth="1"/>
+    <col min="49" max="49" width="17.6640625" customWidth="1"/>
+    <col min="52" max="52" width="13.109375" customWidth="1"/>
+    <col min="53" max="53" width="14.21875" customWidth="1"/>
+    <col min="54" max="54" width="17.77734375" customWidth="1"/>
+    <col min="55" max="55" width="10.5546875" customWidth="1"/>
+    <col min="56" max="56" width="18.21875" customWidth="1"/>
+    <col min="57" max="57" width="10.88671875" customWidth="1"/>
+    <col min="58" max="58" width="14.21875" customWidth="1"/>
+    <col min="59" max="59" width="9.109375" customWidth="1"/>
+    <col min="61" max="61" width="11.21875" customWidth="1"/>
+    <col min="63" max="63" width="16.44140625" customWidth="1"/>
+    <col min="64" max="64" width="17.77734375" customWidth="1"/>
+    <col min="65" max="65" width="18.33203125" customWidth="1"/>
+    <col min="66" max="66" width="22.21875" customWidth="1"/>
+    <col min="67" max="67" width="13.5546875" customWidth="1"/>
+    <col min="69" max="69" width="13.44140625" customWidth="1"/>
+    <col min="70" max="70" width="24.21875" customWidth="1"/>
+    <col min="72" max="72" width="14.21875" customWidth="1"/>
+    <col min="74" max="74" width="12.77734375" customWidth="1"/>
+    <col min="75" max="75" width="22.33203125" customWidth="1"/>
+    <col min="77" max="77" width="27.21875" customWidth="1"/>
+    <col min="78" max="78" width="26.5546875" customWidth="1"/>
+    <col min="80" max="80" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:78" ht="59" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:78" ht="58.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>73</v>
       </c>
@@ -5585,7 +5585,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>79</v>
       </c>
@@ -5821,7 +5821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>78</v>
       </c>
@@ -6057,7 +6057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>77</v>
       </c>
@@ -6293,7 +6293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>82</v>
       </c>
@@ -6529,7 +6529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>76</v>
       </c>
@@ -6765,7 +6765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>75</v>
       </c>
@@ -7001,7 +7001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>74</v>
       </c>
@@ -7237,7 +7237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>80</v>
       </c>
@@ -7473,7 +7473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>81</v>
       </c>
@@ -7709,7 +7709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>83</v>
       </c>

</xml_diff>

<commit_message>
new meal planner algo
</commit_message>
<xml_diff>
--- a/data/quiz-data.xlsx
+++ b/data/quiz-data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VIT\Placement\Internship\SFS intern\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ninju\Internship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CCF839E-3819-4841-A665-5B121A1B1702}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBD50CE6-4F58-482E-B974-B84587B6BD09}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Training" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="145">
   <si>
     <t>Constipation</t>
   </si>
@@ -439,6 +439,30 @@
   </si>
   <si>
     <t>Gender 456123</t>
+  </si>
+  <si>
+    <t>Any particular food restrictions?</t>
+  </si>
+  <si>
+    <t>No Meat at all</t>
+  </si>
+  <si>
+    <t>No Red Meat only</t>
+  </si>
+  <si>
+    <t>No Fish</t>
+  </si>
+  <si>
+    <t>No Crustaceans</t>
+  </si>
+  <si>
+    <t>No Sea Food at all</t>
+  </si>
+  <si>
+    <t>No Milk &amp; Dairy products</t>
+  </si>
+  <si>
+    <t>No Eggs</t>
   </si>
 </sst>
 </file>
@@ -824,23 +848,23 @@
       <selection activeCell="C2" sqref="C2:C78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.21875" customWidth="1"/>
-    <col min="2" max="2" width="35.33203125" customWidth="1"/>
-    <col min="3" max="3" width="15.77734375" customWidth="1"/>
-    <col min="4" max="4" width="16.21875" customWidth="1"/>
-    <col min="5" max="5" width="16.77734375" customWidth="1"/>
-    <col min="6" max="6" width="15.77734375" customWidth="1"/>
+    <col min="1" max="1" width="20.1796875" customWidth="1"/>
+    <col min="2" max="2" width="35.36328125" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" customWidth="1"/>
+    <col min="4" max="4" width="16.1796875" customWidth="1"/>
+    <col min="5" max="5" width="16.81640625" customWidth="1"/>
+    <col min="6" max="6" width="15.81640625" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="13.77734375" customWidth="1"/>
-    <col min="9" max="9" width="18.77734375" customWidth="1"/>
+    <col min="8" max="8" width="13.81640625" customWidth="1"/>
+    <col min="9" max="9" width="18.81640625" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
-    <col min="11" max="11" width="13.44140625" customWidth="1"/>
-    <col min="12" max="12" width="12.6640625" customWidth="1"/>
+    <col min="11" max="11" width="13.453125" customWidth="1"/>
+    <col min="12" max="12" width="12.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="50.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="54" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>95</v>
       </c>
@@ -878,7 +902,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -916,7 +940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -954,7 +978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1</v>
       </c>
@@ -992,7 +1016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1030,7 +1054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1068,7 +1092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1106,7 +1130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1144,7 +1168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1182,7 +1206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1220,7 +1244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1258,7 +1282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1296,7 +1320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1334,7 +1358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1372,7 +1396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1410,7 +1434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2</v>
       </c>
@@ -1448,7 +1472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1486,7 +1510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2</v>
       </c>
@@ -1524,7 +1548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1562,7 +1586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>2</v>
       </c>
@@ -1600,7 +1624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>2</v>
       </c>
@@ -1638,7 +1662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>2</v>
       </c>
@@ -1676,7 +1700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>2</v>
       </c>
@@ -1714,7 +1738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>2</v>
       </c>
@@ -1752,7 +1776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1790,7 +1814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>2</v>
       </c>
@@ -1828,7 +1852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>2</v>
       </c>
@@ -1866,7 +1890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>2</v>
       </c>
@@ -1904,7 +1928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>2</v>
       </c>
@@ -1942,7 +1966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>2</v>
       </c>
@@ -1980,7 +2004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>3</v>
       </c>
@@ -2018,7 +2042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>3</v>
       </c>
@@ -2056,7 +2080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>3</v>
       </c>
@@ -2094,7 +2118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>4</v>
       </c>
@@ -2132,7 +2156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>4</v>
       </c>
@@ -2170,7 +2194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>4</v>
       </c>
@@ -2208,7 +2232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>4</v>
       </c>
@@ -2246,7 +2270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>5</v>
       </c>
@@ -2284,7 +2308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>5</v>
       </c>
@@ -2322,7 +2346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>5</v>
       </c>
@@ -2360,7 +2384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>5</v>
       </c>
@@ -2398,7 +2422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>6</v>
       </c>
@@ -2436,7 +2460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>6</v>
       </c>
@@ -2474,7 +2498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>6</v>
       </c>
@@ -2512,7 +2536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>6</v>
       </c>
@@ -2550,7 +2574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>6</v>
       </c>
@@ -2588,7 +2612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>6</v>
       </c>
@@ -2626,7 +2650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>6</v>
       </c>
@@ -2664,7 +2688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>6</v>
       </c>
@@ -2702,7 +2726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>6</v>
       </c>
@@ -2740,7 +2764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>6</v>
       </c>
@@ -2778,7 +2802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>6</v>
       </c>
@@ -2816,7 +2840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>6</v>
       </c>
@@ -2854,7 +2878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>6</v>
       </c>
@@ -2892,7 +2916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>6</v>
       </c>
@@ -2930,7 +2954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>7</v>
       </c>
@@ -2968,7 +2992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>7</v>
       </c>
@@ -3006,7 +3030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>7</v>
       </c>
@@ -3044,7 +3068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>7</v>
       </c>
@@ -3082,7 +3106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>7</v>
       </c>
@@ -3120,7 +3144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>7</v>
       </c>
@@ -3158,7 +3182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>8</v>
       </c>
@@ -3196,7 +3220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>8</v>
       </c>
@@ -3234,7 +3258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>8</v>
       </c>
@@ -3272,7 +3296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>8</v>
       </c>
@@ -3310,7 +3334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>8</v>
       </c>
@@ -3348,7 +3372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>9</v>
       </c>
@@ -3386,7 +3410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>9</v>
       </c>
@@ -3424,7 +3448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>10</v>
       </c>
@@ -3462,7 +3486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>10</v>
       </c>
@@ -3500,7 +3524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>10</v>
       </c>
@@ -3538,7 +3562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>10</v>
       </c>
@@ -3576,7 +3600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>10</v>
       </c>
@@ -3614,7 +3638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>10</v>
       </c>
@@ -3652,7 +3676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>10</v>
       </c>
@@ -3690,7 +3714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>10</v>
       </c>
@@ -3728,7 +3752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>10</v>
       </c>
@@ -3766,7 +3790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>10</v>
       </c>
@@ -3811,30 +3835,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{209B6C40-D49A-460E-9F0A-D52ECA57AEC1}">
-  <dimension ref="A1:F94"/>
+  <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C94" sqref="C94"/>
+    <sheetView tabSelected="1" topLeftCell="D88" workbookViewId="0">
+      <selection activeCell="F106" sqref="F106"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" customWidth="1"/>
+    <col min="1" max="1" width="17.90625" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="24.77734375" customWidth="1"/>
-    <col min="4" max="4" width="73.77734375" customWidth="1"/>
-    <col min="5" max="5" width="26.77734375" customWidth="1"/>
-    <col min="6" max="6" width="41.5546875" customWidth="1"/>
-    <col min="7" max="7" width="23.88671875" customWidth="1"/>
-    <col min="8" max="8" width="21.5546875" customWidth="1"/>
-    <col min="9" max="9" width="22.33203125" customWidth="1"/>
-    <col min="10" max="10" width="25.77734375" customWidth="1"/>
-    <col min="11" max="11" width="22.5546875" customWidth="1"/>
-    <col min="12" max="12" width="19.88671875" customWidth="1"/>
+    <col min="3" max="3" width="24.81640625" customWidth="1"/>
+    <col min="4" max="4" width="73.81640625" customWidth="1"/>
+    <col min="5" max="5" width="26.81640625" customWidth="1"/>
+    <col min="6" max="6" width="41.54296875" customWidth="1"/>
+    <col min="7" max="7" width="23.90625" customWidth="1"/>
+    <col min="8" max="8" width="21.54296875" customWidth="1"/>
+    <col min="9" max="9" width="22.36328125" customWidth="1"/>
+    <col min="10" max="10" width="25.81640625" customWidth="1"/>
+    <col min="11" max="11" width="22.54296875" customWidth="1"/>
+    <col min="12" max="12" width="19.90625" customWidth="1"/>
     <col min="13" max="13" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>116</v>
       </c>
@@ -3854,7 +3878,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -3874,7 +3898,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -3890,7 +3914,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
         <v>1</v>
       </c>
@@ -3906,7 +3930,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
         <v>1</v>
       </c>
@@ -3926,7 +3950,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>1</v>
       </c>
@@ -3942,7 +3966,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>1</v>
       </c>
@@ -3958,7 +3982,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
         <v>1</v>
       </c>
@@ -3974,7 +3998,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6">
         <v>1</v>
       </c>
@@ -3990,7 +4014,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="6">
         <v>1</v>
       </c>
@@ -4008,7 +4032,7 @@
       </c>
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <v>1</v>
       </c>
@@ -4026,7 +4050,7 @@
       </c>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="6">
         <v>1</v>
       </c>
@@ -4044,7 +4068,7 @@
       </c>
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="6">
         <v>1</v>
       </c>
@@ -4062,7 +4086,7 @@
       </c>
       <c r="F13" s="7"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2</v>
       </c>
@@ -4082,7 +4106,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2</v>
       </c>
@@ -4096,7 +4120,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2</v>
       </c>
@@ -4110,7 +4134,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2</v>
       </c>
@@ -4124,7 +4148,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2</v>
       </c>
@@ -4138,7 +4162,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>2</v>
       </c>
@@ -4152,7 +4176,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>2</v>
       </c>
@@ -4166,7 +4190,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>2</v>
       </c>
@@ -4180,7 +4204,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>2</v>
       </c>
@@ -4194,7 +4218,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>2</v>
       </c>
@@ -4208,7 +4232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>2</v>
       </c>
@@ -4222,7 +4246,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>2</v>
       </c>
@@ -4236,7 +4260,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>2</v>
       </c>
@@ -4250,7 +4274,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>2</v>
       </c>
@@ -4264,7 +4288,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>2</v>
       </c>
@@ -4284,7 +4308,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>2</v>
       </c>
@@ -4298,7 +4322,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>2</v>
       </c>
@@ -4312,7 +4336,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>2</v>
       </c>
@@ -4326,7 +4350,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>2</v>
       </c>
@@ -4340,7 +4364,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>2</v>
       </c>
@@ -4354,7 +4378,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>2</v>
       </c>
@@ -4368,7 +4392,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>2</v>
       </c>
@@ -4382,7 +4406,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>2</v>
       </c>
@@ -4396,7 +4420,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>2</v>
       </c>
@@ -4410,7 +4434,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>2</v>
       </c>
@@ -4424,7 +4448,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>2</v>
       </c>
@@ -4438,7 +4462,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>2</v>
       </c>
@@ -4452,7 +4476,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>2</v>
       </c>
@@ -4466,7 +4490,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>2</v>
       </c>
@@ -4480,7 +4504,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>2</v>
       </c>
@@ -4500,7 +4524,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>2</v>
       </c>
@@ -4514,7 +4538,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>2</v>
       </c>
@@ -4528,7 +4552,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>2</v>
       </c>
@@ -4548,7 +4572,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>2</v>
       </c>
@@ -4562,7 +4586,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>2</v>
       </c>
@@ -4576,7 +4600,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>2</v>
       </c>
@@ -4590,7 +4614,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>2</v>
       </c>
@@ -4610,7 +4634,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>2</v>
       </c>
@@ -4624,7 +4648,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>2</v>
       </c>
@@ -4638,7 +4662,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>2</v>
       </c>
@@ -4652,7 +4676,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>2</v>
       </c>
@@ -4672,7 +4696,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>2</v>
       </c>
@@ -4686,7 +4710,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>2</v>
       </c>
@@ -4700,7 +4724,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>2</v>
       </c>
@@ -4714,7 +4738,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>2</v>
       </c>
@@ -4728,7 +4752,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>2</v>
       </c>
@@ -4742,7 +4766,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>2</v>
       </c>
@@ -4756,7 +4780,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>2</v>
       </c>
@@ -4770,7 +4794,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>2</v>
       </c>
@@ -4784,7 +4808,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>2</v>
       </c>
@@ -4798,7 +4822,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>2</v>
       </c>
@@ -4812,7 +4836,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>2</v>
       </c>
@@ -4826,7 +4850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>2</v>
       </c>
@@ -4840,7 +4864,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>2</v>
       </c>
@@ -4854,7 +4878,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>3</v>
       </c>
@@ -4874,7 +4898,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>3</v>
       </c>
@@ -4888,7 +4912,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>3</v>
       </c>
@@ -4902,7 +4926,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>3</v>
       </c>
@@ -4916,7 +4940,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>3</v>
       </c>
@@ -4930,7 +4954,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>3</v>
       </c>
@@ -4944,7 +4968,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>3</v>
       </c>
@@ -4964,7 +4988,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>3</v>
       </c>
@@ -4978,7 +5002,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>3</v>
       </c>
@@ -4992,7 +5016,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>3</v>
       </c>
@@ -5006,7 +5030,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>3</v>
       </c>
@@ -5020,7 +5044,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>3</v>
       </c>
@@ -5040,7 +5064,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>3</v>
       </c>
@@ -5054,7 +5078,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>3</v>
       </c>
@@ -5074,7 +5098,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>3</v>
       </c>
@@ -5088,7 +5112,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>3</v>
       </c>
@@ -5102,7 +5126,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>3</v>
       </c>
@@ -5116,7 +5140,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>3</v>
       </c>
@@ -5130,7 +5154,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>3</v>
       </c>
@@ -5144,7 +5168,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>3</v>
       </c>
@@ -5158,7 +5182,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>3</v>
       </c>
@@ -5172,7 +5196,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>3</v>
       </c>
@@ -5186,7 +5210,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>3</v>
       </c>
@@ -5200,65 +5224,169 @@
         <v>22</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B91" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C91">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D91" t="s">
-        <v>107</v>
+        <v>137</v>
       </c>
       <c r="E91" t="s">
         <v>110</v>
       </c>
       <c r="F91" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A92">
+        <v>3</v>
+      </c>
+      <c r="B92" t="s">
+        <v>119</v>
+      </c>
+      <c r="C92">
+        <v>5</v>
+      </c>
+      <c r="F92" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A93">
+        <v>3</v>
+      </c>
+      <c r="B93" t="s">
+        <v>119</v>
+      </c>
+      <c r="C93">
+        <v>5</v>
+      </c>
+      <c r="F93" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A94">
+        <v>3</v>
+      </c>
+      <c r="B94" t="s">
+        <v>119</v>
+      </c>
+      <c r="C94">
+        <v>5</v>
+      </c>
+      <c r="F94" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A95">
+        <v>3</v>
+      </c>
+      <c r="B95" t="s">
+        <v>119</v>
+      </c>
+      <c r="C95">
+        <v>5</v>
+      </c>
+      <c r="F95" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A96">
+        <v>3</v>
+      </c>
+      <c r="B96" t="s">
+        <v>119</v>
+      </c>
+      <c r="C96">
+        <v>5</v>
+      </c>
+      <c r="F96" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A97">
+        <v>3</v>
+      </c>
+      <c r="B97" t="s">
+        <v>119</v>
+      </c>
+      <c r="C97">
+        <v>5</v>
+      </c>
+      <c r="F97" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A98">
+        <v>4</v>
+      </c>
+      <c r="B98" t="s">
+        <v>120</v>
+      </c>
+      <c r="C98">
+        <v>1</v>
+      </c>
+      <c r="D98" t="s">
+        <v>107</v>
+      </c>
+      <c r="E98" t="s">
+        <v>110</v>
+      </c>
+      <c r="F98" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A92">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A99">
         <v>4</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B99" t="s">
         <v>120</v>
       </c>
-      <c r="C92">
-        <v>1</v>
-      </c>
-      <c r="F92" t="s">
+      <c r="C99">
+        <v>1</v>
+      </c>
+      <c r="F99" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A93">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A100">
         <v>4</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B100" t="s">
         <v>120</v>
       </c>
-      <c r="C93">
-        <v>1</v>
-      </c>
-      <c r="F93" t="s">
+      <c r="C100">
+        <v>1</v>
+      </c>
+      <c r="F100" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A94">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A101">
         <v>4</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B101" t="s">
         <v>120</v>
       </c>
-      <c r="C94">
-        <v>1</v>
-      </c>
-      <c r="F94" t="s">
+      <c r="C101">
+        <v>1</v>
+      </c>
+      <c r="F101" t="s">
         <v>115</v>
       </c>
     </row>
@@ -5276,80 +5404,80 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.5546875" customWidth="1"/>
-    <col min="2" max="2" width="28.77734375" customWidth="1"/>
-    <col min="3" max="3" width="18.44140625" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" customWidth="1"/>
-    <col min="5" max="5" width="18.21875" customWidth="1"/>
+    <col min="1" max="1" width="21.54296875" customWidth="1"/>
+    <col min="2" max="2" width="28.81640625" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" customWidth="1"/>
+    <col min="4" max="4" width="18.90625" customWidth="1"/>
+    <col min="5" max="5" width="18.1796875" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="29.21875" customWidth="1"/>
-    <col min="8" max="8" width="15.109375" customWidth="1"/>
-    <col min="9" max="9" width="13.21875" customWidth="1"/>
-    <col min="10" max="10" width="29.21875" customWidth="1"/>
-    <col min="11" max="11" width="21.77734375" customWidth="1"/>
-    <col min="12" max="12" width="18.5546875" customWidth="1"/>
-    <col min="13" max="13" width="15.77734375" customWidth="1"/>
-    <col min="16" max="16" width="11.21875" customWidth="1"/>
-    <col min="17" max="17" width="18.21875" customWidth="1"/>
+    <col min="7" max="7" width="29.1796875" customWidth="1"/>
+    <col min="8" max="8" width="15.08984375" customWidth="1"/>
+    <col min="9" max="9" width="13.1796875" customWidth="1"/>
+    <col min="10" max="10" width="29.1796875" customWidth="1"/>
+    <col min="11" max="11" width="21.81640625" customWidth="1"/>
+    <col min="12" max="12" width="18.54296875" customWidth="1"/>
+    <col min="13" max="13" width="15.81640625" customWidth="1"/>
+    <col min="16" max="16" width="11.1796875" customWidth="1"/>
+    <col min="17" max="17" width="18.1796875" customWidth="1"/>
     <col min="18" max="18" width="36" customWidth="1"/>
-    <col min="19" max="19" width="8.88671875" customWidth="1"/>
+    <col min="19" max="19" width="8.90625" customWidth="1"/>
     <col min="20" max="20" width="30" customWidth="1"/>
-    <col min="21" max="21" width="12.77734375" customWidth="1"/>
-    <col min="22" max="22" width="11.6640625" customWidth="1"/>
-    <col min="23" max="23" width="11.33203125" customWidth="1"/>
-    <col min="24" max="24" width="15.44140625" customWidth="1"/>
-    <col min="25" max="25" width="31.5546875" customWidth="1"/>
-    <col min="26" max="26" width="20.33203125" customWidth="1"/>
-    <col min="27" max="27" width="10.77734375" customWidth="1"/>
-    <col min="28" max="28" width="18.88671875" customWidth="1"/>
-    <col min="29" max="29" width="25.21875" customWidth="1"/>
-    <col min="30" max="30" width="23.88671875" customWidth="1"/>
-    <col min="31" max="31" width="18.77734375" customWidth="1"/>
-    <col min="32" max="32" width="11.5546875" customWidth="1"/>
-    <col min="33" max="33" width="17.6640625" customWidth="1"/>
-    <col min="34" max="34" width="26.44140625" customWidth="1"/>
-    <col min="35" max="35" width="15.88671875" customWidth="1"/>
-    <col min="36" max="36" width="33.21875" customWidth="1"/>
-    <col min="37" max="37" width="34.77734375" customWidth="1"/>
-    <col min="38" max="38" width="15.21875" customWidth="1"/>
+    <col min="21" max="21" width="12.81640625" customWidth="1"/>
+    <col min="22" max="22" width="11.6328125" customWidth="1"/>
+    <col min="23" max="23" width="11.36328125" customWidth="1"/>
+    <col min="24" max="24" width="15.453125" customWidth="1"/>
+    <col min="25" max="25" width="31.54296875" customWidth="1"/>
+    <col min="26" max="26" width="20.36328125" customWidth="1"/>
+    <col min="27" max="27" width="10.81640625" customWidth="1"/>
+    <col min="28" max="28" width="18.90625" customWidth="1"/>
+    <col min="29" max="29" width="25.1796875" customWidth="1"/>
+    <col min="30" max="30" width="23.90625" customWidth="1"/>
+    <col min="31" max="31" width="18.81640625" customWidth="1"/>
+    <col min="32" max="32" width="11.54296875" customWidth="1"/>
+    <col min="33" max="33" width="17.6328125" customWidth="1"/>
+    <col min="34" max="34" width="26.453125" customWidth="1"/>
+    <col min="35" max="35" width="15.90625" customWidth="1"/>
+    <col min="36" max="36" width="33.1796875" customWidth="1"/>
+    <col min="37" max="37" width="34.81640625" customWidth="1"/>
+    <col min="38" max="38" width="15.1796875" customWidth="1"/>
     <col min="39" max="39" width="33" customWidth="1"/>
     <col min="40" max="40" width="32" customWidth="1"/>
-    <col min="41" max="41" width="25.5546875" customWidth="1"/>
-    <col min="42" max="42" width="11.21875" customWidth="1"/>
-    <col min="43" max="43" width="14.44140625" customWidth="1"/>
-    <col min="44" max="44" width="31.33203125" customWidth="1"/>
-    <col min="45" max="45" width="23.21875" customWidth="1"/>
-    <col min="46" max="46" width="34.44140625" customWidth="1"/>
-    <col min="47" max="47" width="12.44140625" customWidth="1"/>
-    <col min="48" max="48" width="10.77734375" customWidth="1"/>
-    <col min="49" max="49" width="17.6640625" customWidth="1"/>
-    <col min="52" max="52" width="13.109375" customWidth="1"/>
-    <col min="53" max="53" width="14.21875" customWidth="1"/>
-    <col min="54" max="54" width="17.77734375" customWidth="1"/>
-    <col min="55" max="55" width="10.5546875" customWidth="1"/>
-    <col min="56" max="56" width="18.21875" customWidth="1"/>
-    <col min="57" max="57" width="10.88671875" customWidth="1"/>
-    <col min="58" max="58" width="14.21875" customWidth="1"/>
-    <col min="59" max="59" width="9.109375" customWidth="1"/>
-    <col min="61" max="61" width="11.21875" customWidth="1"/>
-    <col min="63" max="63" width="16.44140625" customWidth="1"/>
-    <col min="64" max="64" width="17.77734375" customWidth="1"/>
-    <col min="65" max="65" width="18.33203125" customWidth="1"/>
-    <col min="66" max="66" width="22.21875" customWidth="1"/>
-    <col min="67" max="67" width="13.5546875" customWidth="1"/>
-    <col min="69" max="69" width="13.44140625" customWidth="1"/>
-    <col min="70" max="70" width="24.21875" customWidth="1"/>
-    <col min="72" max="72" width="14.21875" customWidth="1"/>
-    <col min="74" max="74" width="12.77734375" customWidth="1"/>
-    <col min="75" max="75" width="22.33203125" customWidth="1"/>
-    <col min="77" max="77" width="27.21875" customWidth="1"/>
-    <col min="78" max="78" width="26.5546875" customWidth="1"/>
-    <col min="80" max="80" width="11.88671875" customWidth="1"/>
+    <col min="41" max="41" width="25.54296875" customWidth="1"/>
+    <col min="42" max="42" width="11.1796875" customWidth="1"/>
+    <col min="43" max="43" width="14.453125" customWidth="1"/>
+    <col min="44" max="44" width="31.36328125" customWidth="1"/>
+    <col min="45" max="45" width="23.1796875" customWidth="1"/>
+    <col min="46" max="46" width="34.453125" customWidth="1"/>
+    <col min="47" max="47" width="12.453125" customWidth="1"/>
+    <col min="48" max="48" width="10.81640625" customWidth="1"/>
+    <col min="49" max="49" width="17.6328125" customWidth="1"/>
+    <col min="52" max="52" width="13.08984375" customWidth="1"/>
+    <col min="53" max="53" width="14.1796875" customWidth="1"/>
+    <col min="54" max="54" width="17.81640625" customWidth="1"/>
+    <col min="55" max="55" width="10.54296875" customWidth="1"/>
+    <col min="56" max="56" width="18.1796875" customWidth="1"/>
+    <col min="57" max="57" width="10.90625" customWidth="1"/>
+    <col min="58" max="58" width="14.1796875" customWidth="1"/>
+    <col min="59" max="59" width="9.08984375" customWidth="1"/>
+    <col min="61" max="61" width="11.1796875" customWidth="1"/>
+    <col min="63" max="63" width="16.453125" customWidth="1"/>
+    <col min="64" max="64" width="17.81640625" customWidth="1"/>
+    <col min="65" max="65" width="18.36328125" customWidth="1"/>
+    <col min="66" max="66" width="22.1796875" customWidth="1"/>
+    <col min="67" max="67" width="13.54296875" customWidth="1"/>
+    <col min="69" max="69" width="13.453125" customWidth="1"/>
+    <col min="70" max="70" width="24.1796875" customWidth="1"/>
+    <col min="72" max="72" width="14.1796875" customWidth="1"/>
+    <col min="74" max="74" width="12.81640625" customWidth="1"/>
+    <col min="75" max="75" width="22.36328125" customWidth="1"/>
+    <col min="77" max="77" width="27.1796875" customWidth="1"/>
+    <col min="78" max="78" width="26.54296875" customWidth="1"/>
+    <col min="80" max="80" width="11.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:78" ht="58.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:78" ht="59" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>73</v>
       </c>
@@ -5585,7 +5713,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>79</v>
       </c>
@@ -5821,7 +5949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>78</v>
       </c>
@@ -6057,7 +6185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>77</v>
       </c>
@@ -6293,7 +6421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>82</v>
       </c>
@@ -6529,7 +6657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>76</v>
       </c>
@@ -6765,7 +6893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>75</v>
       </c>
@@ -7001,7 +7129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>74</v>
       </c>
@@ -7237,7 +7365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>80</v>
       </c>
@@ -7473,7 +7601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>81</v>
       </c>
@@ -7709,7 +7837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>83</v>
       </c>

</xml_diff>

<commit_message>
new approach at quiz evaluator
</commit_message>
<xml_diff>
--- a/data/quiz-data.xlsx
+++ b/data/quiz-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VIT\Placement\Internship\SFS intern\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VIT\Placement\Internship\SFS intern\Project-Backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CCF839E-3819-4841-A665-5B121A1B1702}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF2E37E-AAB3-4BB5-86C5-817739F219DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Training" sheetId="3" r:id="rId1"/>
@@ -518,7 +518,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -538,6 +538,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -818,10 +824,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B5FB84D-C3CE-41F8-8DF2-CD77A0B9A49A}">
-  <dimension ref="A1:L78"/>
+  <dimension ref="A1:L79"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C78"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -879,49 +885,41 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
+      <c r="C2" s="9">
+        <v>4</v>
+      </c>
+      <c r="D2" s="9">
+        <v>4</v>
+      </c>
+      <c r="E2" s="9">
+        <v>4</v>
+      </c>
+      <c r="F2" s="10">
+        <v>4</v>
+      </c>
+      <c r="G2" s="9">
+        <v>4</v>
+      </c>
+      <c r="H2" s="9">
+        <v>4</v>
+      </c>
+      <c r="I2" s="10">
+        <v>4</v>
+      </c>
+      <c r="J2" s="10">
+        <v>4</v>
+      </c>
+      <c r="K2" s="9">
+        <v>4</v>
+      </c>
+      <c r="L2" s="5"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -936,7 +934,7 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -959,101 +957,101 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -1073,7 +1071,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1085,7 +1083,7 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -1097,7 +1095,7 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -1111,19 +1109,19 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -1135,7 +1133,7 @@
         <v>0</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -1149,7 +1147,7 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1158,22 +1156,22 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9">
         <v>0</v>
       </c>
       <c r="J9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -1187,7 +1185,7 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -1208,10 +1206,10 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10">
         <v>0</v>
@@ -1225,7 +1223,7 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -1237,7 +1235,7 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -1246,10 +1244,10 @@
         <v>0</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K11">
         <v>0</v>
@@ -1263,13 +1261,13 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -1290,7 +1288,7 @@
         <v>1</v>
       </c>
       <c r="K12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L12">
         <v>0</v>
@@ -1301,31 +1299,31 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
       <c r="H13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K13">
         <v>1</v>
@@ -1339,13 +1337,13 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -1357,13 +1355,13 @@
         <v>0</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14">
         <v>1</v>
       </c>
       <c r="J14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K14">
         <v>1</v>
@@ -1377,19 +1375,19 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15">
         <v>0</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -1398,13 +1396,13 @@
         <v>0</v>
       </c>
       <c r="I15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L15">
         <v>0</v>
@@ -1412,10 +1410,10 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1427,19 +1425,19 @@
         <v>0</v>
       </c>
       <c r="F16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G16">
         <v>0</v>
       </c>
       <c r="H16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I16">
         <v>0</v>
       </c>
       <c r="J16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K16">
         <v>0</v>
@@ -1453,7 +1451,7 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1465,19 +1463,19 @@
         <v>0</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17">
         <v>0</v>
       </c>
       <c r="J17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K17">
         <v>0</v>
@@ -1491,7 +1489,7 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -1506,10 +1504,10 @@
         <v>0</v>
       </c>
       <c r="G18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I18">
         <v>0</v>
@@ -1529,7 +1527,7 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -1567,7 +1565,7 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -1605,7 +1603,7 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -1643,13 +1641,13 @@
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="C22">
         <v>0</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -1661,7 +1659,7 @@
         <v>0</v>
       </c>
       <c r="H22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22">
         <v>0</v>
@@ -1681,13 +1679,13 @@
         <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C23">
         <v>0</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -1705,7 +1703,7 @@
         <v>0</v>
       </c>
       <c r="J23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K23">
         <v>0</v>
@@ -1719,7 +1717,7 @@
         <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -1743,10 +1741,10 @@
         <v>0</v>
       </c>
       <c r="J24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L24">
         <v>0</v>
@@ -1757,7 +1755,7 @@
         <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -1795,85 +1793,85 @@
         <v>2</v>
       </c>
       <c r="B26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>1</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>2</v>
+      </c>
+      <c r="B27" t="s">
         <v>30</v>
       </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
-      <c r="F26">
-        <v>0</v>
-      </c>
-      <c r="G26">
-        <v>0</v>
-      </c>
-      <c r="H26">
-        <v>0</v>
-      </c>
-      <c r="I26">
-        <v>0</v>
-      </c>
-      <c r="J26">
-        <v>0</v>
-      </c>
-      <c r="K26">
-        <v>1</v>
-      </c>
-      <c r="L26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <v>2</v>
-      </c>
-      <c r="B27" t="s">
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>2</v>
+      </c>
+      <c r="B28" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="1">
-        <v>0</v>
-      </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="F27">
-        <v>0</v>
-      </c>
-      <c r="G27">
-        <v>0</v>
-      </c>
-      <c r="H27">
-        <v>0</v>
-      </c>
-      <c r="I27">
-        <v>0</v>
-      </c>
-      <c r="J27">
-        <v>0</v>
-      </c>
-      <c r="K27">
-        <v>1</v>
-      </c>
-      <c r="L27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A28">
-        <v>2</v>
-      </c>
-      <c r="B28" t="s">
-        <v>31</v>
-      </c>
-      <c r="C28">
+      <c r="C28" s="1">
         <v>0</v>
       </c>
       <c r="D28">
@@ -1892,13 +1890,13 @@
         <v>0</v>
       </c>
       <c r="I28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J28">
         <v>0</v>
       </c>
       <c r="K28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L28">
         <v>0</v>
@@ -1909,7 +1907,7 @@
         <v>2</v>
       </c>
       <c r="B29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -1921,7 +1919,7 @@
         <v>0</v>
       </c>
       <c r="F29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G29">
         <v>0</v>
@@ -1930,7 +1928,7 @@
         <v>0</v>
       </c>
       <c r="I29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J29">
         <v>0</v>
@@ -1947,7 +1945,7 @@
         <v>2</v>
       </c>
       <c r="B30" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -1959,7 +1957,7 @@
         <v>0</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G30">
         <v>0</v>
@@ -1982,10 +1980,10 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B31" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -2003,7 +2001,7 @@
         <v>0</v>
       </c>
       <c r="H31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I31">
         <v>0</v>
@@ -2023,7 +2021,7 @@
         <v>3</v>
       </c>
       <c r="B32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -2035,13 +2033,13 @@
         <v>0</v>
       </c>
       <c r="F32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G32">
         <v>0</v>
       </c>
       <c r="H32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I32">
         <v>0</v>
@@ -2061,7 +2059,7 @@
         <v>3</v>
       </c>
       <c r="B33" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -2073,7 +2071,7 @@
         <v>0</v>
       </c>
       <c r="F33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G33">
         <v>0</v>
@@ -2096,10 +2094,10 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B34" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -2137,10 +2135,10 @@
         <v>4</v>
       </c>
       <c r="B35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -2149,7 +2147,7 @@
         <v>0</v>
       </c>
       <c r="F35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G35">
         <v>0</v>
@@ -2175,10 +2173,10 @@
         <v>4</v>
       </c>
       <c r="B36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -2213,7 +2211,7 @@
         <v>4</v>
       </c>
       <c r="B37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -2225,7 +2223,7 @@
         <v>0</v>
       </c>
       <c r="F37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G37">
         <v>0</v>
@@ -2248,10 +2246,10 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B38" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -2289,7 +2287,7 @@
         <v>5</v>
       </c>
       <c r="B39" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -2327,7 +2325,7 @@
         <v>5</v>
       </c>
       <c r="B40" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -2345,10 +2343,10 @@
         <v>0</v>
       </c>
       <c r="H40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J40">
         <v>0</v>
@@ -2365,7 +2363,7 @@
         <v>5</v>
       </c>
       <c r="B41" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -2383,10 +2381,10 @@
         <v>0</v>
       </c>
       <c r="H41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J41">
         <v>0</v>
@@ -2400,10 +2398,10 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B42" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -2415,7 +2413,7 @@
         <v>0</v>
       </c>
       <c r="F42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G42">
         <v>0</v>
@@ -2441,7 +2439,7 @@
         <v>6</v>
       </c>
       <c r="B43" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -2453,7 +2451,7 @@
         <v>0</v>
       </c>
       <c r="F43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G43">
         <v>0</v>
@@ -2462,7 +2460,7 @@
         <v>0</v>
       </c>
       <c r="I43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J43">
         <v>0</v>
@@ -2479,7 +2477,7 @@
         <v>6</v>
       </c>
       <c r="B44" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C44">
         <v>0</v>
@@ -2500,13 +2498,13 @@
         <v>0</v>
       </c>
       <c r="I44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J44">
         <v>0</v>
       </c>
       <c r="K44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L44">
         <v>0</v>
@@ -2517,7 +2515,7 @@
         <v>6</v>
       </c>
       <c r="B45" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C45">
         <v>0</v>
@@ -2555,7 +2553,7 @@
         <v>6</v>
       </c>
       <c r="B46" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C46">
         <v>0</v>
@@ -2593,7 +2591,7 @@
         <v>6</v>
       </c>
       <c r="B47" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -2631,7 +2629,7 @@
         <v>6</v>
       </c>
       <c r="B48" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C48">
         <v>0</v>
@@ -2669,7 +2667,7 @@
         <v>6</v>
       </c>
       <c r="B49" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C49">
         <v>0</v>
@@ -2707,7 +2705,7 @@
         <v>6</v>
       </c>
       <c r="B50" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C50">
         <v>0</v>
@@ -2745,7 +2743,7 @@
         <v>6</v>
       </c>
       <c r="B51" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C51">
         <v>0</v>
@@ -2783,7 +2781,7 @@
         <v>6</v>
       </c>
       <c r="B52" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C52">
         <v>0</v>
@@ -2821,7 +2819,7 @@
         <v>6</v>
       </c>
       <c r="B53" t="s">
-        <v>1</v>
+        <v>70</v>
       </c>
       <c r="C53">
         <v>0</v>
@@ -2859,7 +2857,7 @@
         <v>6</v>
       </c>
       <c r="B54" t="s">
-        <v>71</v>
+        <v>1</v>
       </c>
       <c r="C54">
         <v>0</v>
@@ -2886,10 +2884,10 @@
         <v>0</v>
       </c>
       <c r="K54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L54">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.3">
@@ -2897,7 +2895,7 @@
         <v>6</v>
       </c>
       <c r="B55" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C55">
         <v>0</v>
@@ -2932,10 +2930,10 @@
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B56" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="C56">
         <v>0</v>
@@ -2953,7 +2951,7 @@
         <v>0</v>
       </c>
       <c r="H56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I56">
         <v>0</v>
@@ -2965,7 +2963,7 @@
         <v>0</v>
       </c>
       <c r="L56">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
@@ -2973,7 +2971,7 @@
         <v>7</v>
       </c>
       <c r="B57" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C57">
         <v>0</v>
@@ -3011,7 +3009,7 @@
         <v>7</v>
       </c>
       <c r="B58" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C58">
         <v>0</v>
@@ -3035,7 +3033,7 @@
         <v>0</v>
       </c>
       <c r="J58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K58">
         <v>0</v>
@@ -3049,7 +3047,7 @@
         <v>7</v>
       </c>
       <c r="B59" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C59">
         <v>0</v>
@@ -3087,7 +3085,7 @@
         <v>7</v>
       </c>
       <c r="B60" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C60">
         <v>0</v>
@@ -3111,7 +3109,7 @@
         <v>0</v>
       </c>
       <c r="J60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K60">
         <v>0</v>
@@ -3125,7 +3123,7 @@
         <v>7</v>
       </c>
       <c r="B61" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -3143,7 +3141,7 @@
         <v>0</v>
       </c>
       <c r="H61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I61">
         <v>0</v>
@@ -3160,10 +3158,10 @@
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B62" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="C62">
         <v>0</v>
@@ -3181,13 +3179,13 @@
         <v>0</v>
       </c>
       <c r="H62">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I62">
         <v>0</v>
       </c>
       <c r="J62">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K62">
         <v>0</v>
@@ -3201,7 +3199,7 @@
         <v>8</v>
       </c>
       <c r="B63" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -3225,7 +3223,7 @@
         <v>0</v>
       </c>
       <c r="J63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K63">
         <v>0</v>
@@ -3239,7 +3237,7 @@
         <v>8</v>
       </c>
       <c r="B64" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C64">
         <v>0</v>
@@ -3277,7 +3275,7 @@
         <v>8</v>
       </c>
       <c r="B65" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="C65">
         <v>0</v>
@@ -3315,7 +3313,7 @@
         <v>8</v>
       </c>
       <c r="B66" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="C66">
         <v>0</v>
@@ -3333,7 +3331,7 @@
         <v>0</v>
       </c>
       <c r="H66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I66">
         <v>0</v>
@@ -3345,15 +3343,15 @@
         <v>0</v>
       </c>
       <c r="L66">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B67" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C67">
         <v>0</v>
@@ -3371,7 +3369,7 @@
         <v>0</v>
       </c>
       <c r="H67">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I67">
         <v>0</v>
@@ -3383,7 +3381,7 @@
         <v>0</v>
       </c>
       <c r="L67">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.3">
@@ -3391,7 +3389,7 @@
         <v>9</v>
       </c>
       <c r="B68" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C68">
         <v>0</v>
@@ -3409,7 +3407,7 @@
         <v>0</v>
       </c>
       <c r="H68">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I68">
         <v>0</v>
@@ -3421,27 +3419,27 @@
         <v>0</v>
       </c>
       <c r="L68">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B69" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C69">
         <v>0</v>
       </c>
       <c r="D69">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E69">
         <v>0</v>
       </c>
       <c r="F69">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G69">
         <v>0</v>
@@ -3459,7 +3457,7 @@
         <v>0</v>
       </c>
       <c r="L69">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.3">
@@ -3467,7 +3465,7 @@
         <v>10</v>
       </c>
       <c r="B70" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C70">
         <v>0</v>
@@ -3476,7 +3474,7 @@
         <v>1</v>
       </c>
       <c r="E70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F70">
         <v>1</v>
@@ -3505,19 +3503,19 @@
         <v>10</v>
       </c>
       <c r="B71" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C71">
         <v>0</v>
       </c>
       <c r="D71">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E71">
         <v>1</v>
       </c>
       <c r="F71">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G71">
         <v>0</v>
@@ -3543,7 +3541,7 @@
         <v>10</v>
       </c>
       <c r="B72" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C72">
         <v>0</v>
@@ -3581,7 +3579,7 @@
         <v>10</v>
       </c>
       <c r="B73" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C73">
         <v>0</v>
@@ -3619,7 +3617,7 @@
         <v>10</v>
       </c>
       <c r="B74" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C74">
         <v>0</v>
@@ -3628,7 +3626,7 @@
         <v>0</v>
       </c>
       <c r="E74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F74">
         <v>0</v>
@@ -3637,7 +3635,7 @@
         <v>0</v>
       </c>
       <c r="H74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I74">
         <v>0</v>
@@ -3646,7 +3644,7 @@
         <v>0</v>
       </c>
       <c r="K74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L74">
         <v>0</v>
@@ -3657,13 +3655,13 @@
         <v>10</v>
       </c>
       <c r="B75" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C75">
         <v>0</v>
       </c>
       <c r="D75">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E75">
         <v>0</v>
@@ -3675,7 +3673,7 @@
         <v>0</v>
       </c>
       <c r="H75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I75">
         <v>0</v>
@@ -3684,7 +3682,7 @@
         <v>0</v>
       </c>
       <c r="K75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L75">
         <v>0</v>
@@ -3695,7 +3693,7 @@
         <v>10</v>
       </c>
       <c r="B76" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C76">
         <v>0</v>
@@ -3704,7 +3702,7 @@
         <v>1</v>
       </c>
       <c r="E76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F76">
         <v>0</v>
@@ -3713,7 +3711,7 @@
         <v>0</v>
       </c>
       <c r="H76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I76">
         <v>0</v>
@@ -3733,16 +3731,16 @@
         <v>10</v>
       </c>
       <c r="B77" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C77">
         <v>0</v>
       </c>
       <c r="D77">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E77">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F77">
         <v>0</v>
@@ -3751,7 +3749,7 @@
         <v>0</v>
       </c>
       <c r="H77">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I77">
         <v>0</v>
@@ -3763,7 +3761,7 @@
         <v>0</v>
       </c>
       <c r="L77">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.3">
@@ -3771,41 +3769,80 @@
         <v>10</v>
       </c>
       <c r="B78" t="s">
+        <v>59</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+      <c r="D78">
+        <v>0</v>
+      </c>
+      <c r="E78">
+        <v>0</v>
+      </c>
+      <c r="F78">
+        <v>0</v>
+      </c>
+      <c r="G78">
+        <v>0</v>
+      </c>
+      <c r="H78">
+        <v>0</v>
+      </c>
+      <c r="I78">
+        <v>0</v>
+      </c>
+      <c r="J78">
+        <v>0</v>
+      </c>
+      <c r="K78">
+        <v>0</v>
+      </c>
+      <c r="L78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>10</v>
+      </c>
+      <c r="B79" t="s">
         <v>22</v>
       </c>
-      <c r="C78">
-        <v>0</v>
-      </c>
-      <c r="D78">
-        <v>0</v>
-      </c>
-      <c r="E78">
-        <v>0</v>
-      </c>
-      <c r="F78">
-        <v>0</v>
-      </c>
-      <c r="G78">
-        <v>0</v>
-      </c>
-      <c r="H78">
-        <v>0</v>
-      </c>
-      <c r="I78">
-        <v>0</v>
-      </c>
-      <c r="J78">
-        <v>0</v>
-      </c>
-      <c r="K78">
-        <v>0</v>
-      </c>
-      <c r="L78">
+      <c r="C79">
+        <v>0</v>
+      </c>
+      <c r="D79">
+        <v>0</v>
+      </c>
+      <c r="E79">
+        <v>0</v>
+      </c>
+      <c r="F79">
+        <v>0</v>
+      </c>
+      <c r="G79">
+        <v>0</v>
+      </c>
+      <c r="H79">
+        <v>0</v>
+      </c>
+      <c r="I79">
+        <v>0</v>
+      </c>
+      <c r="J79">
+        <v>0</v>
+      </c>
+      <c r="K79">
+        <v>0</v>
+      </c>
+      <c r="L79">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3813,7 +3850,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{209B6C40-D49A-460E-9F0A-D52ECA57AEC1}">
   <dimension ref="A1:F94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C94" sqref="C94"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
change in auth flow
</commit_message>
<xml_diff>
--- a/data/quiz-data.xlsx
+++ b/data/quiz-data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VIT\Placement\Internship\SFS intern\Project-Backend\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ninju\Internship\Project-Backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF2E37E-AAB3-4BB5-86C5-817739F219DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1463704-3D02-4332-A862-7DCA0CE8226B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Training" sheetId="3" r:id="rId1"/>
@@ -294,9 +294,6 @@
     <t>Low stomach acid 5</t>
   </si>
   <si>
-    <t>Inflamed Gut 1</t>
-  </si>
-  <si>
     <t>Bacterial Imbalance 7</t>
   </si>
   <si>
@@ -438,7 +435,10 @@
     <t>Dersired weight</t>
   </si>
   <si>
-    <t>Gender 456123</t>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Inflamed Gut</t>
   </si>
 </sst>
 </file>
@@ -827,28 +827,28 @@
   <dimension ref="A1:L79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.21875" customWidth="1"/>
-    <col min="2" max="2" width="35.33203125" customWidth="1"/>
-    <col min="3" max="3" width="15.77734375" customWidth="1"/>
-    <col min="4" max="4" width="16.21875" customWidth="1"/>
-    <col min="5" max="5" width="16.77734375" customWidth="1"/>
-    <col min="6" max="6" width="15.77734375" customWidth="1"/>
+    <col min="1" max="1" width="20.1796875" customWidth="1"/>
+    <col min="2" max="2" width="35.36328125" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" customWidth="1"/>
+    <col min="4" max="4" width="16.1796875" customWidth="1"/>
+    <col min="5" max="5" width="16.81640625" customWidth="1"/>
+    <col min="6" max="6" width="15.81640625" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="13.77734375" customWidth="1"/>
-    <col min="9" max="9" width="18.77734375" customWidth="1"/>
+    <col min="8" max="8" width="13.81640625" customWidth="1"/>
+    <col min="9" max="9" width="18.81640625" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
-    <col min="11" max="11" width="13.44140625" customWidth="1"/>
-    <col min="12" max="12" width="12.6640625" customWidth="1"/>
+    <col min="11" max="11" width="13.453125" customWidth="1"/>
+    <col min="12" max="12" width="12.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="50.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="54" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1" t="s">
         <v>73</v>
@@ -866,25 +866,25 @@
         <v>87</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="L1" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C2" s="9">
         <v>4</v>
       </c>
@@ -914,7 +914,7 @@
       </c>
       <c r="L2" s="5"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -952,7 +952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1</v>
       </c>
@@ -990,7 +990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1066,7 +1066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1104,7 +1104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1142,7 +1142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1180,7 +1180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1218,7 +1218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1294,7 +1294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1332,7 +1332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1370,7 +1370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1408,7 +1408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1446,7 +1446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1484,7 +1484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2</v>
       </c>
@@ -1522,7 +1522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1560,7 +1560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>2</v>
       </c>
@@ -1598,7 +1598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>2</v>
       </c>
@@ -1636,7 +1636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>2</v>
       </c>
@@ -1674,7 +1674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>2</v>
       </c>
@@ -1712,7 +1712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>2</v>
       </c>
@@ -1750,7 +1750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1788,7 +1788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>2</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>2</v>
       </c>
@@ -1864,7 +1864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>2</v>
       </c>
@@ -1902,7 +1902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>2</v>
       </c>
@@ -1940,7 +1940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>2</v>
       </c>
@@ -1978,7 +1978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>2</v>
       </c>
@@ -2016,7 +2016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>3</v>
       </c>
@@ -2054,7 +2054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>3</v>
       </c>
@@ -2092,7 +2092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>3</v>
       </c>
@@ -2130,7 +2130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>4</v>
       </c>
@@ -2168,7 +2168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>4</v>
       </c>
@@ -2206,7 +2206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>4</v>
       </c>
@@ -2244,7 +2244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>4</v>
       </c>
@@ -2282,7 +2282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>5</v>
       </c>
@@ -2320,7 +2320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>5</v>
       </c>
@@ -2358,7 +2358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>5</v>
       </c>
@@ -2396,7 +2396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>5</v>
       </c>
@@ -2434,7 +2434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>6</v>
       </c>
@@ -2472,7 +2472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>6</v>
       </c>
@@ -2510,7 +2510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>6</v>
       </c>
@@ -2548,7 +2548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>6</v>
       </c>
@@ -2586,7 +2586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>6</v>
       </c>
@@ -2624,7 +2624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>6</v>
       </c>
@@ -2662,7 +2662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>6</v>
       </c>
@@ -2700,7 +2700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>6</v>
       </c>
@@ -2738,7 +2738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>6</v>
       </c>
@@ -2776,7 +2776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>6</v>
       </c>
@@ -2814,7 +2814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>6</v>
       </c>
@@ -2852,7 +2852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>6</v>
       </c>
@@ -2890,7 +2890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>6</v>
       </c>
@@ -2928,7 +2928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>6</v>
       </c>
@@ -2966,7 +2966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>7</v>
       </c>
@@ -3004,7 +3004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>7</v>
       </c>
@@ -3042,7 +3042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>7</v>
       </c>
@@ -3080,7 +3080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>7</v>
       </c>
@@ -3118,7 +3118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>7</v>
       </c>
@@ -3156,7 +3156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>7</v>
       </c>
@@ -3194,7 +3194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>8</v>
       </c>
@@ -3232,7 +3232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>8</v>
       </c>
@@ -3270,7 +3270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>8</v>
       </c>
@@ -3308,7 +3308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>8</v>
       </c>
@@ -3346,7 +3346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>8</v>
       </c>
@@ -3384,7 +3384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>9</v>
       </c>
@@ -3422,7 +3422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>9</v>
       </c>
@@ -3460,7 +3460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>10</v>
       </c>
@@ -3498,7 +3498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>10</v>
       </c>
@@ -3536,7 +3536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>10</v>
       </c>
@@ -3574,7 +3574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>10</v>
       </c>
@@ -3612,7 +3612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>10</v>
       </c>
@@ -3650,7 +3650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>10</v>
       </c>
@@ -3688,7 +3688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>10</v>
       </c>
@@ -3726,7 +3726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>10</v>
       </c>
@@ -3764,7 +3764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>10</v>
       </c>
@@ -3802,7 +3802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>10</v>
       </c>
@@ -3850,73 +3850,73 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{209B6C40-D49A-460E-9F0A-D52ECA57AEC1}">
   <dimension ref="A1:F94"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C94" sqref="C94"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="F85" sqref="F85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" customWidth="1"/>
+    <col min="1" max="1" width="17.90625" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="24.77734375" customWidth="1"/>
-    <col min="4" max="4" width="73.77734375" customWidth="1"/>
-    <col min="5" max="5" width="26.77734375" customWidth="1"/>
-    <col min="6" max="6" width="41.5546875" customWidth="1"/>
-    <col min="7" max="7" width="23.88671875" customWidth="1"/>
-    <col min="8" max="8" width="21.5546875" customWidth="1"/>
-    <col min="9" max="9" width="22.33203125" customWidth="1"/>
-    <col min="10" max="10" width="25.77734375" customWidth="1"/>
-    <col min="11" max="11" width="22.5546875" customWidth="1"/>
-    <col min="12" max="12" width="19.88671875" customWidth="1"/>
+    <col min="3" max="3" width="24.81640625" customWidth="1"/>
+    <col min="4" max="4" width="73.81640625" customWidth="1"/>
+    <col min="5" max="5" width="26.81640625" customWidth="1"/>
+    <col min="6" max="6" width="41.54296875" customWidth="1"/>
+    <col min="7" max="7" width="23.90625" customWidth="1"/>
+    <col min="8" max="8" width="21.54296875" customWidth="1"/>
+    <col min="9" max="9" width="22.36328125" customWidth="1"/>
+    <col min="10" max="10" width="25.81640625" customWidth="1"/>
+    <col min="11" max="11" width="22.54296875" customWidth="1"/>
+    <col min="12" max="12" width="19.90625" customWidth="1"/>
     <col min="13" max="13" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" t="s">
         <v>116</v>
       </c>
-      <c r="B1" t="s">
-        <v>117</v>
-      </c>
       <c r="C1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="6">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2" s="6">
+        <v>1</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="C2" s="6">
-        <v>1</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C3" s="6">
         <v>1</v>
@@ -3924,15 +3924,15 @@
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
         <v>1</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C4" s="6">
         <v>1</v>
@@ -3940,35 +3940,35 @@
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="6">
+        <v>1</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" s="6">
+        <v>2</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="6">
-        <v>1</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="C5" s="6">
-        <v>2</v>
-      </c>
-      <c r="D5" s="6" t="s">
+      <c r="E5" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="F5" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>1</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C6" s="6">
         <v>2</v>
@@ -3976,15 +3976,15 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="8" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>1</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C7" s="6">
         <v>2</v>
@@ -3992,15 +3992,15 @@
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
         <v>1</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C8" s="6">
         <v>2</v>
@@ -4008,15 +4008,15 @@
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="8" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6">
         <v>1</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C9" s="6">
         <v>2</v>
@@ -4024,107 +4024,107 @@
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="8" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="6">
         <v>1</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C10" s="6">
         <v>3</v>
       </c>
       <c r="D10" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E10" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="E10" s="6" t="s">
-        <v>132</v>
-      </c>
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <v>1</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C11" s="6">
         <v>4</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="6">
         <v>1</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C12" s="6">
         <v>5</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="6">
         <v>1</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C13" s="6">
         <v>6</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F13" s="7"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -4133,12 +4133,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -4147,12 +4147,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -4161,12 +4161,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -4175,12 +4175,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -4189,12 +4189,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -4203,12 +4203,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -4217,12 +4217,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -4231,12 +4231,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -4245,12 +4245,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -4259,12 +4259,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -4273,12 +4273,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>2</v>
       </c>
       <c r="B26" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -4287,12 +4287,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>2</v>
       </c>
       <c r="B27" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -4301,32 +4301,32 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>2</v>
       </c>
       <c r="B28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C28">
         <v>2</v>
       </c>
       <c r="D28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E28" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F28" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>2</v>
       </c>
       <c r="B29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C29">
         <v>2</v>
@@ -4335,12 +4335,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>2</v>
       </c>
       <c r="B30" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C30">
         <v>2</v>
@@ -4349,12 +4349,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>2</v>
       </c>
       <c r="B31" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C31">
         <v>2</v>
@@ -4363,12 +4363,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>2</v>
       </c>
       <c r="B32" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C32">
         <v>2</v>
@@ -4377,12 +4377,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C33">
         <v>2</v>
@@ -4391,12 +4391,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>2</v>
       </c>
       <c r="B34" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C34">
         <v>2</v>
@@ -4405,12 +4405,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>2</v>
       </c>
       <c r="B35" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C35">
         <v>2</v>
@@ -4419,12 +4419,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>2</v>
       </c>
       <c r="B36" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C36">
         <v>2</v>
@@ -4433,12 +4433,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>2</v>
       </c>
       <c r="B37" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C37">
         <v>2</v>
@@ -4447,12 +4447,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>2</v>
       </c>
       <c r="B38" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C38">
         <v>2</v>
@@ -4461,12 +4461,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>2</v>
       </c>
       <c r="B39" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C39">
         <v>2</v>
@@ -4475,12 +4475,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>2</v>
       </c>
       <c r="B40" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C40">
         <v>2</v>
@@ -4489,12 +4489,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>2</v>
       </c>
       <c r="B41" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C41">
         <v>2</v>
@@ -4503,12 +4503,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>2</v>
       </c>
       <c r="B42" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C42">
         <v>2</v>
@@ -4517,32 +4517,32 @@
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>2</v>
       </c>
       <c r="B43" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C43">
         <v>3</v>
       </c>
       <c r="D43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E43" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F43" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>2</v>
       </c>
       <c r="B44" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C44">
         <v>3</v>
@@ -4551,12 +4551,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>2</v>
       </c>
       <c r="B45" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C45">
         <v>3</v>
@@ -4565,32 +4565,32 @@
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>2</v>
       </c>
       <c r="B46" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C46">
         <v>4</v>
       </c>
       <c r="D46" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E46" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F46" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>2</v>
       </c>
       <c r="B47" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C47">
         <v>4</v>
@@ -4599,12 +4599,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>2</v>
       </c>
       <c r="B48" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C48">
         <v>4</v>
@@ -4613,12 +4613,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>2</v>
       </c>
       <c r="B49" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C49">
         <v>4</v>
@@ -4627,32 +4627,32 @@
         <v>38</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>2</v>
       </c>
       <c r="B50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C50">
         <v>5</v>
       </c>
       <c r="D50" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E50" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F50" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>2</v>
       </c>
       <c r="B51" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C51">
         <v>5</v>
@@ -4661,12 +4661,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>2</v>
       </c>
       <c r="B52" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C52">
         <v>5</v>
@@ -4675,12 +4675,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>2</v>
       </c>
       <c r="B53" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C53">
         <v>5</v>
@@ -4689,32 +4689,32 @@
         <v>22</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>2</v>
       </c>
       <c r="B54" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C54">
         <v>6</v>
       </c>
       <c r="D54" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E54" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F54" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>2</v>
       </c>
       <c r="B55" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C55">
         <v>6</v>
@@ -4723,12 +4723,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>2</v>
       </c>
       <c r="B56" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C56">
         <v>6</v>
@@ -4737,12 +4737,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>2</v>
       </c>
       <c r="B57" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C57">
         <v>6</v>
@@ -4751,12 +4751,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>2</v>
       </c>
       <c r="B58" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C58">
         <v>6</v>
@@ -4765,12 +4765,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>2</v>
       </c>
       <c r="B59" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C59">
         <v>6</v>
@@ -4779,12 +4779,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>2</v>
       </c>
       <c r="B60" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C60">
         <v>6</v>
@@ -4793,12 +4793,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>2</v>
       </c>
       <c r="B61" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C61">
         <v>6</v>
@@ -4807,12 +4807,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>2</v>
       </c>
       <c r="B62" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C62">
         <v>6</v>
@@ -4821,12 +4821,12 @@
         <v>68</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>2</v>
       </c>
       <c r="B63" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C63">
         <v>6</v>
@@ -4835,12 +4835,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>2</v>
       </c>
       <c r="B64" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C64">
         <v>6</v>
@@ -4849,12 +4849,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>2</v>
       </c>
       <c r="B65" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C65">
         <v>6</v>
@@ -4863,12 +4863,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>2</v>
       </c>
       <c r="B66" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C66">
         <v>6</v>
@@ -4877,12 +4877,12 @@
         <v>71</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>2</v>
       </c>
       <c r="B67" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C67">
         <v>6</v>
@@ -4891,32 +4891,32 @@
         <v>72</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>3</v>
       </c>
       <c r="B68" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C68">
         <v>1</v>
       </c>
       <c r="D68" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E68" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F68" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>3</v>
       </c>
       <c r="B69" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C69">
         <v>1</v>
@@ -4925,12 +4925,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>3</v>
       </c>
       <c r="B70" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C70">
         <v>1</v>
@@ -4939,12 +4939,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>3</v>
       </c>
       <c r="B71" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C71">
         <v>1</v>
@@ -4953,12 +4953,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>3</v>
       </c>
       <c r="B72" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C72">
         <v>1</v>
@@ -4967,12 +4967,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>3</v>
       </c>
       <c r="B73" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C73">
         <v>1</v>
@@ -4981,32 +4981,32 @@
         <v>22</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>3</v>
       </c>
       <c r="B74" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C74">
         <v>2</v>
       </c>
       <c r="D74" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E74" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F74" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>3</v>
       </c>
       <c r="B75" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C75">
         <v>2</v>
@@ -5015,12 +5015,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>3</v>
       </c>
       <c r="B76" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C76">
         <v>2</v>
@@ -5029,12 +5029,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>3</v>
       </c>
       <c r="B77" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C77">
         <v>2</v>
@@ -5043,12 +5043,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>3</v>
       </c>
       <c r="B78" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C78">
         <v>2</v>
@@ -5057,32 +5057,32 @@
         <v>48</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>3</v>
       </c>
       <c r="B79" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C79">
         <v>3</v>
       </c>
       <c r="D79" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E79" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F79" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>3</v>
       </c>
       <c r="B80" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C80">
         <v>3</v>
@@ -5091,32 +5091,32 @@
         <v>50</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>3</v>
       </c>
       <c r="B81" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C81">
         <v>4</v>
       </c>
       <c r="D81" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E81" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F81" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>3</v>
       </c>
       <c r="B82" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C82">
         <v>4</v>
@@ -5125,12 +5125,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>3</v>
       </c>
       <c r="B83" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C83">
         <v>4</v>
@@ -5139,12 +5139,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>3</v>
       </c>
       <c r="B84" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C84">
         <v>4</v>
@@ -5153,12 +5153,12 @@
         <v>54</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>3</v>
       </c>
       <c r="B85" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C85">
         <v>4</v>
@@ -5167,12 +5167,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>3</v>
       </c>
       <c r="B86" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C86">
         <v>4</v>
@@ -5181,12 +5181,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>3</v>
       </c>
       <c r="B87" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C87">
         <v>4</v>
@@ -5195,12 +5195,12 @@
         <v>57</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>3</v>
       </c>
       <c r="B88" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C88">
         <v>4</v>
@@ -5209,12 +5209,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>3</v>
       </c>
       <c r="B89" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C89">
         <v>4</v>
@@ -5223,12 +5223,12 @@
         <v>59</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>3</v>
       </c>
       <c r="B90" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C90">
         <v>4</v>
@@ -5237,66 +5237,66 @@
         <v>22</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>4</v>
       </c>
       <c r="B91" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C91">
         <v>1</v>
       </c>
       <c r="D91" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E91" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F91" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>4</v>
       </c>
       <c r="B92" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C92">
         <v>1</v>
       </c>
       <c r="F92" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>4</v>
       </c>
       <c r="B93" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C93">
         <v>1</v>
       </c>
       <c r="F93" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>4</v>
       </c>
       <c r="B94" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C94">
         <v>1</v>
       </c>
       <c r="F94" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -5313,80 +5313,80 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.5546875" customWidth="1"/>
-    <col min="2" max="2" width="28.77734375" customWidth="1"/>
-    <col min="3" max="3" width="18.44140625" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" customWidth="1"/>
-    <col min="5" max="5" width="18.21875" customWidth="1"/>
+    <col min="1" max="1" width="21.54296875" customWidth="1"/>
+    <col min="2" max="2" width="28.81640625" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" customWidth="1"/>
+    <col min="4" max="4" width="18.90625" customWidth="1"/>
+    <col min="5" max="5" width="18.1796875" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="29.21875" customWidth="1"/>
-    <col min="8" max="8" width="15.109375" customWidth="1"/>
-    <col min="9" max="9" width="13.21875" customWidth="1"/>
-    <col min="10" max="10" width="29.21875" customWidth="1"/>
-    <col min="11" max="11" width="21.77734375" customWidth="1"/>
-    <col min="12" max="12" width="18.5546875" customWidth="1"/>
-    <col min="13" max="13" width="15.77734375" customWidth="1"/>
-    <col min="16" max="16" width="11.21875" customWidth="1"/>
-    <col min="17" max="17" width="18.21875" customWidth="1"/>
+    <col min="7" max="7" width="29.1796875" customWidth="1"/>
+    <col min="8" max="8" width="15.08984375" customWidth="1"/>
+    <col min="9" max="9" width="13.1796875" customWidth="1"/>
+    <col min="10" max="10" width="29.1796875" customWidth="1"/>
+    <col min="11" max="11" width="21.81640625" customWidth="1"/>
+    <col min="12" max="12" width="18.54296875" customWidth="1"/>
+    <col min="13" max="13" width="15.81640625" customWidth="1"/>
+    <col min="16" max="16" width="11.1796875" customWidth="1"/>
+    <col min="17" max="17" width="18.1796875" customWidth="1"/>
     <col min="18" max="18" width="36" customWidth="1"/>
-    <col min="19" max="19" width="8.88671875" customWidth="1"/>
+    <col min="19" max="19" width="8.90625" customWidth="1"/>
     <col min="20" max="20" width="30" customWidth="1"/>
-    <col min="21" max="21" width="12.77734375" customWidth="1"/>
-    <col min="22" max="22" width="11.6640625" customWidth="1"/>
-    <col min="23" max="23" width="11.33203125" customWidth="1"/>
-    <col min="24" max="24" width="15.44140625" customWidth="1"/>
-    <col min="25" max="25" width="31.5546875" customWidth="1"/>
-    <col min="26" max="26" width="20.33203125" customWidth="1"/>
-    <col min="27" max="27" width="10.77734375" customWidth="1"/>
-    <col min="28" max="28" width="18.88671875" customWidth="1"/>
-    <col min="29" max="29" width="25.21875" customWidth="1"/>
-    <col min="30" max="30" width="23.88671875" customWidth="1"/>
-    <col min="31" max="31" width="18.77734375" customWidth="1"/>
-    <col min="32" max="32" width="11.5546875" customWidth="1"/>
-    <col min="33" max="33" width="17.6640625" customWidth="1"/>
-    <col min="34" max="34" width="26.44140625" customWidth="1"/>
-    <col min="35" max="35" width="15.88671875" customWidth="1"/>
-    <col min="36" max="36" width="33.21875" customWidth="1"/>
-    <col min="37" max="37" width="34.77734375" customWidth="1"/>
-    <col min="38" max="38" width="15.21875" customWidth="1"/>
+    <col min="21" max="21" width="12.81640625" customWidth="1"/>
+    <col min="22" max="22" width="11.6328125" customWidth="1"/>
+    <col min="23" max="23" width="11.36328125" customWidth="1"/>
+    <col min="24" max="24" width="15.453125" customWidth="1"/>
+    <col min="25" max="25" width="31.54296875" customWidth="1"/>
+    <col min="26" max="26" width="20.36328125" customWidth="1"/>
+    <col min="27" max="27" width="10.81640625" customWidth="1"/>
+    <col min="28" max="28" width="18.90625" customWidth="1"/>
+    <col min="29" max="29" width="25.1796875" customWidth="1"/>
+    <col min="30" max="30" width="23.90625" customWidth="1"/>
+    <col min="31" max="31" width="18.81640625" customWidth="1"/>
+    <col min="32" max="32" width="11.54296875" customWidth="1"/>
+    <col min="33" max="33" width="17.6328125" customWidth="1"/>
+    <col min="34" max="34" width="26.453125" customWidth="1"/>
+    <col min="35" max="35" width="15.90625" customWidth="1"/>
+    <col min="36" max="36" width="33.1796875" customWidth="1"/>
+    <col min="37" max="37" width="34.81640625" customWidth="1"/>
+    <col min="38" max="38" width="15.1796875" customWidth="1"/>
     <col min="39" max="39" width="33" customWidth="1"/>
     <col min="40" max="40" width="32" customWidth="1"/>
-    <col min="41" max="41" width="25.5546875" customWidth="1"/>
-    <col min="42" max="42" width="11.21875" customWidth="1"/>
-    <col min="43" max="43" width="14.44140625" customWidth="1"/>
-    <col min="44" max="44" width="31.33203125" customWidth="1"/>
-    <col min="45" max="45" width="23.21875" customWidth="1"/>
-    <col min="46" max="46" width="34.44140625" customWidth="1"/>
-    <col min="47" max="47" width="12.44140625" customWidth="1"/>
-    <col min="48" max="48" width="10.77734375" customWidth="1"/>
-    <col min="49" max="49" width="17.6640625" customWidth="1"/>
-    <col min="52" max="52" width="13.109375" customWidth="1"/>
-    <col min="53" max="53" width="14.21875" customWidth="1"/>
-    <col min="54" max="54" width="17.77734375" customWidth="1"/>
-    <col min="55" max="55" width="10.5546875" customWidth="1"/>
-    <col min="56" max="56" width="18.21875" customWidth="1"/>
-    <col min="57" max="57" width="10.88671875" customWidth="1"/>
-    <col min="58" max="58" width="14.21875" customWidth="1"/>
-    <col min="59" max="59" width="9.109375" customWidth="1"/>
-    <col min="61" max="61" width="11.21875" customWidth="1"/>
-    <col min="63" max="63" width="16.44140625" customWidth="1"/>
-    <col min="64" max="64" width="17.77734375" customWidth="1"/>
-    <col min="65" max="65" width="18.33203125" customWidth="1"/>
-    <col min="66" max="66" width="22.21875" customWidth="1"/>
-    <col min="67" max="67" width="13.5546875" customWidth="1"/>
-    <col min="69" max="69" width="13.44140625" customWidth="1"/>
-    <col min="70" max="70" width="24.21875" customWidth="1"/>
-    <col min="72" max="72" width="14.21875" customWidth="1"/>
-    <col min="74" max="74" width="12.77734375" customWidth="1"/>
-    <col min="75" max="75" width="22.33203125" customWidth="1"/>
-    <col min="77" max="77" width="27.21875" customWidth="1"/>
-    <col min="78" max="78" width="26.5546875" customWidth="1"/>
-    <col min="80" max="80" width="11.88671875" customWidth="1"/>
+    <col min="41" max="41" width="25.54296875" customWidth="1"/>
+    <col min="42" max="42" width="11.1796875" customWidth="1"/>
+    <col min="43" max="43" width="14.453125" customWidth="1"/>
+    <col min="44" max="44" width="31.36328125" customWidth="1"/>
+    <col min="45" max="45" width="23.1796875" customWidth="1"/>
+    <col min="46" max="46" width="34.453125" customWidth="1"/>
+    <col min="47" max="47" width="12.453125" customWidth="1"/>
+    <col min="48" max="48" width="10.81640625" customWidth="1"/>
+    <col min="49" max="49" width="17.6328125" customWidth="1"/>
+    <col min="52" max="52" width="13.08984375" customWidth="1"/>
+    <col min="53" max="53" width="14.1796875" customWidth="1"/>
+    <col min="54" max="54" width="17.81640625" customWidth="1"/>
+    <col min="55" max="55" width="10.54296875" customWidth="1"/>
+    <col min="56" max="56" width="18.1796875" customWidth="1"/>
+    <col min="57" max="57" width="10.90625" customWidth="1"/>
+    <col min="58" max="58" width="14.1796875" customWidth="1"/>
+    <col min="59" max="59" width="9.08984375" customWidth="1"/>
+    <col min="61" max="61" width="11.1796875" customWidth="1"/>
+    <col min="63" max="63" width="16.453125" customWidth="1"/>
+    <col min="64" max="64" width="17.81640625" customWidth="1"/>
+    <col min="65" max="65" width="18.36328125" customWidth="1"/>
+    <col min="66" max="66" width="22.1796875" customWidth="1"/>
+    <col min="67" max="67" width="13.54296875" customWidth="1"/>
+    <col min="69" max="69" width="13.453125" customWidth="1"/>
+    <col min="70" max="70" width="24.1796875" customWidth="1"/>
+    <col min="72" max="72" width="14.1796875" customWidth="1"/>
+    <col min="74" max="74" width="12.81640625" customWidth="1"/>
+    <col min="75" max="75" width="22.36328125" customWidth="1"/>
+    <col min="77" max="77" width="27.1796875" customWidth="1"/>
+    <col min="78" max="78" width="26.54296875" customWidth="1"/>
+    <col min="80" max="80" width="11.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:78" ht="58.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:78" ht="59" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>73</v>
       </c>
@@ -5622,7 +5622,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>79</v>
       </c>
@@ -5858,7 +5858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>78</v>
       </c>
@@ -6094,7 +6094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>77</v>
       </c>
@@ -6330,7 +6330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>82</v>
       </c>
@@ -6566,7 +6566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>76</v>
       </c>
@@ -6802,7 +6802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>75</v>
       </c>
@@ -7038,7 +7038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>74</v>
       </c>
@@ -7274,7 +7274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>80</v>
       </c>
@@ -7510,7 +7510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>81</v>
       </c>
@@ -7746,7 +7746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>83</v>
       </c>

</xml_diff>